<commit_message>
Calculate euclidean distance to cluster center
</commit_message>
<xml_diff>
--- a/chapter-02/exercise-02.xlsx
+++ b/chapter-02/exercise-02.xlsx
@@ -9,17 +9,18 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="14400" windowHeight="17460" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="14400" windowHeight="17460" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="OfferInformation" sheetId="1" r:id="rId1"/>
     <sheet name="Transactions" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
     <sheet name="Matrix" sheetId="4" r:id="rId4"/>
+    <sheet name="4MC" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <pivotCaches>
-    <pivotCache cacheId="7" r:id="rId5"/>
+    <pivotCache cacheId="7" r:id="rId6"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="806" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1050" uniqueCount="153">
   <si>
     <t>Campaign</t>
   </si>
@@ -468,6 +469,30 @@
   </si>
   <si>
     <t>Count of Offer #</t>
+  </si>
+  <si>
+    <t>Cluster 1</t>
+  </si>
+  <si>
+    <t>Cluster 2</t>
+  </si>
+  <si>
+    <t>Cluster 3</t>
+  </si>
+  <si>
+    <t>Cluster 4</t>
+  </si>
+  <si>
+    <t>Distance to Cluster 1</t>
+  </si>
+  <si>
+    <t>Distance to Cluster 2</t>
+  </si>
+  <si>
+    <t>Distance to Cluster 3</t>
+  </si>
+  <si>
+    <t>Distance to Cluster 4</t>
   </si>
 </sst>
 </file>
@@ -11221,15 +11246,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:DF36"/>
+  <dimension ref="A1:DE33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I34" sqref="I34"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="DE33" sqref="A1:DE33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:110" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:109" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>39</v>
       </c>
@@ -11558,7 +11583,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="2" spans="1:110" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:109" x14ac:dyDescent="0.2">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -11613,11 +11638,8 @@
       <c r="DE2">
         <v>10</v>
       </c>
-      <c r="DF2" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="3" spans="1:110" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:109" x14ac:dyDescent="0.2">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -11672,11 +11694,8 @@
       <c r="DE3">
         <v>10</v>
       </c>
-      <c r="DF3">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:110" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:109" x14ac:dyDescent="0.2">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -11719,11 +11738,8 @@
       <c r="DE4">
         <v>6</v>
       </c>
-      <c r="DF4">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:110" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:109" x14ac:dyDescent="0.2">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -11784,11 +11800,8 @@
       <c r="DE5">
         <v>12</v>
       </c>
-      <c r="DF5">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:110" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:109" x14ac:dyDescent="0.2">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -11825,11 +11838,8 @@
       <c r="DE6">
         <v>4</v>
       </c>
-      <c r="DF6">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:110" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:109" x14ac:dyDescent="0.2">
       <c r="A7" s="4">
         <v>6</v>
       </c>
@@ -11890,11 +11900,8 @@
       <c r="DE7">
         <v>12</v>
       </c>
-      <c r="DF7">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:110" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:109" x14ac:dyDescent="0.2">
       <c r="A8" s="4">
         <v>7</v>
       </c>
@@ -11976,11 +11983,8 @@
       <c r="DE8">
         <v>19</v>
       </c>
-      <c r="DF8">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:110" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:109" x14ac:dyDescent="0.2">
       <c r="A9" s="4">
         <v>8</v>
       </c>
@@ -12065,11 +12069,8 @@
       <c r="DE9">
         <v>20</v>
       </c>
-      <c r="DF9">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="1:110" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:109" x14ac:dyDescent="0.2">
       <c r="A10" s="4">
         <v>9</v>
       </c>
@@ -12124,11 +12125,8 @@
       <c r="DE10">
         <v>10</v>
       </c>
-      <c r="DF10">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="1:110" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:109" x14ac:dyDescent="0.2">
       <c r="A11" s="4">
         <v>10</v>
       </c>
@@ -12174,11 +12172,8 @@
       <c r="DE11">
         <v>7</v>
       </c>
-      <c r="DF11">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:110" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:109" x14ac:dyDescent="0.2">
       <c r="A12" s="4">
         <v>11</v>
       </c>
@@ -12242,11 +12237,8 @@
       <c r="DE12">
         <v>13</v>
       </c>
-      <c r="DF12">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="1:110" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:109" x14ac:dyDescent="0.2">
       <c r="A13" s="4">
         <v>12</v>
       </c>
@@ -12286,11 +12278,8 @@
       <c r="DE13">
         <v>5</v>
       </c>
-      <c r="DF13">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" spans="1:110" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:109" x14ac:dyDescent="0.2">
       <c r="A14" s="4">
         <v>13</v>
       </c>
@@ -12333,11 +12322,8 @@
       <c r="DE14">
         <v>6</v>
       </c>
-      <c r="DF14">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:110" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:109" x14ac:dyDescent="0.2">
       <c r="A15" s="4">
         <v>14</v>
       </c>
@@ -12389,11 +12375,8 @@
       <c r="DE15">
         <v>9</v>
       </c>
-      <c r="DF15">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="16" spans="1:110" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:109" x14ac:dyDescent="0.2">
       <c r="A16" s="4">
         <v>15</v>
       </c>
@@ -12436,11 +12419,8 @@
       <c r="DE16">
         <v>6</v>
       </c>
-      <c r="DF16">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="17" spans="1:110" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:109" x14ac:dyDescent="0.2">
       <c r="A17" s="4">
         <v>16</v>
       </c>
@@ -12480,11 +12460,8 @@
       <c r="DE17">
         <v>5</v>
       </c>
-      <c r="DF17">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="18" spans="1:110" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:109" x14ac:dyDescent="0.2">
       <c r="A18" s="4">
         <v>17</v>
       </c>
@@ -12530,11 +12507,8 @@
       <c r="DE18">
         <v>7</v>
       </c>
-      <c r="DF18">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:110" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:109" x14ac:dyDescent="0.2">
       <c r="A19" s="4">
         <v>18</v>
       </c>
@@ -12601,11 +12575,8 @@
       <c r="DE19">
         <v>14</v>
       </c>
-      <c r="DF19">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="20" spans="1:110" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="1:109" x14ac:dyDescent="0.2">
       <c r="A20" s="4">
         <v>19</v>
       </c>
@@ -12645,11 +12616,8 @@
       <c r="DE20">
         <v>5</v>
       </c>
-      <c r="DF20">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="21" spans="1:110" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="1:109" x14ac:dyDescent="0.2">
       <c r="A21" s="4">
         <v>20</v>
       </c>
@@ -12692,11 +12660,8 @@
       <c r="DE21">
         <v>6</v>
       </c>
-      <c r="DF21">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="22" spans="1:110" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="1:109" x14ac:dyDescent="0.2">
       <c r="A22" s="4">
         <v>21</v>
       </c>
@@ -12733,11 +12698,8 @@
       <c r="DE22">
         <v>4</v>
       </c>
-      <c r="DF22">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="23" spans="1:110" x14ac:dyDescent="0.2">
+    </row>
+    <row r="23" spans="1:109" x14ac:dyDescent="0.2">
       <c r="A23" s="4">
         <v>22</v>
       </c>
@@ -12825,11 +12787,8 @@
       <c r="DE23">
         <v>21</v>
       </c>
-      <c r="DF23">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="24" spans="1:110" x14ac:dyDescent="0.2">
+    </row>
+    <row r="24" spans="1:109" x14ac:dyDescent="0.2">
       <c r="A24" s="4">
         <v>23</v>
       </c>
@@ -12869,11 +12828,8 @@
       <c r="DE24">
         <v>5</v>
       </c>
-      <c r="DF24">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="25" spans="1:110" x14ac:dyDescent="0.2">
+    </row>
+    <row r="25" spans="1:109" x14ac:dyDescent="0.2">
       <c r="A25" s="4">
         <v>24</v>
       </c>
@@ -12934,11 +12890,8 @@
       <c r="DE25">
         <v>12</v>
       </c>
-      <c r="DF25">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="26" spans="1:110" x14ac:dyDescent="0.2">
+    </row>
+    <row r="26" spans="1:109" x14ac:dyDescent="0.2">
       <c r="A26" s="4">
         <v>25</v>
       </c>
@@ -12981,11 +12934,8 @@
       <c r="DE26">
         <v>6</v>
       </c>
-      <c r="DF26">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="27" spans="1:110" x14ac:dyDescent="0.2">
+    </row>
+    <row r="27" spans="1:109" x14ac:dyDescent="0.2">
       <c r="A27" s="4">
         <v>26</v>
       </c>
@@ -13055,11 +13005,8 @@
       <c r="DE27">
         <v>15</v>
       </c>
-      <c r="DF27">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="28" spans="1:110" x14ac:dyDescent="0.2">
+    </row>
+    <row r="28" spans="1:109" x14ac:dyDescent="0.2">
       <c r="A28" s="4">
         <v>27</v>
       </c>
@@ -13111,11 +13058,8 @@
       <c r="DE28">
         <v>9</v>
       </c>
-      <c r="DF28">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="29" spans="1:110" x14ac:dyDescent="0.2">
+    </row>
+    <row r="29" spans="1:109" x14ac:dyDescent="0.2">
       <c r="A29" s="4">
         <v>28</v>
       </c>
@@ -13158,11 +13102,8 @@
       <c r="DE29">
         <v>6</v>
       </c>
-      <c r="DF29">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="30" spans="1:110" x14ac:dyDescent="0.2">
+    </row>
+    <row r="30" spans="1:109" x14ac:dyDescent="0.2">
       <c r="A30" s="4">
         <v>29</v>
       </c>
@@ -13238,11 +13179,8 @@
       <c r="DE30">
         <v>17</v>
       </c>
-      <c r="DF30">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="31" spans="1:110" x14ac:dyDescent="0.2">
+    </row>
+    <row r="31" spans="1:109" x14ac:dyDescent="0.2">
       <c r="A31" s="4">
         <v>30</v>
       </c>
@@ -13333,11 +13271,8 @@
       <c r="DE31">
         <v>22</v>
       </c>
-      <c r="DF31">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="32" spans="1:110" x14ac:dyDescent="0.2">
+    </row>
+    <row r="32" spans="1:109" x14ac:dyDescent="0.2">
       <c r="A32" s="4">
         <v>31</v>
       </c>
@@ -13413,11 +13348,8 @@
       <c r="DE32">
         <v>17</v>
       </c>
-      <c r="DF32">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="33" spans="1:110" x14ac:dyDescent="0.2">
+    </row>
+    <row r="33" spans="1:109" x14ac:dyDescent="0.2">
       <c r="A33" s="4">
         <v>32</v>
       </c>
@@ -13454,18 +13386,3785 @@
       <c r="DE33">
         <v>4</v>
       </c>
-      <c r="DF33">
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:DI37"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="A37" sqref="A37"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:113" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="L1" t="s">
+        <v>78</v>
+      </c>
+      <c r="M1" t="s">
+        <v>71</v>
+      </c>
+      <c r="N1" t="s">
+        <v>51</v>
+      </c>
+      <c r="O1" t="s">
+        <v>105</v>
+      </c>
+      <c r="P1" t="s">
+        <v>77</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>138</v>
+      </c>
+      <c r="R1" t="s">
+        <v>106</v>
+      </c>
+      <c r="S1" t="s">
+        <v>117</v>
+      </c>
+      <c r="T1" t="s">
+        <v>116</v>
+      </c>
+      <c r="U1" t="s">
+        <v>43</v>
+      </c>
+      <c r="V1" t="s">
+        <v>137</v>
+      </c>
+      <c r="W1" t="s">
+        <v>82</v>
+      </c>
+      <c r="X1" t="s">
+        <v>85</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>64</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>91</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>99</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>103</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>111</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>121</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>112</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>92</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>139</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>94</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>126</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>107</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>62</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>118</v>
+      </c>
+      <c r="AP1" t="s">
+        <v>76</v>
+      </c>
+      <c r="AQ1" t="s">
+        <v>135</v>
+      </c>
+      <c r="AR1" t="s">
+        <v>69</v>
+      </c>
+      <c r="AS1" t="s">
+        <v>63</v>
+      </c>
+      <c r="AT1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AU1" t="s">
+        <v>80</v>
+      </c>
+      <c r="AV1" t="s">
+        <v>109</v>
+      </c>
+      <c r="AW1" t="s">
+        <v>122</v>
+      </c>
+      <c r="AX1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AY1" t="s">
+        <v>119</v>
+      </c>
+      <c r="AZ1" t="s">
+        <v>134</v>
+      </c>
+      <c r="BA1" t="s">
+        <v>41</v>
+      </c>
+      <c r="BB1" t="s">
+        <v>44</v>
+      </c>
+      <c r="BC1" t="s">
+        <v>108</v>
+      </c>
+      <c r="BD1" t="s">
+        <v>74</v>
+      </c>
+      <c r="BE1" t="s">
+        <v>61</v>
+      </c>
+      <c r="BF1" t="s">
+        <v>65</v>
+      </c>
+      <c r="BG1" t="s">
+        <v>125</v>
+      </c>
+      <c r="BH1" t="s">
+        <v>60</v>
+      </c>
+      <c r="BI1" t="s">
+        <v>56</v>
+      </c>
+      <c r="BJ1" t="s">
+        <v>50</v>
+      </c>
+      <c r="BK1" t="s">
+        <v>45</v>
+      </c>
+      <c r="BL1" t="s">
+        <v>83</v>
+      </c>
+      <c r="BM1" t="s">
+        <v>55</v>
+      </c>
+      <c r="BN1" t="s">
+        <v>129</v>
+      </c>
+      <c r="BO1" t="s">
+        <v>101</v>
+      </c>
+      <c r="BP1" t="s">
+        <v>95</v>
+      </c>
+      <c r="BQ1" t="s">
+        <v>97</v>
+      </c>
+      <c r="BR1" t="s">
+        <v>124</v>
+      </c>
+      <c r="BS1" t="s">
+        <v>79</v>
+      </c>
+      <c r="BT1" t="s">
+        <v>96</v>
+      </c>
+      <c r="BU1" t="s">
+        <v>133</v>
+      </c>
+      <c r="BV1" t="s">
+        <v>90</v>
+      </c>
+      <c r="BW1" t="s">
+        <v>68</v>
+      </c>
+      <c r="BX1" t="s">
+        <v>136</v>
+      </c>
+      <c r="BY1" t="s">
+        <v>102</v>
+      </c>
+      <c r="BZ1" t="s">
+        <v>86</v>
+      </c>
+      <c r="CA1" t="s">
+        <v>130</v>
+      </c>
+      <c r="CB1" t="s">
+        <v>123</v>
+      </c>
+      <c r="CC1" t="s">
+        <v>81</v>
+      </c>
+      <c r="CD1" t="s">
+        <v>104</v>
+      </c>
+      <c r="CE1" t="s">
+        <v>120</v>
+      </c>
+      <c r="CF1" t="s">
+        <v>113</v>
+      </c>
+      <c r="CG1" t="s">
+        <v>98</v>
+      </c>
+      <c r="CH1" t="s">
+        <v>84</v>
+      </c>
+      <c r="CI1" t="s">
+        <v>66</v>
+      </c>
+      <c r="CJ1" t="s">
+        <v>48</v>
+      </c>
+      <c r="CK1" t="s">
+        <v>100</v>
+      </c>
+      <c r="CL1" t="s">
+        <v>128</v>
+      </c>
+      <c r="CM1" t="s">
+        <v>132</v>
+      </c>
+      <c r="CN1" t="s">
+        <v>72</v>
+      </c>
+      <c r="CO1" t="s">
+        <v>127</v>
+      </c>
+      <c r="CP1" t="s">
+        <v>75</v>
+      </c>
+      <c r="CQ1" t="s">
+        <v>40</v>
+      </c>
+      <c r="CR1" t="s">
+        <v>93</v>
+      </c>
+      <c r="CS1" t="s">
+        <v>131</v>
+      </c>
+      <c r="CT1" t="s">
+        <v>52</v>
+      </c>
+      <c r="CU1" t="s">
+        <v>53</v>
+      </c>
+      <c r="CV1" t="s">
+        <v>58</v>
+      </c>
+      <c r="CW1" t="s">
+        <v>89</v>
+      </c>
+      <c r="CX1" t="s">
+        <v>88</v>
+      </c>
+      <c r="CY1" t="s">
+        <v>67</v>
+      </c>
+      <c r="CZ1" t="s">
+        <v>110</v>
+      </c>
+      <c r="DA1" t="s">
+        <v>115</v>
+      </c>
+      <c r="DB1" t="s">
+        <v>59</v>
+      </c>
+      <c r="DC1" t="s">
+        <v>42</v>
+      </c>
+      <c r="DD1" t="s">
+        <v>49</v>
+      </c>
+      <c r="DE1" t="s">
+        <v>114</v>
+      </c>
+      <c r="DF1" t="s">
+        <v>73</v>
+      </c>
+      <c r="DG1" t="s">
+        <v>70</v>
+      </c>
+      <c r="DH1" t="s">
+        <v>141</v>
+      </c>
+      <c r="DI1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="2" spans="1:113" x14ac:dyDescent="0.2">
+      <c r="A2" s="4">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2">
+        <v>72</v>
+      </c>
+      <c r="E2">
+        <v>56</v>
+      </c>
+      <c r="F2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" t="s">
+        <v>9</v>
+      </c>
+      <c r="V2">
+        <v>1</v>
+      </c>
+      <c r="AI2">
+        <v>1</v>
+      </c>
+      <c r="AK2">
+        <v>1</v>
+      </c>
+      <c r="AX2">
+        <v>1</v>
+      </c>
+      <c r="BL2">
+        <v>1</v>
+      </c>
+      <c r="BY2">
+        <v>1</v>
+      </c>
+      <c r="CB2">
+        <v>1</v>
+      </c>
+      <c r="CO2">
+        <v>1</v>
+      </c>
+      <c r="CU2">
+        <v>1</v>
+      </c>
+      <c r="DE2">
+        <v>1</v>
+      </c>
+      <c r="DI2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:113" x14ac:dyDescent="0.2">
+      <c r="A3" s="4">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3">
+        <v>72</v>
+      </c>
+      <c r="E3">
         <v>17</v>
       </c>
-    </row>
-    <row r="34" spans="1:110" x14ac:dyDescent="0.2">
+      <c r="F3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" t="s">
+        <v>9</v>
+      </c>
+      <c r="R3">
+        <v>1</v>
+      </c>
+      <c r="W3">
+        <v>1</v>
+      </c>
+      <c r="AC3">
+        <v>1</v>
+      </c>
+      <c r="AI3">
+        <v>1</v>
+      </c>
+      <c r="AX3">
+        <v>1</v>
+      </c>
+      <c r="BI3">
+        <v>1</v>
+      </c>
+      <c r="BL3">
+        <v>1</v>
+      </c>
+      <c r="BY3">
+        <v>1</v>
+      </c>
+      <c r="CJ3">
+        <v>1</v>
+      </c>
+      <c r="CQ3">
+        <v>1</v>
+      </c>
+      <c r="DI3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:113" x14ac:dyDescent="0.2">
+      <c r="A4" s="4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4">
+        <v>144</v>
+      </c>
+      <c r="E4">
+        <v>32</v>
+      </c>
+      <c r="F4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" t="s">
+        <v>14</v>
+      </c>
+      <c r="T4">
+        <v>1</v>
+      </c>
+      <c r="BE4">
+        <v>1</v>
+      </c>
+      <c r="BG4">
+        <v>1</v>
+      </c>
+      <c r="BS4">
+        <v>1</v>
+      </c>
+      <c r="CF4">
+        <v>1</v>
+      </c>
+      <c r="CK4">
+        <v>1</v>
+      </c>
+      <c r="DI4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:113" x14ac:dyDescent="0.2">
+      <c r="A5" s="4">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5">
+        <v>72</v>
+      </c>
+      <c r="E5">
+        <v>48</v>
+      </c>
+      <c r="F5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" t="s">
+        <v>14</v>
+      </c>
+      <c r="V5">
+        <v>1</v>
+      </c>
+      <c r="Y5">
+        <v>1</v>
+      </c>
+      <c r="AB5">
+        <v>1</v>
+      </c>
+      <c r="AS5">
+        <v>1</v>
+      </c>
+      <c r="BE5">
+        <v>1</v>
+      </c>
+      <c r="BS5">
+        <v>1</v>
+      </c>
+      <c r="CN5">
+        <v>1</v>
+      </c>
+      <c r="CO5">
+        <v>1</v>
+      </c>
+      <c r="CU5">
+        <v>1</v>
+      </c>
+      <c r="CX5">
+        <v>1</v>
+      </c>
+      <c r="CZ5">
+        <v>1</v>
+      </c>
+      <c r="DF5">
+        <v>1</v>
+      </c>
+      <c r="DI5">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:113" x14ac:dyDescent="0.2">
+      <c r="A6" s="4">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6">
+        <v>144</v>
+      </c>
+      <c r="E6">
+        <v>44</v>
+      </c>
+      <c r="F6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6" t="s">
+        <v>14</v>
+      </c>
+      <c r="CA6">
+        <v>1</v>
+      </c>
+      <c r="CD6">
+        <v>1</v>
+      </c>
+      <c r="CN6">
+        <v>1</v>
+      </c>
+      <c r="CO6">
+        <v>1</v>
+      </c>
+      <c r="DI6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:113" x14ac:dyDescent="0.2">
+      <c r="A7" s="4">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7">
+        <v>144</v>
+      </c>
+      <c r="E7">
+        <v>86</v>
+      </c>
+      <c r="F7" t="s">
+        <v>20</v>
+      </c>
+      <c r="G7" t="s">
+        <v>9</v>
+      </c>
+      <c r="AQ7">
+        <v>1</v>
+      </c>
+      <c r="AS7">
+        <v>1</v>
+      </c>
+      <c r="BC7">
+        <v>1</v>
+      </c>
+      <c r="BE7">
+        <v>1</v>
+      </c>
+      <c r="BK7">
+        <v>1</v>
+      </c>
+      <c r="BN7">
+        <v>1</v>
+      </c>
+      <c r="CF7">
+        <v>1</v>
+      </c>
+      <c r="CO7">
+        <v>1</v>
+      </c>
+      <c r="CP7">
+        <v>1</v>
+      </c>
+      <c r="CX7">
+        <v>1</v>
+      </c>
+      <c r="DF7">
+        <v>1</v>
+      </c>
+      <c r="DG7">
+        <v>1</v>
+      </c>
+      <c r="DI7">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:113" x14ac:dyDescent="0.2">
+      <c r="A8" s="4">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8">
+        <v>6</v>
+      </c>
+      <c r="E8">
+        <v>40</v>
+      </c>
+      <c r="F8" t="s">
+        <v>21</v>
+      </c>
+      <c r="G8" t="s">
+        <v>14</v>
+      </c>
+      <c r="O8">
+        <v>1</v>
+      </c>
+      <c r="P8">
+        <v>1</v>
+      </c>
+      <c r="U8">
+        <v>1</v>
+      </c>
+      <c r="X8">
+        <v>1</v>
+      </c>
+      <c r="AF8">
+        <v>1</v>
+      </c>
+      <c r="AP8">
+        <v>1</v>
+      </c>
+      <c r="AS8">
+        <v>1</v>
+      </c>
+      <c r="AW8">
+        <v>1</v>
+      </c>
+      <c r="AY8">
+        <v>1</v>
+      </c>
+      <c r="BD8">
+        <v>1</v>
+      </c>
+      <c r="BF8">
+        <v>1</v>
+      </c>
+      <c r="BG8">
+        <v>1</v>
+      </c>
+      <c r="BN8">
+        <v>1</v>
+      </c>
+      <c r="BQ8">
+        <v>1</v>
+      </c>
+      <c r="CG8">
+        <v>1</v>
+      </c>
+      <c r="CI8">
+        <v>1</v>
+      </c>
+      <c r="CK8">
+        <v>1</v>
+      </c>
+      <c r="CT8">
+        <v>1</v>
+      </c>
+      <c r="DA8">
+        <v>1</v>
+      </c>
+      <c r="DI8">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:113" x14ac:dyDescent="0.2">
+      <c r="A9" s="4">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9">
+        <v>6</v>
+      </c>
+      <c r="E9">
+        <v>45</v>
+      </c>
+      <c r="F9" t="s">
+        <v>22</v>
+      </c>
+      <c r="G9" t="s">
+        <v>9</v>
+      </c>
+      <c r="S9">
+        <v>1</v>
+      </c>
+      <c r="T9">
+        <v>1</v>
+      </c>
+      <c r="AF9">
+        <v>1</v>
+      </c>
+      <c r="AG9">
+        <v>1</v>
+      </c>
+      <c r="AQ9">
+        <v>1</v>
+      </c>
+      <c r="AU9">
+        <v>1</v>
+      </c>
+      <c r="AW9">
+        <v>1</v>
+      </c>
+      <c r="AY9">
+        <v>1</v>
+      </c>
+      <c r="BB9">
+        <v>1</v>
+      </c>
+      <c r="BF9">
+        <v>1</v>
+      </c>
+      <c r="BN9">
+        <v>1</v>
+      </c>
+      <c r="BO9">
+        <v>1</v>
+      </c>
+      <c r="BS9">
+        <v>1</v>
+      </c>
+      <c r="BU9">
+        <v>1</v>
+      </c>
+      <c r="BX9">
+        <v>1</v>
+      </c>
+      <c r="CK9">
+        <v>1</v>
+      </c>
+      <c r="CR9">
+        <v>1</v>
+      </c>
+      <c r="CS9">
+        <v>1</v>
+      </c>
+      <c r="CW9">
+        <v>1</v>
+      </c>
+      <c r="DD9">
+        <v>1</v>
+      </c>
+      <c r="DI9">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:113" x14ac:dyDescent="0.2">
+      <c r="A10" s="4">
+        <v>9</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10">
+        <v>144</v>
+      </c>
+      <c r="E10">
+        <v>57</v>
+      </c>
+      <c r="F10" t="s">
+        <v>20</v>
+      </c>
+      <c r="G10" t="s">
+        <v>9</v>
+      </c>
+      <c r="M10">
+        <v>1</v>
+      </c>
+      <c r="AK10">
+        <v>1</v>
+      </c>
+      <c r="AN10">
+        <v>1</v>
+      </c>
+      <c r="BH10">
+        <v>1</v>
+      </c>
+      <c r="CC10">
+        <v>1</v>
+      </c>
+      <c r="CE10">
+        <v>1</v>
+      </c>
+      <c r="CO10">
+        <v>1</v>
+      </c>
+      <c r="CU10">
+        <v>1</v>
+      </c>
+      <c r="CV10">
+        <v>1</v>
+      </c>
+      <c r="DG10">
+        <v>1</v>
+      </c>
+      <c r="DI10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:113" x14ac:dyDescent="0.2">
+      <c r="A11" s="4">
+        <v>10</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11">
+        <v>72</v>
+      </c>
+      <c r="E11">
+        <v>52</v>
+      </c>
+      <c r="F11" t="s">
+        <v>25</v>
+      </c>
+      <c r="G11" t="s">
+        <v>9</v>
+      </c>
+      <c r="P11">
+        <v>1</v>
+      </c>
+      <c r="Q11">
+        <v>1</v>
+      </c>
+      <c r="AQ11">
+        <v>1</v>
+      </c>
+      <c r="BG11">
+        <v>1</v>
+      </c>
+      <c r="BK11">
+        <v>1</v>
+      </c>
+      <c r="BY11">
+        <v>1</v>
+      </c>
+      <c r="DE11">
+        <v>1</v>
+      </c>
+      <c r="DI11">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:113" x14ac:dyDescent="0.2">
+      <c r="A12" s="4">
+        <v>11</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12">
+        <v>72</v>
+      </c>
+      <c r="E12">
+        <v>85</v>
+      </c>
+      <c r="F12" t="s">
+        <v>8</v>
+      </c>
+      <c r="G12" t="s">
+        <v>9</v>
+      </c>
+      <c r="T12">
+        <v>1</v>
+      </c>
+      <c r="Y12">
+        <v>1</v>
+      </c>
+      <c r="Z12">
+        <v>1</v>
+      </c>
+      <c r="AI12">
+        <v>1</v>
+      </c>
+      <c r="AM12">
+        <v>1</v>
+      </c>
+      <c r="AR12">
+        <v>1</v>
+      </c>
+      <c r="AV12">
+        <v>1</v>
+      </c>
+      <c r="AX12">
+        <v>1</v>
+      </c>
+      <c r="BH12">
+        <v>1</v>
+      </c>
+      <c r="BI12">
+        <v>1</v>
+      </c>
+      <c r="BV12">
+        <v>1</v>
+      </c>
+      <c r="CO12">
+        <v>1</v>
+      </c>
+      <c r="CU12">
+        <v>1</v>
+      </c>
+      <c r="DI12">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:113" x14ac:dyDescent="0.2">
+      <c r="A13" s="4">
+        <v>12</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13">
+        <v>72</v>
+      </c>
+      <c r="E13">
+        <v>83</v>
+      </c>
+      <c r="F13" t="s">
+        <v>21</v>
+      </c>
+      <c r="G13" t="s">
+        <v>9</v>
+      </c>
+      <c r="AE13">
+        <v>1</v>
+      </c>
+      <c r="AO13">
+        <v>1</v>
+      </c>
+      <c r="AV13">
+        <v>1</v>
+      </c>
+      <c r="BJ13">
+        <v>1</v>
+      </c>
+      <c r="BQ13">
+        <v>1</v>
+      </c>
+      <c r="DI13">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:113" x14ac:dyDescent="0.2">
+      <c r="A14" s="4">
+        <v>13</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" t="s">
+        <v>27</v>
+      </c>
+      <c r="D14">
+        <v>6</v>
+      </c>
+      <c r="E14">
+        <v>43</v>
+      </c>
+      <c r="F14" t="s">
+        <v>20</v>
+      </c>
+      <c r="G14" t="s">
+        <v>9</v>
+      </c>
+      <c r="X14">
+        <v>1</v>
+      </c>
+      <c r="AU14">
+        <v>1</v>
+      </c>
+      <c r="AW14">
+        <v>1</v>
+      </c>
+      <c r="AY14">
+        <v>1</v>
+      </c>
+      <c r="BD14">
+        <v>1</v>
+      </c>
+      <c r="CS14">
+        <v>1</v>
+      </c>
+      <c r="DI14">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:113" x14ac:dyDescent="0.2">
+      <c r="A15" s="4">
+        <v>14</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" t="s">
+        <v>27</v>
+      </c>
+      <c r="D15">
+        <v>72</v>
+      </c>
+      <c r="E15">
+        <v>64</v>
+      </c>
+      <c r="F15" t="s">
+        <v>20</v>
+      </c>
+      <c r="G15" t="s">
+        <v>9</v>
+      </c>
+      <c r="AK15">
+        <v>1</v>
+      </c>
+      <c r="AL15">
+        <v>1</v>
+      </c>
+      <c r="BK15">
+        <v>1</v>
+      </c>
+      <c r="CD15">
+        <v>1</v>
+      </c>
+      <c r="CN15">
+        <v>1</v>
+      </c>
+      <c r="CP15">
+        <v>1</v>
+      </c>
+      <c r="CU15">
+        <v>1</v>
+      </c>
+      <c r="DB15">
+        <v>1</v>
+      </c>
+      <c r="DE15">
+        <v>1</v>
+      </c>
+      <c r="DI15">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:113" x14ac:dyDescent="0.2">
+      <c r="A16" s="4">
+        <v>15</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" t="s">
+        <v>16</v>
+      </c>
+      <c r="D16">
+        <v>144</v>
+      </c>
+      <c r="E16">
+        <v>19</v>
+      </c>
+      <c r="F16" t="s">
+        <v>29</v>
+      </c>
+      <c r="G16" t="s">
+        <v>9</v>
+      </c>
+      <c r="AL16">
+        <v>1</v>
+      </c>
+      <c r="AX16">
+        <v>1</v>
+      </c>
+      <c r="BH16">
+        <v>1</v>
+      </c>
+      <c r="BK16">
+        <v>1</v>
+      </c>
+      <c r="CN16">
+        <v>1</v>
+      </c>
+      <c r="DG16">
+        <v>1</v>
+      </c>
+      <c r="DI16">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:113" x14ac:dyDescent="0.2">
+      <c r="A17" s="4">
+        <v>16</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" t="s">
+        <v>27</v>
+      </c>
+      <c r="D17">
+        <v>72</v>
+      </c>
+      <c r="E17">
+        <v>88</v>
+      </c>
+      <c r="F17" t="s">
+        <v>25</v>
+      </c>
+      <c r="G17" t="s">
+        <v>9</v>
+      </c>
+      <c r="AB17">
+        <v>1</v>
+      </c>
+      <c r="AO17">
+        <v>1</v>
+      </c>
+      <c r="BH17">
+        <v>1</v>
+      </c>
+      <c r="BV17">
+        <v>1</v>
+      </c>
+      <c r="CV17">
+        <v>1</v>
+      </c>
+      <c r="DI17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:113" x14ac:dyDescent="0.2">
+      <c r="A18" s="4">
+        <v>17</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C18" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18">
+        <v>12</v>
+      </c>
+      <c r="E18">
+        <v>47</v>
+      </c>
+      <c r="F18" t="s">
+        <v>31</v>
+      </c>
+      <c r="G18" t="s">
+        <v>9</v>
+      </c>
+      <c r="R18">
+        <v>1</v>
+      </c>
+      <c r="AC18">
+        <v>1</v>
+      </c>
+      <c r="AJ18">
+        <v>1</v>
+      </c>
+      <c r="BA18">
+        <v>1</v>
+      </c>
+      <c r="BM18">
+        <v>1</v>
+      </c>
+      <c r="BP18">
+        <v>1</v>
+      </c>
+      <c r="BZ18">
+        <v>1</v>
+      </c>
+      <c r="DI18">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:113" x14ac:dyDescent="0.2">
+      <c r="A19" s="4">
+        <v>18</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C19" t="s">
+        <v>12</v>
+      </c>
+      <c r="D19">
+        <v>6</v>
+      </c>
+      <c r="E19">
+        <v>50</v>
+      </c>
+      <c r="F19" t="s">
+        <v>13</v>
+      </c>
+      <c r="G19" t="s">
+        <v>9</v>
+      </c>
+      <c r="L19">
+        <v>1</v>
+      </c>
+      <c r="AQ19">
+        <v>1</v>
+      </c>
+      <c r="AU19">
+        <v>1</v>
+      </c>
+      <c r="AY19">
+        <v>1</v>
+      </c>
+      <c r="BD19">
+        <v>1</v>
+      </c>
+      <c r="BR19">
+        <v>1</v>
+      </c>
+      <c r="BW19">
+        <v>1</v>
+      </c>
+      <c r="BX19">
+        <v>1</v>
+      </c>
+      <c r="CG19">
+        <v>1</v>
+      </c>
+      <c r="CL19">
+        <v>1</v>
+      </c>
+      <c r="CS19">
+        <v>1</v>
+      </c>
+      <c r="CT19">
+        <v>1</v>
+      </c>
+      <c r="CY19">
+        <v>1</v>
+      </c>
+      <c r="DC19">
+        <v>1</v>
+      </c>
+      <c r="DI19">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:113" x14ac:dyDescent="0.2">
+      <c r="A20" s="4">
+        <v>19</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C20" t="s">
+        <v>15</v>
+      </c>
+      <c r="D20">
+        <v>12</v>
+      </c>
+      <c r="E20">
+        <v>66</v>
+      </c>
+      <c r="F20" t="s">
+        <v>31</v>
+      </c>
+      <c r="G20" t="s">
+        <v>9</v>
+      </c>
+      <c r="P20">
+        <v>1</v>
+      </c>
+      <c r="AS20">
+        <v>1</v>
+      </c>
+      <c r="BN20">
+        <v>1</v>
+      </c>
+      <c r="BT20">
+        <v>1</v>
+      </c>
+      <c r="CK20">
+        <v>1</v>
+      </c>
+      <c r="DI20">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:113" x14ac:dyDescent="0.2">
+      <c r="A21" s="4">
+        <v>20</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C21" t="s">
+        <v>16</v>
+      </c>
+      <c r="D21">
+        <v>72</v>
+      </c>
+      <c r="E21">
+        <v>82</v>
+      </c>
+      <c r="F21" t="s">
+        <v>29</v>
+      </c>
+      <c r="G21" t="s">
+        <v>9</v>
+      </c>
+      <c r="AB21">
+        <v>1</v>
+      </c>
+      <c r="AM21">
+        <v>1</v>
+      </c>
+      <c r="BC21">
+        <v>1</v>
+      </c>
+      <c r="BV21">
+        <v>1</v>
+      </c>
+      <c r="CN21">
+        <v>1</v>
+      </c>
+      <c r="CO21">
+        <v>1</v>
+      </c>
+      <c r="DI21">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:113" x14ac:dyDescent="0.2">
+      <c r="A22" s="4">
+        <v>21</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C22" t="s">
+        <v>15</v>
+      </c>
+      <c r="D22">
+        <v>12</v>
+      </c>
+      <c r="E22">
+        <v>50</v>
+      </c>
+      <c r="F22" t="s">
+        <v>25</v>
+      </c>
+      <c r="G22" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q22">
+        <v>1</v>
+      </c>
+      <c r="CK22">
+        <v>1</v>
+      </c>
+      <c r="CL22">
+        <v>1</v>
+      </c>
+      <c r="DF22">
+        <v>1</v>
+      </c>
+      <c r="DI22">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:113" x14ac:dyDescent="0.2">
+      <c r="A23" s="4">
+        <v>22</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C23" t="s">
+        <v>15</v>
+      </c>
+      <c r="D23">
+        <v>72</v>
+      </c>
+      <c r="E23">
+        <v>63</v>
+      </c>
+      <c r="F23" t="s">
+        <v>8</v>
+      </c>
+      <c r="G23" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q23">
+        <v>1</v>
+      </c>
+      <c r="T23">
+        <v>1</v>
+      </c>
+      <c r="V23">
+        <v>1</v>
+      </c>
+      <c r="AE23">
+        <v>1</v>
+      </c>
+      <c r="AH23">
+        <v>1</v>
+      </c>
+      <c r="AI23">
+        <v>1</v>
+      </c>
+      <c r="AK23">
+        <v>1</v>
+      </c>
+      <c r="AR23">
+        <v>1</v>
+      </c>
+      <c r="AS23">
+        <v>1</v>
+      </c>
+      <c r="AV23">
+        <v>1</v>
+      </c>
+      <c r="AX23">
+        <v>1</v>
+      </c>
+      <c r="BE23">
+        <v>1</v>
+      </c>
+      <c r="BK23">
+        <v>1</v>
+      </c>
+      <c r="BN23">
+        <v>1</v>
+      </c>
+      <c r="CB23">
+        <v>1</v>
+      </c>
+      <c r="CF23">
+        <v>1</v>
+      </c>
+      <c r="CK23">
+        <v>1</v>
+      </c>
+      <c r="CN23">
+        <v>1</v>
+      </c>
+      <c r="DB23">
+        <v>1</v>
+      </c>
+      <c r="DC23">
+        <v>1</v>
+      </c>
+      <c r="DG23">
+        <v>1</v>
+      </c>
+      <c r="DI23">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:113" x14ac:dyDescent="0.2">
+      <c r="A24" s="4">
+        <v>23</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C24" t="s">
+        <v>24</v>
+      </c>
+      <c r="D24">
+        <v>144</v>
+      </c>
+      <c r="E24">
+        <v>39</v>
+      </c>
+      <c r="F24" t="s">
+        <v>22</v>
+      </c>
+      <c r="G24" t="s">
+        <v>9</v>
+      </c>
+      <c r="AK24">
+        <v>1</v>
+      </c>
+      <c r="BK24">
+        <v>1</v>
+      </c>
+      <c r="BY24">
+        <v>1</v>
+      </c>
+      <c r="CE24">
+        <v>1</v>
+      </c>
+      <c r="CP24">
+        <v>1</v>
+      </c>
+      <c r="DI24">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:113" x14ac:dyDescent="0.2">
+      <c r="A25" s="4">
+        <v>24</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C25" t="s">
+        <v>10</v>
+      </c>
+      <c r="D25">
+        <v>6</v>
+      </c>
+      <c r="E25">
+        <v>34</v>
+      </c>
+      <c r="F25" t="s">
+        <v>29</v>
+      </c>
+      <c r="G25" t="s">
+        <v>9</v>
+      </c>
+      <c r="N25">
+        <v>1</v>
+      </c>
+      <c r="R25">
+        <v>1</v>
+      </c>
+      <c r="W25">
+        <v>1</v>
+      </c>
+      <c r="AA25">
+        <v>1</v>
+      </c>
+      <c r="AC25">
+        <v>1</v>
+      </c>
+      <c r="AJ25">
+        <v>1</v>
+      </c>
+      <c r="AZ25">
+        <v>1</v>
+      </c>
+      <c r="BA25">
+        <v>1</v>
+      </c>
+      <c r="BM25">
+        <v>1</v>
+      </c>
+      <c r="BP25">
+        <v>1</v>
+      </c>
+      <c r="BZ25">
+        <v>1</v>
+      </c>
+      <c r="CQ25">
+        <v>1</v>
+      </c>
+      <c r="DI25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="26" spans="1:113" x14ac:dyDescent="0.2">
+      <c r="A26" s="4">
+        <v>25</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C26" t="s">
+        <v>16</v>
+      </c>
+      <c r="D26">
+        <v>72</v>
+      </c>
+      <c r="E26">
+        <v>59</v>
+      </c>
+      <c r="F26" t="s">
+        <v>13</v>
+      </c>
+      <c r="G26" t="s">
+        <v>14</v>
+      </c>
+      <c r="AE26">
+        <v>1</v>
+      </c>
+      <c r="AM26">
+        <v>1</v>
+      </c>
+      <c r="BJ26">
+        <v>1</v>
+      </c>
+      <c r="CO26">
+        <v>1</v>
+      </c>
+      <c r="CV26">
+        <v>1</v>
+      </c>
+      <c r="DB26">
+        <v>1</v>
+      </c>
+      <c r="DI26">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:113" x14ac:dyDescent="0.2">
+      <c r="A27" s="4">
+        <v>26</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C27" t="s">
+        <v>10</v>
+      </c>
+      <c r="D27">
+        <v>144</v>
+      </c>
+      <c r="E27">
+        <v>83</v>
+      </c>
+      <c r="F27" t="s">
+        <v>21</v>
+      </c>
+      <c r="G27" t="s">
+        <v>9</v>
+      </c>
+      <c r="N27">
+        <v>1</v>
+      </c>
+      <c r="R27">
+        <v>1</v>
+      </c>
+      <c r="W27">
+        <v>1</v>
+      </c>
+      <c r="AA27">
+        <v>1</v>
+      </c>
+      <c r="AC27">
+        <v>1</v>
+      </c>
+      <c r="AO27">
+        <v>1</v>
+      </c>
+      <c r="AZ27">
+        <v>1</v>
+      </c>
+      <c r="BA27">
+        <v>1</v>
+      </c>
+      <c r="BP27">
+        <v>1</v>
+      </c>
+      <c r="BY27">
+        <v>1</v>
+      </c>
+      <c r="CJ27">
+        <v>1</v>
+      </c>
+      <c r="CM27">
+        <v>1</v>
+      </c>
+      <c r="CN27">
+        <v>1</v>
+      </c>
+      <c r="CO27">
+        <v>1</v>
+      </c>
+      <c r="CU27">
+        <v>1</v>
+      </c>
+      <c r="DI27">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="28" spans="1:113" x14ac:dyDescent="0.2">
+      <c r="A28" s="4">
+        <v>27</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C28" t="s">
+        <v>15</v>
+      </c>
+      <c r="D28">
+        <v>72</v>
+      </c>
+      <c r="E28">
+        <v>88</v>
+      </c>
+      <c r="F28" t="s">
+        <v>17</v>
+      </c>
+      <c r="G28" t="s">
+        <v>9</v>
+      </c>
+      <c r="M28">
+        <v>1</v>
+      </c>
+      <c r="AG28">
+        <v>1</v>
+      </c>
+      <c r="AH28">
+        <v>1</v>
+      </c>
+      <c r="AS28">
+        <v>1</v>
+      </c>
+      <c r="BE28">
+        <v>1</v>
+      </c>
+      <c r="BH28">
+        <v>1</v>
+      </c>
+      <c r="BY28">
+        <v>1</v>
+      </c>
+      <c r="CX28">
+        <v>1</v>
+      </c>
+      <c r="DF28">
+        <v>1</v>
+      </c>
+      <c r="DI28">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="29" spans="1:113" x14ac:dyDescent="0.2">
+      <c r="A29" s="4">
+        <v>28</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C29" t="s">
+        <v>16</v>
+      </c>
+      <c r="D29">
+        <v>12</v>
+      </c>
+      <c r="E29">
+        <v>56</v>
+      </c>
+      <c r="F29" t="s">
+        <v>8</v>
+      </c>
+      <c r="G29" t="s">
+        <v>14</v>
+      </c>
+      <c r="V29">
+        <v>1</v>
+      </c>
+      <c r="Y29">
+        <v>1</v>
+      </c>
+      <c r="AI29">
+        <v>1</v>
+      </c>
+      <c r="AT29">
+        <v>1</v>
+      </c>
+      <c r="BI29">
+        <v>1</v>
+      </c>
+      <c r="BJ29">
+        <v>1</v>
+      </c>
+      <c r="DI29">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:113" x14ac:dyDescent="0.2">
+      <c r="A30" s="4">
+        <v>29</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C30" t="s">
+        <v>36</v>
+      </c>
+      <c r="D30">
+        <v>6</v>
+      </c>
+      <c r="E30">
+        <v>87</v>
+      </c>
+      <c r="F30" t="s">
+        <v>8</v>
+      </c>
+      <c r="G30" t="s">
+        <v>9</v>
+      </c>
+      <c r="L30">
+        <v>1</v>
+      </c>
+      <c r="S30">
+        <v>1</v>
+      </c>
+      <c r="U30">
+        <v>1</v>
+      </c>
+      <c r="X30">
+        <v>1</v>
+      </c>
+      <c r="AD30">
+        <v>1</v>
+      </c>
+      <c r="AF30">
+        <v>1</v>
+      </c>
+      <c r="AT30">
+        <v>1</v>
+      </c>
+      <c r="AW30">
+        <v>1</v>
+      </c>
+      <c r="BD30">
+        <v>1</v>
+      </c>
+      <c r="BO30">
+        <v>1</v>
+      </c>
+      <c r="BV30">
+        <v>1</v>
+      </c>
+      <c r="BX30">
+        <v>1</v>
+      </c>
+      <c r="CI30">
+        <v>1</v>
+      </c>
+      <c r="CR30">
+        <v>1</v>
+      </c>
+      <c r="CT30">
+        <v>1</v>
+      </c>
+      <c r="CY30">
+        <v>1</v>
+      </c>
+      <c r="DA30">
+        <v>1</v>
+      </c>
+      <c r="DI30">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="31" spans="1:113" x14ac:dyDescent="0.2">
+      <c r="A31" s="4">
+        <v>30</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C31" t="s">
+        <v>7</v>
+      </c>
+      <c r="D31">
+        <v>6</v>
+      </c>
+      <c r="E31">
+        <v>54</v>
+      </c>
+      <c r="F31" t="s">
+        <v>8</v>
+      </c>
+      <c r="G31" t="s">
+        <v>9</v>
+      </c>
+      <c r="L31">
+        <v>1</v>
+      </c>
+      <c r="O31">
+        <v>1</v>
+      </c>
+      <c r="U31">
+        <v>1</v>
+      </c>
+      <c r="V31">
+        <v>1</v>
+      </c>
+      <c r="X31">
+        <v>1</v>
+      </c>
+      <c r="Z31">
+        <v>1</v>
+      </c>
+      <c r="AD31">
+        <v>1</v>
+      </c>
+      <c r="AF31">
+        <v>1</v>
+      </c>
+      <c r="AI31">
+        <v>1</v>
+      </c>
+      <c r="AU31">
+        <v>1</v>
+      </c>
+      <c r="AW31">
+        <v>1</v>
+      </c>
+      <c r="AY31">
+        <v>1</v>
+      </c>
+      <c r="BF31">
+        <v>1</v>
+      </c>
+      <c r="BR31">
+        <v>1</v>
+      </c>
+      <c r="BW31">
+        <v>1</v>
+      </c>
+      <c r="BX31">
+        <v>1</v>
+      </c>
+      <c r="CB31">
+        <v>1</v>
+      </c>
+      <c r="CR31">
+        <v>1</v>
+      </c>
+      <c r="CT31">
+        <v>1</v>
+      </c>
+      <c r="CV31">
+        <v>1</v>
+      </c>
+      <c r="DB31">
+        <v>1</v>
+      </c>
+      <c r="DD31">
+        <v>1</v>
+      </c>
+      <c r="DI31">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="32" spans="1:113" x14ac:dyDescent="0.2">
+      <c r="A32" s="4">
+        <v>31</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C32" t="s">
+        <v>15</v>
+      </c>
+      <c r="D32">
+        <v>72</v>
+      </c>
+      <c r="E32">
+        <v>89</v>
+      </c>
+      <c r="F32" t="s">
+        <v>8</v>
+      </c>
+      <c r="G32" t="s">
+        <v>9</v>
+      </c>
+      <c r="P32">
+        <v>1</v>
+      </c>
+      <c r="Q32">
+        <v>1</v>
+      </c>
+      <c r="Y32">
+        <v>1</v>
+      </c>
+      <c r="AI32">
+        <v>1</v>
+      </c>
+      <c r="AN32">
+        <v>1</v>
+      </c>
+      <c r="BC32">
+        <v>1</v>
+      </c>
+      <c r="BK32">
+        <v>1</v>
+      </c>
+      <c r="BN32">
+        <v>1</v>
+      </c>
+      <c r="BS32">
+        <v>1</v>
+      </c>
+      <c r="BT32">
+        <v>1</v>
+      </c>
+      <c r="BV32">
+        <v>1</v>
+      </c>
+      <c r="CB32">
+        <v>1</v>
+      </c>
+      <c r="CH32">
+        <v>1</v>
+      </c>
+      <c r="CX32">
+        <v>1</v>
+      </c>
+      <c r="DC32">
+        <v>1</v>
+      </c>
+      <c r="DE32">
+        <v>1</v>
+      </c>
+      <c r="DG32">
+        <v>1</v>
+      </c>
+      <c r="DI32">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="33" spans="1:113" x14ac:dyDescent="0.2">
+      <c r="A33" s="4">
+        <v>32</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C33" t="s">
+        <v>16</v>
+      </c>
+      <c r="D33">
+        <v>72</v>
+      </c>
+      <c r="E33">
+        <v>45</v>
+      </c>
+      <c r="F33" t="s">
+        <v>31</v>
+      </c>
+      <c r="G33" t="s">
+        <v>14</v>
+      </c>
+      <c r="AB33">
+        <v>1</v>
+      </c>
+      <c r="AM33">
+        <v>1</v>
+      </c>
+      <c r="BC33">
+        <v>1</v>
+      </c>
+      <c r="DG33">
+        <v>1</v>
+      </c>
+      <c r="DI33">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:113" x14ac:dyDescent="0.2">
+      <c r="G34" t="s">
+        <v>149</v>
+      </c>
+      <c r="L34">
+        <f t="array" ref="L34">SQRT(SUM((L$2:L$33-$H$2:$H$33)^2))</f>
+        <v>1.7320508075688772</v>
+      </c>
+      <c r="M34">
+        <f t="array" ref="M34">SQRT(SUM((M$2:M$33-$H$2:$H$33)^2))</f>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="N34">
+        <f t="array" ref="N34">SQRT(SUM((N$2:N$33-$H$2:$H$33)^2))</f>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="O34">
+        <f t="array" ref="O34">SQRT(SUM((O$2:O$33-$H$2:$H$33)^2))</f>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="P34">
+        <f t="array" ref="P34">SQRT(SUM((P$2:P$33-$H$2:$H$33)^2))</f>
+        <v>2</v>
+      </c>
+      <c r="Q34">
+        <f t="array" ref="Q34">SQRT(SUM((Q$2:Q$33-$H$2:$H$33)^2))</f>
+        <v>2</v>
+      </c>
+      <c r="R34">
+        <f t="array" ref="R34">SQRT(SUM((R$2:R$33-$H$2:$H$33)^2))</f>
+        <v>2</v>
+      </c>
+      <c r="S34">
+        <f t="array" ref="S34">SQRT(SUM((S$2:S$33-$H$2:$H$33)^2))</f>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="T34">
+        <f t="array" ref="T34">SQRT(SUM((T$2:T$33-$H$2:$H$33)^2))</f>
+        <v>2</v>
+      </c>
+      <c r="U34">
+        <f t="array" ref="U34">SQRT(SUM((U$2:U$33-$H$2:$H$33)^2))</f>
+        <v>1.7320508075688772</v>
+      </c>
+      <c r="V34">
+        <f t="array" ref="V34">SQRT(SUM((V$2:V$33-$H$2:$H$33)^2))</f>
+        <v>2.2360679774997898</v>
+      </c>
+      <c r="W34">
+        <f t="array" ref="W34">SQRT(SUM((W$2:W$33-$H$2:$H$33)^2))</f>
+        <v>1.7320508075688772</v>
+      </c>
+      <c r="X34">
+        <f t="array" ref="X34">SQRT(SUM((X$2:X$33-$H$2:$H$33)^2))</f>
+        <v>2</v>
+      </c>
+      <c r="Y34">
+        <f t="array" ref="Y34">SQRT(SUM((Y$2:Y$33-$H$2:$H$33)^2))</f>
+        <v>2</v>
+      </c>
+      <c r="Z34">
+        <f t="array" ref="Z34">SQRT(SUM((Z$2:Z$33-$H$2:$H$33)^2))</f>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="AA34">
+        <f t="array" ref="AA34">SQRT(SUM((AA$2:AA$33-$H$2:$H$33)^2))</f>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="AB34">
+        <f t="array" ref="AB34">SQRT(SUM((AB$2:AB$33-$H$2:$H$33)^2))</f>
+        <v>2</v>
+      </c>
+      <c r="AC34">
+        <f t="array" ref="AC34">SQRT(SUM((AC$2:AC$33-$H$2:$H$33)^2))</f>
+        <v>2</v>
+      </c>
+      <c r="AD34">
+        <f t="array" ref="AD34">SQRT(SUM((AD$2:AD$33-$H$2:$H$33)^2))</f>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="AE34">
+        <f t="array" ref="AE34">SQRT(SUM((AE$2:AE$33-$H$2:$H$33)^2))</f>
+        <v>1.7320508075688772</v>
+      </c>
+      <c r="AF34">
+        <f t="array" ref="AF34">SQRT(SUM((AF$2:AF$33-$H$2:$H$33)^2))</f>
+        <v>2</v>
+      </c>
+      <c r="AG34">
+        <f t="array" ref="AG34">SQRT(SUM((AG$2:AG$33-$H$2:$H$33)^2))</f>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="AH34">
+        <f t="array" ref="AH34">SQRT(SUM((AH$2:AH$33-$H$2:$H$33)^2))</f>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="AI34">
+        <f t="array" ref="AI34">SQRT(SUM((AI$2:AI$33-$H$2:$H$33)^2))</f>
+        <v>2.6457513110645907</v>
+      </c>
+      <c r="AJ34">
+        <f t="array" ref="AJ34">SQRT(SUM((AJ$2:AJ$33-$H$2:$H$33)^2))</f>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="AK34">
+        <f t="array" ref="AK34">SQRT(SUM((AK$2:AK$33-$H$2:$H$33)^2))</f>
+        <v>2.2360679774997898</v>
+      </c>
+      <c r="AL34">
+        <f t="array" ref="AL34">SQRT(SUM((AL$2:AL$33-$H$2:$H$33)^2))</f>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="AM34">
+        <f t="array" ref="AM34">SQRT(SUM((AM$2:AM$33-$H$2:$H$33)^2))</f>
+        <v>2</v>
+      </c>
+      <c r="AN34">
+        <f t="array" ref="AN34">SQRT(SUM((AN$2:AN$33-$H$2:$H$33)^2))</f>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="AO34">
+        <f t="array" ref="AO34">SQRT(SUM((AO$2:AO$33-$H$2:$H$33)^2))</f>
+        <v>1.7320508075688772</v>
+      </c>
+      <c r="AP34">
+        <f t="array" ref="AP34">SQRT(SUM((AP$2:AP$33-$H$2:$H$33)^2))</f>
+        <v>1</v>
+      </c>
+      <c r="AQ34">
+        <f t="array" ref="AQ34">SQRT(SUM((AQ$2:AQ$33-$H$2:$H$33)^2))</f>
+        <v>2</v>
+      </c>
+      <c r="AR34">
+        <f t="array" ref="AR34">SQRT(SUM((AR$2:AR$33-$H$2:$H$33)^2))</f>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="AS34">
+        <f t="array" ref="AS34">SQRT(SUM((AS$2:AS$33-$H$2:$H$33)^2))</f>
+        <v>2.4494897427831779</v>
+      </c>
+      <c r="AT34">
+        <f t="array" ref="AT34">SQRT(SUM((AT$2:AT$33-$H$2:$H$33)^2))</f>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="AU34">
+        <f t="array" ref="AU34">SQRT(SUM((AU$2:AU$33-$H$2:$H$33)^2))</f>
+        <v>2</v>
+      </c>
+      <c r="AV34">
+        <f t="array" ref="AV34">SQRT(SUM((AV$2:AV$33-$H$2:$H$33)^2))</f>
+        <v>1.7320508075688772</v>
+      </c>
+      <c r="AW34">
+        <f t="array" ref="AW34">SQRT(SUM((AW$2:AW$33-$H$2:$H$33)^2))</f>
+        <v>2.2360679774997898</v>
+      </c>
+      <c r="AX34">
+        <f t="array" ref="AX34">SQRT(SUM((AX$2:AX$33-$H$2:$H$33)^2))</f>
+        <v>2.2360679774997898</v>
+      </c>
+      <c r="AY34">
+        <f t="array" ref="AY34">SQRT(SUM((AY$2:AY$33-$H$2:$H$33)^2))</f>
+        <v>2.2360679774997898</v>
+      </c>
+      <c r="AZ34">
+        <f t="array" ref="AZ34">SQRT(SUM((AZ$2:AZ$33-$H$2:$H$33)^2))</f>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="BA34">
+        <f t="array" ref="BA34">SQRT(SUM((BA$2:BA$33-$H$2:$H$33)^2))</f>
+        <v>1.7320508075688772</v>
+      </c>
+      <c r="BB34">
+        <f t="array" ref="BB34">SQRT(SUM((BB$2:BB$33-$H$2:$H$33)^2))</f>
+        <v>1</v>
+      </c>
+      <c r="BC34">
+        <f t="array" ref="BC34">SQRT(SUM((BC$2:BC$33-$H$2:$H$33)^2))</f>
+        <v>2</v>
+      </c>
+      <c r="BD34">
+        <f t="array" ref="BD34">SQRT(SUM((BD$2:BD$33-$H$2:$H$33)^2))</f>
+        <v>2</v>
+      </c>
+      <c r="BE34">
+        <f t="array" ref="BE34">SQRT(SUM((BE$2:BE$33-$H$2:$H$33)^2))</f>
+        <v>2.2360679774997898</v>
+      </c>
+      <c r="BF34">
+        <f t="array" ref="BF34">SQRT(SUM((BF$2:BF$33-$H$2:$H$33)^2))</f>
+        <v>1.7320508075688772</v>
+      </c>
+      <c r="BG34">
+        <f t="array" ref="BG34">SQRT(SUM((BG$2:BG$33-$H$2:$H$33)^2))</f>
+        <v>1.7320508075688772</v>
+      </c>
+      <c r="BH34">
+        <f t="array" ref="BH34">SQRT(SUM((BH$2:BH$33-$H$2:$H$33)^2))</f>
+        <v>2.2360679774997898</v>
+      </c>
+      <c r="BI34">
+        <f t="array" ref="BI34">SQRT(SUM((BI$2:BI$33-$H$2:$H$33)^2))</f>
+        <v>1.7320508075688772</v>
+      </c>
+      <c r="BJ34">
+        <f t="array" ref="BJ34">SQRT(SUM((BJ$2:BJ$33-$H$2:$H$33)^2))</f>
+        <v>1.7320508075688772</v>
+      </c>
+      <c r="BK34">
+        <f t="array" ref="BK34">SQRT(SUM((BK$2:BK$33-$H$2:$H$33)^2))</f>
+        <v>2.6457513110645907</v>
+      </c>
+      <c r="BL34">
+        <f t="array" ref="BL34">SQRT(SUM((BL$2:BL$33-$H$2:$H$33)^2))</f>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="BM34">
+        <f t="array" ref="BM34">SQRT(SUM((BM$2:BM$33-$H$2:$H$33)^2))</f>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="BN34">
+        <f t="array" ref="BN34">SQRT(SUM((BN$2:BN$33-$H$2:$H$33)^2))</f>
+        <v>2.4494897427831779</v>
+      </c>
+      <c r="BO34">
+        <f t="array" ref="BO34">SQRT(SUM((BO$2:BO$33-$H$2:$H$33)^2))</f>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="BP34">
+        <f t="array" ref="BP34">SQRT(SUM((BP$2:BP$33-$H$2:$H$33)^2))</f>
+        <v>1.7320508075688772</v>
+      </c>
+      <c r="BQ34">
+        <f t="array" ref="BQ34">SQRT(SUM((BQ$2:BQ$33-$H$2:$H$33)^2))</f>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="BR34">
+        <f t="array" ref="BR34">SQRT(SUM((BR$2:BR$33-$H$2:$H$33)^2))</f>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="BS34">
+        <f t="array" ref="BS34">SQRT(SUM((BS$2:BS$33-$H$2:$H$33)^2))</f>
+        <v>2</v>
+      </c>
+      <c r="BT34">
+        <f t="array" ref="BT34">SQRT(SUM((BT$2:BT$33-$H$2:$H$33)^2))</f>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="BU34">
+        <f t="array" ref="BU34">SQRT(SUM((BU$2:BU$33-$H$2:$H$33)^2))</f>
+        <v>1</v>
+      </c>
+      <c r="BV34">
+        <f t="array" ref="BV34">SQRT(SUM((BV$2:BV$33-$H$2:$H$33)^2))</f>
+        <v>2.2360679774997898</v>
+      </c>
+      <c r="BW34">
+        <f t="array" ref="BW34">SQRT(SUM((BW$2:BW$33-$H$2:$H$33)^2))</f>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="BX34">
+        <f t="array" ref="BX34">SQRT(SUM((BX$2:BX$33-$H$2:$H$33)^2))</f>
+        <v>2</v>
+      </c>
+      <c r="BY34">
+        <f t="array" ref="BY34">SQRT(SUM((BY$2:BY$33-$H$2:$H$33)^2))</f>
+        <v>2.4494897427831779</v>
+      </c>
+      <c r="BZ34">
+        <f t="array" ref="BZ34">SQRT(SUM((BZ$2:BZ$33-$H$2:$H$33)^2))</f>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="CA34">
+        <f t="array" ref="CA34">SQRT(SUM((CA$2:CA$33-$H$2:$H$33)^2))</f>
+        <v>1</v>
+      </c>
+      <c r="CB34">
+        <f t="array" ref="CB34">SQRT(SUM((CB$2:CB$33-$H$2:$H$33)^2))</f>
+        <v>2</v>
+      </c>
+      <c r="CC34">
+        <f t="array" ref="CC34">SQRT(SUM((CC$2:CC$33-$H$2:$H$33)^2))</f>
+        <v>1</v>
+      </c>
+      <c r="CD34">
+        <f t="array" ref="CD34">SQRT(SUM((CD$2:CD$33-$H$2:$H$33)^2))</f>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="CE34">
+        <f t="array" ref="CE34">SQRT(SUM((CE$2:CE$33-$H$2:$H$33)^2))</f>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="CF34">
+        <f t="array" ref="CF34">SQRT(SUM((CF$2:CF$33-$H$2:$H$33)^2))</f>
+        <v>1.7320508075688772</v>
+      </c>
+      <c r="CG34">
+        <f t="array" ref="CG34">SQRT(SUM((CG$2:CG$33-$H$2:$H$33)^2))</f>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="CH34">
+        <f t="array" ref="CH34">SQRT(SUM((CH$2:CH$33-$H$2:$H$33)^2))</f>
+        <v>1</v>
+      </c>
+      <c r="CI34">
+        <f t="array" ref="CI34">SQRT(SUM((CI$2:CI$33-$H$2:$H$33)^2))</f>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="CJ34">
+        <f t="array" ref="CJ34">SQRT(SUM((CJ$2:CJ$33-$H$2:$H$33)^2))</f>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="CK34">
+        <f t="array" ref="CK34">SQRT(SUM((CK$2:CK$33-$H$2:$H$33)^2))</f>
+        <v>2.4494897427831779</v>
+      </c>
+      <c r="CL34">
+        <f t="array" ref="CL34">SQRT(SUM((CL$2:CL$33-$H$2:$H$33)^2))</f>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="CM34">
+        <f t="array" ref="CM34">SQRT(SUM((CM$2:CM$33-$H$2:$H$33)^2))</f>
+        <v>1</v>
+      </c>
+      <c r="CN34">
+        <f t="array" ref="CN34">SQRT(SUM((CN$2:CN$33-$H$2:$H$33)^2))</f>
+        <v>2.6457513110645907</v>
+      </c>
+      <c r="CO34">
+        <f t="array" ref="CO34">SQRT(SUM((CO$2:CO$33-$H$2:$H$33)^2))</f>
+        <v>3</v>
+      </c>
+      <c r="CP34">
+        <f t="array" ref="CP34">SQRT(SUM((CP$2:CP$33-$H$2:$H$33)^2))</f>
+        <v>1.7320508075688772</v>
+      </c>
+      <c r="CQ34">
+        <f t="array" ref="CQ34">SQRT(SUM((CQ$2:CQ$33-$H$2:$H$33)^2))</f>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="CR34">
+        <f t="array" ref="CR34">SQRT(SUM((CR$2:CR$33-$H$2:$H$33)^2))</f>
+        <v>1.7320508075688772</v>
+      </c>
+      <c r="CS34">
+        <f t="array" ref="CS34">SQRT(SUM((CS$2:CS$33-$H$2:$H$33)^2))</f>
+        <v>1.7320508075688772</v>
+      </c>
+      <c r="CT34">
+        <f t="array" ref="CT34">SQRT(SUM((CT$2:CT$33-$H$2:$H$33)^2))</f>
+        <v>2</v>
+      </c>
+      <c r="CU34">
+        <f t="array" ref="CU34">SQRT(SUM((CU$2:CU$33-$H$2:$H$33)^2))</f>
+        <v>2.4494897427831779</v>
+      </c>
+      <c r="CV34">
+        <f t="array" ref="CV34">SQRT(SUM((CV$2:CV$33-$H$2:$H$33)^2))</f>
+        <v>2</v>
+      </c>
+      <c r="CW34">
+        <f t="array" ref="CW34">SQRT(SUM((CW$2:CW$33-$H$2:$H$33)^2))</f>
+        <v>1</v>
+      </c>
+      <c r="CX34">
+        <f t="array" ref="CX34">SQRT(SUM((CX$2:CX$33-$H$2:$H$33)^2))</f>
+        <v>2</v>
+      </c>
+      <c r="CY34">
+        <f t="array" ref="CY34">SQRT(SUM((CY$2:CY$33-$H$2:$H$33)^2))</f>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="CZ34">
+        <f t="array" ref="CZ34">SQRT(SUM((CZ$2:CZ$33-$H$2:$H$33)^2))</f>
+        <v>1</v>
+      </c>
+      <c r="DA34">
+        <f t="array" ref="DA34">SQRT(SUM((DA$2:DA$33-$H$2:$H$33)^2))</f>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="DB34">
+        <f t="array" ref="DB34">SQRT(SUM((DB$2:DB$33-$H$2:$H$33)^2))</f>
+        <v>2</v>
+      </c>
+      <c r="DC34">
+        <f t="array" ref="DC34">SQRT(SUM((DC$2:DC$33-$H$2:$H$33)^2))</f>
+        <v>1.7320508075688772</v>
+      </c>
+      <c r="DD34">
+        <f t="array" ref="DD34">SQRT(SUM((DD$2:DD$33-$H$2:$H$33)^2))</f>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="DE34">
+        <f t="array" ref="DE34">SQRT(SUM((DE$2:DE$33-$H$2:$H$33)^2))</f>
+        <v>2</v>
+      </c>
       <c r="DF34">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="36" spans="1:110" x14ac:dyDescent="0.2">
+        <f t="array" ref="DF34">SQRT(SUM((DF$2:DF$33-$H$2:$H$33)^2))</f>
+        <v>2</v>
+      </c>
+      <c r="DG34">
+        <f t="array" ref="DG34">SQRT(SUM((DG$2:DG$33-$H$2:$H$33)^2))</f>
+        <v>2.4494897427831779</v>
+      </c>
+    </row>
+    <row r="35" spans="1:113" x14ac:dyDescent="0.2">
+      <c r="G35" t="s">
+        <v>150</v>
+      </c>
+      <c r="L35">
+        <f t="array" ref="L35">SQRT(SUM((L$2:L$33-$I$2:$I$33)^2))</f>
+        <v>1.7320508075688772</v>
+      </c>
+      <c r="M35">
+        <f t="array" ref="M35">SQRT(SUM((M$2:M$33-$I$2:$I$33)^2))</f>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="N35">
+        <f t="array" ref="N35">SQRT(SUM((N$2:N$33-$I$2:$I$33)^2))</f>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="O35">
+        <f t="array" ref="O35">SQRT(SUM((O$2:O$33-$I$2:$I$33)^2))</f>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="P35">
+        <f t="array" ref="P35">SQRT(SUM((P$2:P$33-$I$2:$I$33)^2))</f>
+        <v>2</v>
+      </c>
+      <c r="Q35">
+        <f t="array" ref="Q35">SQRT(SUM((Q$2:Q$33-$I$2:$I$33)^2))</f>
+        <v>2</v>
+      </c>
+      <c r="R35">
+        <f t="array" ref="R35">SQRT(SUM((R$2:R$33-$I$2:$I$33)^2))</f>
+        <v>2</v>
+      </c>
+      <c r="S35">
+        <f t="array" ref="S35">SQRT(SUM((S$2:S$33-$I$2:$I$33)^2))</f>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="T35">
+        <f t="array" ref="T35">SQRT(SUM((T$2:T$33-$I$2:$I$33)^2))</f>
+        <v>2</v>
+      </c>
+      <c r="U35">
+        <f t="array" ref="U35">SQRT(SUM((U$2:U$33-$I$2:$I$33)^2))</f>
+        <v>1.7320508075688772</v>
+      </c>
+      <c r="V35">
+        <f t="array" ref="V35">SQRT(SUM((V$2:V$33-$I$2:$I$33)^2))</f>
+        <v>2.2360679774997898</v>
+      </c>
+      <c r="W35">
+        <f t="array" ref="W35">SQRT(SUM((W$2:W$33-$I$2:$I$33)^2))</f>
+        <v>1.7320508075688772</v>
+      </c>
+      <c r="X35">
+        <f t="array" ref="X35">SQRT(SUM((X$2:X$33-$I$2:$I$33)^2))</f>
+        <v>2</v>
+      </c>
+      <c r="Y35">
+        <f t="array" ref="Y35">SQRT(SUM((Y$2:Y$33-$I$2:$I$33)^2))</f>
+        <v>2</v>
+      </c>
+      <c r="Z35">
+        <f t="array" ref="Z35">SQRT(SUM((Z$2:Z$33-$I$2:$I$33)^2))</f>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="AA35">
+        <f t="array" ref="AA35">SQRT(SUM((AA$2:AA$33-$I$2:$I$33)^2))</f>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="AB35">
+        <f t="array" ref="AB35">SQRT(SUM((AB$2:AB$33-$I$2:$I$33)^2))</f>
+        <v>2</v>
+      </c>
+      <c r="AC35">
+        <f t="array" ref="AC35">SQRT(SUM((AC$2:AC$33-$I$2:$I$33)^2))</f>
+        <v>2</v>
+      </c>
+      <c r="AD35">
+        <f t="array" ref="AD35">SQRT(SUM((AD$2:AD$33-$I$2:$I$33)^2))</f>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="AE35">
+        <f t="array" ref="AE35">SQRT(SUM((AE$2:AE$33-$I$2:$I$33)^2))</f>
+        <v>1.7320508075688772</v>
+      </c>
+      <c r="AF35">
+        <f t="array" ref="AF35">SQRT(SUM((AF$2:AF$33-$I$2:$I$33)^2))</f>
+        <v>2</v>
+      </c>
+      <c r="AG35">
+        <f t="array" ref="AG35">SQRT(SUM((AG$2:AG$33-$I$2:$I$33)^2))</f>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="AH35">
+        <f t="array" ref="AH35">SQRT(SUM((AH$2:AH$33-$I$2:$I$33)^2))</f>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="AI35">
+        <f t="array" ref="AI35">SQRT(SUM((AI$2:AI$33-$I$2:$I$33)^2))</f>
+        <v>2.6457513110645907</v>
+      </c>
+      <c r="AJ35">
+        <f t="array" ref="AJ35">SQRT(SUM((AJ$2:AJ$33-$I$2:$I$33)^2))</f>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="AK35">
+        <f t="array" ref="AK35">SQRT(SUM((AK$2:AK$33-$I$2:$I$33)^2))</f>
+        <v>2.2360679774997898</v>
+      </c>
+      <c r="AL35">
+        <f t="array" ref="AL35">SQRT(SUM((AL$2:AL$33-$I$2:$I$33)^2))</f>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="AM35">
+        <f t="array" ref="AM35">SQRT(SUM((AM$2:AM$33-$I$2:$I$33)^2))</f>
+        <v>2</v>
+      </c>
+      <c r="AN35">
+        <f t="array" ref="AN35">SQRT(SUM((AN$2:AN$33-$I$2:$I$33)^2))</f>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="AO35">
+        <f t="array" ref="AO35">SQRT(SUM((AO$2:AO$33-$I$2:$I$33)^2))</f>
+        <v>1.7320508075688772</v>
+      </c>
+      <c r="AP35">
+        <f t="array" ref="AP35">SQRT(SUM((AP$2:AP$33-$I$2:$I$33)^2))</f>
+        <v>1</v>
+      </c>
+      <c r="AQ35">
+        <f t="array" ref="AQ35">SQRT(SUM((AQ$2:AQ$33-$I$2:$I$33)^2))</f>
+        <v>2</v>
+      </c>
+      <c r="AR35">
+        <f t="array" ref="AR35">SQRT(SUM((AR$2:AR$33-$I$2:$I$33)^2))</f>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="AS35">
+        <f t="array" ref="AS35">SQRT(SUM((AS$2:AS$33-$I$2:$I$33)^2))</f>
+        <v>2.4494897427831779</v>
+      </c>
+      <c r="AT35">
+        <f t="array" ref="AT35">SQRT(SUM((AT$2:AT$33-$I$2:$I$33)^2))</f>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="AU35">
+        <f t="array" ref="AU35">SQRT(SUM((AU$2:AU$33-$I$2:$I$33)^2))</f>
+        <v>2</v>
+      </c>
+      <c r="AV35">
+        <f t="array" ref="AV35">SQRT(SUM((AV$2:AV$33-$I$2:$I$33)^2))</f>
+        <v>1.7320508075688772</v>
+      </c>
+      <c r="AW35">
+        <f t="array" ref="AW35">SQRT(SUM((AW$2:AW$33-$I$2:$I$33)^2))</f>
+        <v>2.2360679774997898</v>
+      </c>
+      <c r="AX35">
+        <f t="array" ref="AX35">SQRT(SUM((AX$2:AX$33-$I$2:$I$33)^2))</f>
+        <v>2.2360679774997898</v>
+      </c>
+      <c r="AY35">
+        <f t="array" ref="AY35">SQRT(SUM((AY$2:AY$33-$I$2:$I$33)^2))</f>
+        <v>2.2360679774997898</v>
+      </c>
+      <c r="AZ35">
+        <f t="array" ref="AZ35">SQRT(SUM((AZ$2:AZ$33-$I$2:$I$33)^2))</f>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="BA35">
+        <f t="array" ref="BA35">SQRT(SUM((BA$2:BA$33-$I$2:$I$33)^2))</f>
+        <v>1.7320508075688772</v>
+      </c>
+      <c r="BB35">
+        <f t="array" ref="BB35">SQRT(SUM((BB$2:BB$33-$I$2:$I$33)^2))</f>
+        <v>1</v>
+      </c>
+      <c r="BC35">
+        <f t="array" ref="BC35">SQRT(SUM((BC$2:BC$33-$I$2:$I$33)^2))</f>
+        <v>2</v>
+      </c>
+      <c r="BD35">
+        <f t="array" ref="BD35">SQRT(SUM((BD$2:BD$33-$I$2:$I$33)^2))</f>
+        <v>2</v>
+      </c>
+      <c r="BE35">
+        <f t="array" ref="BE35">SQRT(SUM((BE$2:BE$33-$I$2:$I$33)^2))</f>
+        <v>2.2360679774997898</v>
+      </c>
+      <c r="BF35">
+        <f t="array" ref="BF35">SQRT(SUM((BF$2:BF$33-$I$2:$I$33)^2))</f>
+        <v>1.7320508075688772</v>
+      </c>
+      <c r="BG35">
+        <f t="array" ref="BG35">SQRT(SUM((BG$2:BG$33-$I$2:$I$33)^2))</f>
+        <v>1.7320508075688772</v>
+      </c>
+      <c r="BH35">
+        <f t="array" ref="BH35">SQRT(SUM((BH$2:BH$33-$I$2:$I$33)^2))</f>
+        <v>2.2360679774997898</v>
+      </c>
+      <c r="BI35">
+        <f t="array" ref="BI35">SQRT(SUM((BI$2:BI$33-$I$2:$I$33)^2))</f>
+        <v>1.7320508075688772</v>
+      </c>
+      <c r="BJ35">
+        <f t="array" ref="BJ35">SQRT(SUM((BJ$2:BJ$33-$I$2:$I$33)^2))</f>
+        <v>1.7320508075688772</v>
+      </c>
+      <c r="BK35">
+        <f t="array" ref="BK35">SQRT(SUM((BK$2:BK$33-$I$2:$I$33)^2))</f>
+        <v>2.6457513110645907</v>
+      </c>
+      <c r="BL35">
+        <f t="array" ref="BL35">SQRT(SUM((BL$2:BL$33-$I$2:$I$33)^2))</f>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="BM35">
+        <f t="array" ref="BM35">SQRT(SUM((BM$2:BM$33-$I$2:$I$33)^2))</f>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="BN35">
+        <f t="array" ref="BN35">SQRT(SUM((BN$2:BN$33-$I$2:$I$33)^2))</f>
+        <v>2.4494897427831779</v>
+      </c>
+      <c r="BO35">
+        <f t="array" ref="BO35">SQRT(SUM((BO$2:BO$33-$I$2:$I$33)^2))</f>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="BP35">
+        <f t="array" ref="BP35">SQRT(SUM((BP$2:BP$33-$I$2:$I$33)^2))</f>
+        <v>1.7320508075688772</v>
+      </c>
+      <c r="BQ35">
+        <f t="array" ref="BQ35">SQRT(SUM((BQ$2:BQ$33-$I$2:$I$33)^2))</f>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="BR35">
+        <f t="array" ref="BR35">SQRT(SUM((BR$2:BR$33-$I$2:$I$33)^2))</f>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="BS35">
+        <f t="array" ref="BS35">SQRT(SUM((BS$2:BS$33-$I$2:$I$33)^2))</f>
+        <v>2</v>
+      </c>
+      <c r="BT35">
+        <f t="array" ref="BT35">SQRT(SUM((BT$2:BT$33-$I$2:$I$33)^2))</f>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="BU35">
+        <f t="array" ref="BU35">SQRT(SUM((BU$2:BU$33-$I$2:$I$33)^2))</f>
+        <v>1</v>
+      </c>
+      <c r="BV35">
+        <f t="array" ref="BV35">SQRT(SUM((BV$2:BV$33-$I$2:$I$33)^2))</f>
+        <v>2.2360679774997898</v>
+      </c>
+      <c r="BW35">
+        <f t="array" ref="BW35">SQRT(SUM((BW$2:BW$33-$I$2:$I$33)^2))</f>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="BX35">
+        <f t="array" ref="BX35">SQRT(SUM((BX$2:BX$33-$I$2:$I$33)^2))</f>
+        <v>2</v>
+      </c>
+      <c r="BY35">
+        <f t="array" ref="BY35">SQRT(SUM((BY$2:BY$33-$I$2:$I$33)^2))</f>
+        <v>2.4494897427831779</v>
+      </c>
+      <c r="BZ35">
+        <f t="array" ref="BZ35">SQRT(SUM((BZ$2:BZ$33-$I$2:$I$33)^2))</f>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="CA35">
+        <f t="array" ref="CA35">SQRT(SUM((CA$2:CA$33-$I$2:$I$33)^2))</f>
+        <v>1</v>
+      </c>
+      <c r="CB35">
+        <f t="array" ref="CB35">SQRT(SUM((CB$2:CB$33-$I$2:$I$33)^2))</f>
+        <v>2</v>
+      </c>
+      <c r="CC35">
+        <f t="array" ref="CC35">SQRT(SUM((CC$2:CC$33-$I$2:$I$33)^2))</f>
+        <v>1</v>
+      </c>
+      <c r="CD35">
+        <f t="array" ref="CD35">SQRT(SUM((CD$2:CD$33-$I$2:$I$33)^2))</f>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="CE35">
+        <f t="array" ref="CE35">SQRT(SUM((CE$2:CE$33-$I$2:$I$33)^2))</f>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="CF35">
+        <f t="array" ref="CF35">SQRT(SUM((CF$2:CF$33-$I$2:$I$33)^2))</f>
+        <v>1.7320508075688772</v>
+      </c>
+      <c r="CG35">
+        <f t="array" ref="CG35">SQRT(SUM((CG$2:CG$33-$I$2:$I$33)^2))</f>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="CH35">
+        <f t="array" ref="CH35">SQRT(SUM((CH$2:CH$33-$I$2:$I$33)^2))</f>
+        <v>1</v>
+      </c>
+      <c r="CI35">
+        <f t="array" ref="CI35">SQRT(SUM((CI$2:CI$33-$I$2:$I$33)^2))</f>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="CJ35">
+        <f t="array" ref="CJ35">SQRT(SUM((CJ$2:CJ$33-$I$2:$I$33)^2))</f>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="CK35">
+        <f t="array" ref="CK35">SQRT(SUM((CK$2:CK$33-$I$2:$I$33)^2))</f>
+        <v>2.4494897427831779</v>
+      </c>
+      <c r="CL35">
+        <f t="array" ref="CL35">SQRT(SUM((CL$2:CL$33-$I$2:$I$33)^2))</f>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="CM35">
+        <f t="array" ref="CM35">SQRT(SUM((CM$2:CM$33-$I$2:$I$33)^2))</f>
+        <v>1</v>
+      </c>
+      <c r="CN35">
+        <f t="array" ref="CN35">SQRT(SUM((CN$2:CN$33-$I$2:$I$33)^2))</f>
+        <v>2.6457513110645907</v>
+      </c>
+      <c r="CO35">
+        <f t="array" ref="CO35">SQRT(SUM((CO$2:CO$33-$I$2:$I$33)^2))</f>
+        <v>3</v>
+      </c>
+      <c r="CP35">
+        <f t="array" ref="CP35">SQRT(SUM((CP$2:CP$33-$I$2:$I$33)^2))</f>
+        <v>1.7320508075688772</v>
+      </c>
+      <c r="CQ35">
+        <f t="array" ref="CQ35">SQRT(SUM((CQ$2:CQ$33-$I$2:$I$33)^2))</f>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="CR35">
+        <f t="array" ref="CR35">SQRT(SUM((CR$2:CR$33-$I$2:$I$33)^2))</f>
+        <v>1.7320508075688772</v>
+      </c>
+      <c r="CS35">
+        <f t="array" ref="CS35">SQRT(SUM((CS$2:CS$33-$I$2:$I$33)^2))</f>
+        <v>1.7320508075688772</v>
+      </c>
+      <c r="CT35">
+        <f t="array" ref="CT35">SQRT(SUM((CT$2:CT$33-$I$2:$I$33)^2))</f>
+        <v>2</v>
+      </c>
+      <c r="CU35">
+        <f t="array" ref="CU35">SQRT(SUM((CU$2:CU$33-$I$2:$I$33)^2))</f>
+        <v>2.4494897427831779</v>
+      </c>
+      <c r="CV35">
+        <f t="array" ref="CV35">SQRT(SUM((CV$2:CV$33-$I$2:$I$33)^2))</f>
+        <v>2</v>
+      </c>
+      <c r="CW35">
+        <f t="array" ref="CW35">SQRT(SUM((CW$2:CW$33-$I$2:$I$33)^2))</f>
+        <v>1</v>
+      </c>
+      <c r="CX35">
+        <f t="array" ref="CX35">SQRT(SUM((CX$2:CX$33-$I$2:$I$33)^2))</f>
+        <v>2</v>
+      </c>
+      <c r="CY35">
+        <f t="array" ref="CY35">SQRT(SUM((CY$2:CY$33-$I$2:$I$33)^2))</f>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="CZ35">
+        <f t="array" ref="CZ35">SQRT(SUM((CZ$2:CZ$33-$I$2:$I$33)^2))</f>
+        <v>1</v>
+      </c>
+      <c r="DA35">
+        <f t="array" ref="DA35">SQRT(SUM((DA$2:DA$33-$I$2:$I$33)^2))</f>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="DB35">
+        <f t="array" ref="DB35">SQRT(SUM((DB$2:DB$33-$I$2:$I$33)^2))</f>
+        <v>2</v>
+      </c>
+      <c r="DC35">
+        <f t="array" ref="DC35">SQRT(SUM((DC$2:DC$33-$I$2:$I$33)^2))</f>
+        <v>1.7320508075688772</v>
+      </c>
+      <c r="DD35">
+        <f t="array" ref="DD35">SQRT(SUM((DD$2:DD$33-$I$2:$I$33)^2))</f>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="DE35">
+        <f t="array" ref="DE35">SQRT(SUM((DE$2:DE$33-$I$2:$I$33)^2))</f>
+        <v>2</v>
+      </c>
+      <c r="DF35">
+        <f t="array" ref="DF35">SQRT(SUM((DF$2:DF$33-$I$2:$I$33)^2))</f>
+        <v>2</v>
+      </c>
+      <c r="DG35">
+        <f t="array" ref="DG35">SQRT(SUM((DG$2:DG$33-$I$2:$I$33)^2))</f>
+        <v>2.4494897427831779</v>
+      </c>
+    </row>
+    <row r="36" spans="1:113" x14ac:dyDescent="0.2">
+      <c r="G36" t="s">
+        <v>151</v>
+      </c>
+      <c r="L36">
+        <f t="array" ref="L36">SQRT(SUM((L$2:L$33-$J$2:$J$33)^2))</f>
+        <v>1.7320508075688772</v>
+      </c>
+      <c r="M36">
+        <f t="array" ref="M36">SQRT(SUM((M$2:M$33-$J$2:$J$33)^2))</f>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="N36">
+        <f t="array" ref="N36">SQRT(SUM((N$2:N$33-$J$2:$J$33)^2))</f>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="O36">
+        <f t="array" ref="O36">SQRT(SUM((O$2:O$33-$J$2:$J$33)^2))</f>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="P36">
+        <f t="array" ref="P36">SQRT(SUM((P$2:P$33-$J$2:$J$33)^2))</f>
+        <v>2</v>
+      </c>
+      <c r="Q36">
+        <f t="array" ref="Q36">SQRT(SUM((Q$2:Q$33-$J$2:$J$33)^2))</f>
+        <v>2</v>
+      </c>
+      <c r="R36">
+        <f t="array" ref="R36">SQRT(SUM((R$2:R$33-$J$2:$J$33)^2))</f>
+        <v>2</v>
+      </c>
+      <c r="S36">
+        <f t="array" ref="S36">SQRT(SUM((S$2:S$33-$J$2:$J$33)^2))</f>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="T36">
+        <f t="array" ref="T36">SQRT(SUM((T$2:T$33-$J$2:$J$33)^2))</f>
+        <v>2</v>
+      </c>
+      <c r="U36">
+        <f t="array" ref="U36">SQRT(SUM((U$2:U$33-$J$2:$J$33)^2))</f>
+        <v>1.7320508075688772</v>
+      </c>
+      <c r="V36">
+        <f t="array" ref="V36">SQRT(SUM((V$2:V$33-$J$2:$J$33)^2))</f>
+        <v>2.2360679774997898</v>
+      </c>
+      <c r="W36">
+        <f t="array" ref="W36">SQRT(SUM((W$2:W$33-$J$2:$J$33)^2))</f>
+        <v>1.7320508075688772</v>
+      </c>
+      <c r="X36">
+        <f t="array" ref="X36">SQRT(SUM((X$2:X$33-$J$2:$J$33)^2))</f>
+        <v>2</v>
+      </c>
+      <c r="Y36">
+        <f t="array" ref="Y36">SQRT(SUM((Y$2:Y$33-$J$2:$J$33)^2))</f>
+        <v>2</v>
+      </c>
+      <c r="Z36">
+        <f t="array" ref="Z36">SQRT(SUM((Z$2:Z$33-$J$2:$J$33)^2))</f>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="AA36">
+        <f t="array" ref="AA36">SQRT(SUM((AA$2:AA$33-$J$2:$J$33)^2))</f>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="AB36">
+        <f t="array" ref="AB36">SQRT(SUM((AB$2:AB$33-$J$2:$J$33)^2))</f>
+        <v>2</v>
+      </c>
+      <c r="AC36">
+        <f t="array" ref="AC36">SQRT(SUM((AC$2:AC$33-$J$2:$J$33)^2))</f>
+        <v>2</v>
+      </c>
+      <c r="AD36">
+        <f t="array" ref="AD36">SQRT(SUM((AD$2:AD$33-$J$2:$J$33)^2))</f>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="AE36">
+        <f t="array" ref="AE36">SQRT(SUM((AE$2:AE$33-$J$2:$J$33)^2))</f>
+        <v>1.7320508075688772</v>
+      </c>
+      <c r="AF36">
+        <f t="array" ref="AF36">SQRT(SUM((AF$2:AF$33-$J$2:$J$33)^2))</f>
+        <v>2</v>
+      </c>
+      <c r="AG36">
+        <f t="array" ref="AG36">SQRT(SUM((AG$2:AG$33-$J$2:$J$33)^2))</f>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="AH36">
+        <f t="array" ref="AH36">SQRT(SUM((AH$2:AH$33-$J$2:$J$33)^2))</f>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="AI36">
+        <f t="array" ref="AI36">SQRT(SUM((AI$2:AI$33-$J$2:$J$33)^2))</f>
+        <v>2.6457513110645907</v>
+      </c>
+      <c r="AJ36">
+        <f t="array" ref="AJ36">SQRT(SUM((AJ$2:AJ$33-$J$2:$J$33)^2))</f>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="AK36">
+        <f t="array" ref="AK36">SQRT(SUM((AK$2:AK$33-$J$2:$J$33)^2))</f>
+        <v>2.2360679774997898</v>
+      </c>
+      <c r="AL36">
+        <f t="array" ref="AL36">SQRT(SUM((AL$2:AL$33-$J$2:$J$33)^2))</f>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="AM36">
+        <f t="array" ref="AM36">SQRT(SUM((AM$2:AM$33-$J$2:$J$33)^2))</f>
+        <v>2</v>
+      </c>
+      <c r="AN36">
+        <f t="array" ref="AN36">SQRT(SUM((AN$2:AN$33-$J$2:$J$33)^2))</f>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="AO36">
+        <f t="array" ref="AO36">SQRT(SUM((AO$2:AO$33-$J$2:$J$33)^2))</f>
+        <v>1.7320508075688772</v>
+      </c>
+      <c r="AP36">
+        <f t="array" ref="AP36">SQRT(SUM((AP$2:AP$33-$J$2:$J$33)^2))</f>
+        <v>1</v>
+      </c>
+      <c r="AQ36">
+        <f t="array" ref="AQ36">SQRT(SUM((AQ$2:AQ$33-$J$2:$J$33)^2))</f>
+        <v>2</v>
+      </c>
+      <c r="AR36">
+        <f t="array" ref="AR36">SQRT(SUM((AR$2:AR$33-$J$2:$J$33)^2))</f>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="AS36">
+        <f t="array" ref="AS36">SQRT(SUM((AS$2:AS$33-$J$2:$J$33)^2))</f>
+        <v>2.4494897427831779</v>
+      </c>
+      <c r="AT36">
+        <f t="array" ref="AT36">SQRT(SUM((AT$2:AT$33-$J$2:$J$33)^2))</f>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="AU36">
+        <f t="array" ref="AU36">SQRT(SUM((AU$2:AU$33-$J$2:$J$33)^2))</f>
+        <v>2</v>
+      </c>
+      <c r="AV36">
+        <f t="array" ref="AV36">SQRT(SUM((AV$2:AV$33-$J$2:$J$33)^2))</f>
+        <v>1.7320508075688772</v>
+      </c>
+      <c r="AW36">
+        <f t="array" ref="AW36">SQRT(SUM((AW$2:AW$33-$J$2:$J$33)^2))</f>
+        <v>2.2360679774997898</v>
+      </c>
+      <c r="AX36">
+        <f t="array" ref="AX36">SQRT(SUM((AX$2:AX$33-$J$2:$J$33)^2))</f>
+        <v>2.2360679774997898</v>
+      </c>
+      <c r="AY36">
+        <f t="array" ref="AY36">SQRT(SUM((AY$2:AY$33-$J$2:$J$33)^2))</f>
+        <v>2.2360679774997898</v>
+      </c>
+      <c r="AZ36">
+        <f t="array" ref="AZ36">SQRT(SUM((AZ$2:AZ$33-$J$2:$J$33)^2))</f>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="BA36">
+        <f t="array" ref="BA36">SQRT(SUM((BA$2:BA$33-$J$2:$J$33)^2))</f>
+        <v>1.7320508075688772</v>
+      </c>
+      <c r="BB36">
+        <f t="array" ref="BB36">SQRT(SUM((BB$2:BB$33-$J$2:$J$33)^2))</f>
+        <v>1</v>
+      </c>
+      <c r="BC36">
+        <f t="array" ref="BC36">SQRT(SUM((BC$2:BC$33-$J$2:$J$33)^2))</f>
+        <v>2</v>
+      </c>
+      <c r="BD36">
+        <f t="array" ref="BD36">SQRT(SUM((BD$2:BD$33-$J$2:$J$33)^2))</f>
+        <v>2</v>
+      </c>
+      <c r="BE36">
+        <f t="array" ref="BE36">SQRT(SUM((BE$2:BE$33-$J$2:$J$33)^2))</f>
+        <v>2.2360679774997898</v>
+      </c>
+      <c r="BF36">
+        <f t="array" ref="BF36">SQRT(SUM((BF$2:BF$33-$J$2:$J$33)^2))</f>
+        <v>1.7320508075688772</v>
+      </c>
+      <c r="BG36">
+        <f t="array" ref="BG36">SQRT(SUM((BG$2:BG$33-$J$2:$J$33)^2))</f>
+        <v>1.7320508075688772</v>
+      </c>
+      <c r="BH36">
+        <f t="array" ref="BH36">SQRT(SUM((BH$2:BH$33-$J$2:$J$33)^2))</f>
+        <v>2.2360679774997898</v>
+      </c>
+      <c r="BI36">
+        <f t="array" ref="BI36">SQRT(SUM((BI$2:BI$33-$J$2:$J$33)^2))</f>
+        <v>1.7320508075688772</v>
+      </c>
+      <c r="BJ36">
+        <f t="array" ref="BJ36">SQRT(SUM((BJ$2:BJ$33-$J$2:$J$33)^2))</f>
+        <v>1.7320508075688772</v>
+      </c>
+      <c r="BK36">
+        <f t="array" ref="BK36">SQRT(SUM((BK$2:BK$33-$J$2:$J$33)^2))</f>
+        <v>2.6457513110645907</v>
+      </c>
+      <c r="BL36">
+        <f t="array" ref="BL36">SQRT(SUM((BL$2:BL$33-$J$2:$J$33)^2))</f>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="BM36">
+        <f t="array" ref="BM36">SQRT(SUM((BM$2:BM$33-$J$2:$J$33)^2))</f>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="BN36">
+        <f t="array" ref="BN36">SQRT(SUM((BN$2:BN$33-$J$2:$J$33)^2))</f>
+        <v>2.4494897427831779</v>
+      </c>
+      <c r="BO36">
+        <f t="array" ref="BO36">SQRT(SUM((BO$2:BO$33-$J$2:$J$33)^2))</f>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="BP36">
+        <f t="array" ref="BP36">SQRT(SUM((BP$2:BP$33-$J$2:$J$33)^2))</f>
+        <v>1.7320508075688772</v>
+      </c>
+      <c r="BQ36">
+        <f t="array" ref="BQ36">SQRT(SUM((BQ$2:BQ$33-$J$2:$J$33)^2))</f>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="BR36">
+        <f t="array" ref="BR36">SQRT(SUM((BR$2:BR$33-$J$2:$J$33)^2))</f>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="BS36">
+        <f t="array" ref="BS36">SQRT(SUM((BS$2:BS$33-$J$2:$J$33)^2))</f>
+        <v>2</v>
+      </c>
+      <c r="BT36">
+        <f t="array" ref="BT36">SQRT(SUM((BT$2:BT$33-$J$2:$J$33)^2))</f>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="BU36">
+        <f t="array" ref="BU36">SQRT(SUM((BU$2:BU$33-$J$2:$J$33)^2))</f>
+        <v>1</v>
+      </c>
+      <c r="BV36">
+        <f t="array" ref="BV36">SQRT(SUM((BV$2:BV$33-$J$2:$J$33)^2))</f>
+        <v>2.2360679774997898</v>
+      </c>
+      <c r="BW36">
+        <f t="array" ref="BW36">SQRT(SUM((BW$2:BW$33-$J$2:$J$33)^2))</f>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="BX36">
+        <f t="array" ref="BX36">SQRT(SUM((BX$2:BX$33-$J$2:$J$33)^2))</f>
+        <v>2</v>
+      </c>
+      <c r="BY36">
+        <f t="array" ref="BY36">SQRT(SUM((BY$2:BY$33-$J$2:$J$33)^2))</f>
+        <v>2.4494897427831779</v>
+      </c>
+      <c r="BZ36">
+        <f t="array" ref="BZ36">SQRT(SUM((BZ$2:BZ$33-$J$2:$J$33)^2))</f>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="CA36">
+        <f t="array" ref="CA36">SQRT(SUM((CA$2:CA$33-$J$2:$J$33)^2))</f>
+        <v>1</v>
+      </c>
+      <c r="CB36">
+        <f t="array" ref="CB36">SQRT(SUM((CB$2:CB$33-$J$2:$J$33)^2))</f>
+        <v>2</v>
+      </c>
+      <c r="CC36">
+        <f t="array" ref="CC36">SQRT(SUM((CC$2:CC$33-$J$2:$J$33)^2))</f>
+        <v>1</v>
+      </c>
+      <c r="CD36">
+        <f t="array" ref="CD36">SQRT(SUM((CD$2:CD$33-$J$2:$J$33)^2))</f>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="CE36">
+        <f t="array" ref="CE36">SQRT(SUM((CE$2:CE$33-$J$2:$J$33)^2))</f>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="CF36">
+        <f t="array" ref="CF36">SQRT(SUM((CF$2:CF$33-$J$2:$J$33)^2))</f>
+        <v>1.7320508075688772</v>
+      </c>
+      <c r="CG36">
+        <f t="array" ref="CG36">SQRT(SUM((CG$2:CG$33-$J$2:$J$33)^2))</f>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="CH36">
+        <f t="array" ref="CH36">SQRT(SUM((CH$2:CH$33-$J$2:$J$33)^2))</f>
+        <v>1</v>
+      </c>
+      <c r="CI36">
+        <f t="array" ref="CI36">SQRT(SUM((CI$2:CI$33-$J$2:$J$33)^2))</f>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="CJ36">
+        <f t="array" ref="CJ36">SQRT(SUM((CJ$2:CJ$33-$J$2:$J$33)^2))</f>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="CK36">
+        <f t="array" ref="CK36">SQRT(SUM((CK$2:CK$33-$J$2:$J$33)^2))</f>
+        <v>2.4494897427831779</v>
+      </c>
+      <c r="CL36">
+        <f t="array" ref="CL36">SQRT(SUM((CL$2:CL$33-$J$2:$J$33)^2))</f>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="CM36">
+        <f t="array" ref="CM36">SQRT(SUM((CM$2:CM$33-$J$2:$J$33)^2))</f>
+        <v>1</v>
+      </c>
+      <c r="CN36">
+        <f t="array" ref="CN36">SQRT(SUM((CN$2:CN$33-$J$2:$J$33)^2))</f>
+        <v>2.6457513110645907</v>
+      </c>
+      <c r="CO36">
+        <f t="array" ref="CO36">SQRT(SUM((CO$2:CO$33-$J$2:$J$33)^2))</f>
+        <v>3</v>
+      </c>
+      <c r="CP36">
+        <f t="array" ref="CP36">SQRT(SUM((CP$2:CP$33-$J$2:$J$33)^2))</f>
+        <v>1.7320508075688772</v>
+      </c>
+      <c r="CQ36">
+        <f t="array" ref="CQ36">SQRT(SUM((CQ$2:CQ$33-$J$2:$J$33)^2))</f>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="CR36">
+        <f t="array" ref="CR36">SQRT(SUM((CR$2:CR$33-$J$2:$J$33)^2))</f>
+        <v>1.7320508075688772</v>
+      </c>
+      <c r="CS36">
+        <f t="array" ref="CS36">SQRT(SUM((CS$2:CS$33-$J$2:$J$33)^2))</f>
+        <v>1.7320508075688772</v>
+      </c>
+      <c r="CT36">
+        <f t="array" ref="CT36">SQRT(SUM((CT$2:CT$33-$J$2:$J$33)^2))</f>
+        <v>2</v>
+      </c>
+      <c r="CU36">
+        <f t="array" ref="CU36">SQRT(SUM((CU$2:CU$33-$J$2:$J$33)^2))</f>
+        <v>2.4494897427831779</v>
+      </c>
+      <c r="CV36">
+        <f t="array" ref="CV36">SQRT(SUM((CV$2:CV$33-$J$2:$J$33)^2))</f>
+        <v>2</v>
+      </c>
+      <c r="CW36">
+        <f t="array" ref="CW36">SQRT(SUM((CW$2:CW$33-$J$2:$J$33)^2))</f>
+        <v>1</v>
+      </c>
+      <c r="CX36">
+        <f t="array" ref="CX36">SQRT(SUM((CX$2:CX$33-$J$2:$J$33)^2))</f>
+        <v>2</v>
+      </c>
+      <c r="CY36">
+        <f t="array" ref="CY36">SQRT(SUM((CY$2:CY$33-$J$2:$J$33)^2))</f>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="CZ36">
+        <f t="array" ref="CZ36">SQRT(SUM((CZ$2:CZ$33-$J$2:$J$33)^2))</f>
+        <v>1</v>
+      </c>
+      <c r="DA36">
+        <f t="array" ref="DA36">SQRT(SUM((DA$2:DA$33-$J$2:$J$33)^2))</f>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="DB36">
+        <f t="array" ref="DB36">SQRT(SUM((DB$2:DB$33-$J$2:$J$33)^2))</f>
+        <v>2</v>
+      </c>
+      <c r="DC36">
+        <f t="array" ref="DC36">SQRT(SUM((DC$2:DC$33-$J$2:$J$33)^2))</f>
+        <v>1.7320508075688772</v>
+      </c>
+      <c r="DD36">
+        <f t="array" ref="DD36">SQRT(SUM((DD$2:DD$33-$J$2:$J$33)^2))</f>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="DE36">
+        <f t="array" ref="DE36">SQRT(SUM((DE$2:DE$33-$J$2:$J$33)^2))</f>
+        <v>2</v>
+      </c>
       <c r="DF36">
-        <v>324</v>
+        <f t="array" ref="DF36">SQRT(SUM((DF$2:DF$33-$J$2:$J$33)^2))</f>
+        <v>2</v>
+      </c>
+      <c r="DG36">
+        <f t="array" ref="DG36">SQRT(SUM((DG$2:DG$33-$J$2:$J$33)^2))</f>
+        <v>2.4494897427831779</v>
+      </c>
+    </row>
+    <row r="37" spans="1:113" x14ac:dyDescent="0.2">
+      <c r="G37" t="s">
+        <v>152</v>
+      </c>
+      <c r="L37">
+        <f t="array" ref="L37">SQRT(SUM((L$2:L$33-$K$2:$K$33)^2))</f>
+        <v>1.7320508075688772</v>
+      </c>
+      <c r="M37">
+        <f t="array" ref="M37">SQRT(SUM((M$2:M$33-$K$2:$K$33)^2))</f>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="N37">
+        <f t="array" ref="N37">SQRT(SUM((N$2:N$33-$K$2:$K$33)^2))</f>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="O37">
+        <f t="array" ref="O37">SQRT(SUM((O$2:O$33-$K$2:$K$33)^2))</f>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="P37">
+        <f t="array" ref="P37">SQRT(SUM((P$2:P$33-$K$2:$K$33)^2))</f>
+        <v>2</v>
+      </c>
+      <c r="Q37">
+        <f t="array" ref="Q37">SQRT(SUM((Q$2:Q$33-$K$2:$K$33)^2))</f>
+        <v>2</v>
+      </c>
+      <c r="R37">
+        <f t="array" ref="R37">SQRT(SUM((R$2:R$33-$K$2:$K$33)^2))</f>
+        <v>2</v>
+      </c>
+      <c r="S37">
+        <f t="array" ref="S37">SQRT(SUM((S$2:S$33-$K$2:$K$33)^2))</f>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="T37">
+        <f t="array" ref="T37">SQRT(SUM((T$2:T$33-$K$2:$K$33)^2))</f>
+        <v>2</v>
+      </c>
+      <c r="U37">
+        <f t="array" ref="U37">SQRT(SUM((U$2:U$33-$K$2:$K$33)^2))</f>
+        <v>1.7320508075688772</v>
+      </c>
+      <c r="V37">
+        <f t="array" ref="V37">SQRT(SUM((V$2:V$33-$K$2:$K$33)^2))</f>
+        <v>2.2360679774997898</v>
+      </c>
+      <c r="W37">
+        <f t="array" ref="W37">SQRT(SUM((W$2:W$33-$K$2:$K$33)^2))</f>
+        <v>1.7320508075688772</v>
+      </c>
+      <c r="X37">
+        <f t="array" ref="X37">SQRT(SUM((X$2:X$33-$K$2:$K$33)^2))</f>
+        <v>2</v>
+      </c>
+      <c r="Y37">
+        <f t="array" ref="Y37">SQRT(SUM((Y$2:Y$33-$K$2:$K$33)^2))</f>
+        <v>2</v>
+      </c>
+      <c r="Z37">
+        <f t="array" ref="Z37">SQRT(SUM((Z$2:Z$33-$K$2:$K$33)^2))</f>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="AA37">
+        <f t="array" ref="AA37">SQRT(SUM((AA$2:AA$33-$K$2:$K$33)^2))</f>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="AB37">
+        <f t="array" ref="AB37">SQRT(SUM((AB$2:AB$33-$K$2:$K$33)^2))</f>
+        <v>2</v>
+      </c>
+      <c r="AC37">
+        <f t="array" ref="AC37">SQRT(SUM((AC$2:AC$33-$K$2:$K$33)^2))</f>
+        <v>2</v>
+      </c>
+      <c r="AD37">
+        <f t="array" ref="AD37">SQRT(SUM((AD$2:AD$33-$K$2:$K$33)^2))</f>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="AE37">
+        <f t="array" ref="AE37">SQRT(SUM((AE$2:AE$33-$K$2:$K$33)^2))</f>
+        <v>1.7320508075688772</v>
+      </c>
+      <c r="AF37">
+        <f t="array" ref="AF37">SQRT(SUM((AF$2:AF$33-$K$2:$K$33)^2))</f>
+        <v>2</v>
+      </c>
+      <c r="AG37">
+        <f t="array" ref="AG37">SQRT(SUM((AG$2:AG$33-$K$2:$K$33)^2))</f>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="AH37">
+        <f t="array" ref="AH37">SQRT(SUM((AH$2:AH$33-$K$2:$K$33)^2))</f>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="AI37">
+        <f t="array" ref="AI37">SQRT(SUM((AI$2:AI$33-$K$2:$K$33)^2))</f>
+        <v>2.6457513110645907</v>
+      </c>
+      <c r="AJ37">
+        <f t="array" ref="AJ37">SQRT(SUM((AJ$2:AJ$33-$K$2:$K$33)^2))</f>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="AK37">
+        <f t="array" ref="AK37">SQRT(SUM((AK$2:AK$33-$K$2:$K$33)^2))</f>
+        <v>2.2360679774997898</v>
+      </c>
+      <c r="AL37">
+        <f t="array" ref="AL37">SQRT(SUM((AL$2:AL$33-$K$2:$K$33)^2))</f>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="AM37">
+        <f t="array" ref="AM37">SQRT(SUM((AM$2:AM$33-$K$2:$K$33)^2))</f>
+        <v>2</v>
+      </c>
+      <c r="AN37">
+        <f t="array" ref="AN37">SQRT(SUM((AN$2:AN$33-$K$2:$K$33)^2))</f>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="AO37">
+        <f t="array" ref="AO37">SQRT(SUM((AO$2:AO$33-$K$2:$K$33)^2))</f>
+        <v>1.7320508075688772</v>
+      </c>
+      <c r="AP37">
+        <f t="array" ref="AP37">SQRT(SUM((AP$2:AP$33-$K$2:$K$33)^2))</f>
+        <v>1</v>
+      </c>
+      <c r="AQ37">
+        <f t="array" ref="AQ37">SQRT(SUM((AQ$2:AQ$33-$K$2:$K$33)^2))</f>
+        <v>2</v>
+      </c>
+      <c r="AR37">
+        <f t="array" ref="AR37">SQRT(SUM((AR$2:AR$33-$K$2:$K$33)^2))</f>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="AS37">
+        <f t="array" ref="AS37">SQRT(SUM((AS$2:AS$33-$K$2:$K$33)^2))</f>
+        <v>2.4494897427831779</v>
+      </c>
+      <c r="AT37">
+        <f t="array" ref="AT37">SQRT(SUM((AT$2:AT$33-$K$2:$K$33)^2))</f>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="AU37">
+        <f t="array" ref="AU37">SQRT(SUM((AU$2:AU$33-$K$2:$K$33)^2))</f>
+        <v>2</v>
+      </c>
+      <c r="AV37">
+        <f t="array" ref="AV37">SQRT(SUM((AV$2:AV$33-$K$2:$K$33)^2))</f>
+        <v>1.7320508075688772</v>
+      </c>
+      <c r="AW37">
+        <f t="array" ref="AW37">SQRT(SUM((AW$2:AW$33-$K$2:$K$33)^2))</f>
+        <v>2.2360679774997898</v>
+      </c>
+      <c r="AX37">
+        <f t="array" ref="AX37">SQRT(SUM((AX$2:AX$33-$K$2:$K$33)^2))</f>
+        <v>2.2360679774997898</v>
+      </c>
+      <c r="AY37">
+        <f t="array" ref="AY37">SQRT(SUM((AY$2:AY$33-$K$2:$K$33)^2))</f>
+        <v>2.2360679774997898</v>
+      </c>
+      <c r="AZ37">
+        <f t="array" ref="AZ37">SQRT(SUM((AZ$2:AZ$33-$K$2:$K$33)^2))</f>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="BA37">
+        <f t="array" ref="BA37">SQRT(SUM((BA$2:BA$33-$K$2:$K$33)^2))</f>
+        <v>1.7320508075688772</v>
+      </c>
+      <c r="BB37">
+        <f t="array" ref="BB37">SQRT(SUM((BB$2:BB$33-$K$2:$K$33)^2))</f>
+        <v>1</v>
+      </c>
+      <c r="BC37">
+        <f t="array" ref="BC37">SQRT(SUM((BC$2:BC$33-$K$2:$K$33)^2))</f>
+        <v>2</v>
+      </c>
+      <c r="BD37">
+        <f t="array" ref="BD37">SQRT(SUM((BD$2:BD$33-$K$2:$K$33)^2))</f>
+        <v>2</v>
+      </c>
+      <c r="BE37">
+        <f t="array" ref="BE37">SQRT(SUM((BE$2:BE$33-$K$2:$K$33)^2))</f>
+        <v>2.2360679774997898</v>
+      </c>
+      <c r="BF37">
+        <f t="array" ref="BF37">SQRT(SUM((BF$2:BF$33-$K$2:$K$33)^2))</f>
+        <v>1.7320508075688772</v>
+      </c>
+      <c r="BG37">
+        <f t="array" ref="BG37">SQRT(SUM((BG$2:BG$33-$K$2:$K$33)^2))</f>
+        <v>1.7320508075688772</v>
+      </c>
+      <c r="BH37">
+        <f t="array" ref="BH37">SQRT(SUM((BH$2:BH$33-$K$2:$K$33)^2))</f>
+        <v>2.2360679774997898</v>
+      </c>
+      <c r="BI37">
+        <f t="array" ref="BI37">SQRT(SUM((BI$2:BI$33-$K$2:$K$33)^2))</f>
+        <v>1.7320508075688772</v>
+      </c>
+      <c r="BJ37">
+        <f t="array" ref="BJ37">SQRT(SUM((BJ$2:BJ$33-$K$2:$K$33)^2))</f>
+        <v>1.7320508075688772</v>
+      </c>
+      <c r="BK37">
+        <f t="array" ref="BK37">SQRT(SUM((BK$2:BK$33-$K$2:$K$33)^2))</f>
+        <v>2.6457513110645907</v>
+      </c>
+      <c r="BL37">
+        <f t="array" ref="BL37">SQRT(SUM((BL$2:BL$33-$K$2:$K$33)^2))</f>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="BM37">
+        <f t="array" ref="BM37">SQRT(SUM((BM$2:BM$33-$K$2:$K$33)^2))</f>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="BN37">
+        <f t="array" ref="BN37">SQRT(SUM((BN$2:BN$33-$K$2:$K$33)^2))</f>
+        <v>2.4494897427831779</v>
+      </c>
+      <c r="BO37">
+        <f t="array" ref="BO37">SQRT(SUM((BO$2:BO$33-$K$2:$K$33)^2))</f>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="BP37">
+        <f t="array" ref="BP37">SQRT(SUM((BP$2:BP$33-$K$2:$K$33)^2))</f>
+        <v>1.7320508075688772</v>
+      </c>
+      <c r="BQ37">
+        <f t="array" ref="BQ37">SQRT(SUM((BQ$2:BQ$33-$K$2:$K$33)^2))</f>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="BR37">
+        <f t="array" ref="BR37">SQRT(SUM((BR$2:BR$33-$K$2:$K$33)^2))</f>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="BS37">
+        <f t="array" ref="BS37">SQRT(SUM((BS$2:BS$33-$K$2:$K$33)^2))</f>
+        <v>2</v>
+      </c>
+      <c r="BT37">
+        <f t="array" ref="BT37">SQRT(SUM((BT$2:BT$33-$K$2:$K$33)^2))</f>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="BU37">
+        <f t="array" ref="BU37">SQRT(SUM((BU$2:BU$33-$K$2:$K$33)^2))</f>
+        <v>1</v>
+      </c>
+      <c r="BV37">
+        <f t="array" ref="BV37">SQRT(SUM((BV$2:BV$33-$K$2:$K$33)^2))</f>
+        <v>2.2360679774997898</v>
+      </c>
+      <c r="BW37">
+        <f t="array" ref="BW37">SQRT(SUM((BW$2:BW$33-$K$2:$K$33)^2))</f>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="BX37">
+        <f t="array" ref="BX37">SQRT(SUM((BX$2:BX$33-$K$2:$K$33)^2))</f>
+        <v>2</v>
+      </c>
+      <c r="BY37">
+        <f t="array" ref="BY37">SQRT(SUM((BY$2:BY$33-$K$2:$K$33)^2))</f>
+        <v>2.4494897427831779</v>
+      </c>
+      <c r="BZ37">
+        <f t="array" ref="BZ37">SQRT(SUM((BZ$2:BZ$33-$K$2:$K$33)^2))</f>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="CA37">
+        <f t="array" ref="CA37">SQRT(SUM((CA$2:CA$33-$K$2:$K$33)^2))</f>
+        <v>1</v>
+      </c>
+      <c r="CB37">
+        <f t="array" ref="CB37">SQRT(SUM((CB$2:CB$33-$K$2:$K$33)^2))</f>
+        <v>2</v>
+      </c>
+      <c r="CC37">
+        <f t="array" ref="CC37">SQRT(SUM((CC$2:CC$33-$K$2:$K$33)^2))</f>
+        <v>1</v>
+      </c>
+      <c r="CD37">
+        <f t="array" ref="CD37">SQRT(SUM((CD$2:CD$33-$K$2:$K$33)^2))</f>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="CE37">
+        <f t="array" ref="CE37">SQRT(SUM((CE$2:CE$33-$K$2:$K$33)^2))</f>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="CF37">
+        <f t="array" ref="CF37">SQRT(SUM((CF$2:CF$33-$K$2:$K$33)^2))</f>
+        <v>1.7320508075688772</v>
+      </c>
+      <c r="CG37">
+        <f t="array" ref="CG37">SQRT(SUM((CG$2:CG$33-$K$2:$K$33)^2))</f>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="CH37">
+        <f t="array" ref="CH37">SQRT(SUM((CH$2:CH$33-$K$2:$K$33)^2))</f>
+        <v>1</v>
+      </c>
+      <c r="CI37">
+        <f t="array" ref="CI37">SQRT(SUM((CI$2:CI$33-$K$2:$K$33)^2))</f>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="CJ37">
+        <f t="array" ref="CJ37">SQRT(SUM((CJ$2:CJ$33-$K$2:$K$33)^2))</f>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="CK37">
+        <f t="array" ref="CK37">SQRT(SUM((CK$2:CK$33-$K$2:$K$33)^2))</f>
+        <v>2.4494897427831779</v>
+      </c>
+      <c r="CL37">
+        <f t="array" ref="CL37">SQRT(SUM((CL$2:CL$33-$K$2:$K$33)^2))</f>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="CM37">
+        <f t="array" ref="CM37">SQRT(SUM((CM$2:CM$33-$K$2:$K$33)^2))</f>
+        <v>1</v>
+      </c>
+      <c r="CN37">
+        <f t="array" ref="CN37">SQRT(SUM((CN$2:CN$33-$K$2:$K$33)^2))</f>
+        <v>2.6457513110645907</v>
+      </c>
+      <c r="CO37">
+        <f t="array" ref="CO37">SQRT(SUM((CO$2:CO$33-$K$2:$K$33)^2))</f>
+        <v>3</v>
+      </c>
+      <c r="CP37">
+        <f t="array" ref="CP37">SQRT(SUM((CP$2:CP$33-$K$2:$K$33)^2))</f>
+        <v>1.7320508075688772</v>
+      </c>
+      <c r="CQ37">
+        <f t="array" ref="CQ37">SQRT(SUM((CQ$2:CQ$33-$K$2:$K$33)^2))</f>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="CR37">
+        <f t="array" ref="CR37">SQRT(SUM((CR$2:CR$33-$K$2:$K$33)^2))</f>
+        <v>1.7320508075688772</v>
+      </c>
+      <c r="CS37">
+        <f t="array" ref="CS37">SQRT(SUM((CS$2:CS$33-$K$2:$K$33)^2))</f>
+        <v>1.7320508075688772</v>
+      </c>
+      <c r="CT37">
+        <f t="array" ref="CT37">SQRT(SUM((CT$2:CT$33-$K$2:$K$33)^2))</f>
+        <v>2</v>
+      </c>
+      <c r="CU37">
+        <f t="array" ref="CU37">SQRT(SUM((CU$2:CU$33-$K$2:$K$33)^2))</f>
+        <v>2.4494897427831779</v>
+      </c>
+      <c r="CV37">
+        <f t="array" ref="CV37">SQRT(SUM((CV$2:CV$33-$K$2:$K$33)^2))</f>
+        <v>2</v>
+      </c>
+      <c r="CW37">
+        <f t="array" ref="CW37">SQRT(SUM((CW$2:CW$33-$K$2:$K$33)^2))</f>
+        <v>1</v>
+      </c>
+      <c r="CX37">
+        <f t="array" ref="CX37">SQRT(SUM((CX$2:CX$33-$K$2:$K$33)^2))</f>
+        <v>2</v>
+      </c>
+      <c r="CY37">
+        <f t="array" ref="CY37">SQRT(SUM((CY$2:CY$33-$K$2:$K$33)^2))</f>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="CZ37">
+        <f t="array" ref="CZ37">SQRT(SUM((CZ$2:CZ$33-$K$2:$K$33)^2))</f>
+        <v>1</v>
+      </c>
+      <c r="DA37">
+        <f t="array" ref="DA37">SQRT(SUM((DA$2:DA$33-$K$2:$K$33)^2))</f>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="DB37">
+        <f t="array" ref="DB37">SQRT(SUM((DB$2:DB$33-$K$2:$K$33)^2))</f>
+        <v>2</v>
+      </c>
+      <c r="DC37">
+        <f t="array" ref="DC37">SQRT(SUM((DC$2:DC$33-$K$2:$K$33)^2))</f>
+        <v>1.7320508075688772</v>
+      </c>
+      <c r="DD37">
+        <f t="array" ref="DD37">SQRT(SUM((DD$2:DD$33-$K$2:$K$33)^2))</f>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="DE37">
+        <f t="array" ref="DE37">SQRT(SUM((DE$2:DE$33-$K$2:$K$33)^2))</f>
+        <v>2</v>
+      </c>
+      <c r="DF37">
+        <f t="array" ref="DF37">SQRT(SUM((DF$2:DF$33-$K$2:$K$33)^2))</f>
+        <v>2</v>
+      </c>
+      <c r="DG37">
+        <f t="array" ref="DG37">SQRT(SUM((DG$2:DG$33-$K$2:$K$33)^2))</f>
+        <v>2.4494897427831779</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Find the minimum distance and assigned cluster
</commit_message>
<xml_diff>
--- a/chapter-02/exercise-02.xlsx
+++ b/chapter-02/exercise-02.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1050" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1052" uniqueCount="155">
   <si>
     <t>Campaign</t>
   </si>
@@ -493,6 +493,12 @@
   </si>
   <si>
     <t>Distance to Cluster 4</t>
+  </si>
+  <si>
+    <t>Minimum Distance</t>
+  </si>
+  <si>
+    <t>Assigned Cluster</t>
   </si>
 </sst>
 </file>
@@ -13394,10 +13400,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:DI37"/>
+  <dimension ref="A1:DI39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="A37" sqref="A37"/>
+    <sheetView tabSelected="1" topLeftCell="DC5" workbookViewId="0">
+      <selection activeCell="L39" sqref="L39:DG39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -17167,6 +17173,816 @@
         <v>2.4494897427831779</v>
       </c>
     </row>
+    <row r="38" spans="1:113" x14ac:dyDescent="0.2">
+      <c r="G38" t="s">
+        <v>153</v>
+      </c>
+      <c r="L38">
+        <f>MIN(L34:L37)</f>
+        <v>1.7320508075688772</v>
+      </c>
+      <c r="M38">
+        <f t="shared" ref="M38:BX38" si="0">MIN(M34:M37)</f>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="N38">
+        <f t="shared" si="0"/>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="O38">
+        <f t="shared" si="0"/>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="P38">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="Q38">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="R38">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="S38">
+        <f t="shared" si="0"/>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="T38">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="U38">
+        <f t="shared" si="0"/>
+        <v>1.7320508075688772</v>
+      </c>
+      <c r="V38">
+        <f t="shared" si="0"/>
+        <v>2.2360679774997898</v>
+      </c>
+      <c r="W38">
+        <f t="shared" si="0"/>
+        <v>1.7320508075688772</v>
+      </c>
+      <c r="X38">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="Y38">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="Z38">
+        <f t="shared" si="0"/>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="AA38">
+        <f t="shared" si="0"/>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="AB38">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="AC38">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="AD38">
+        <f t="shared" si="0"/>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="AE38">
+        <f t="shared" si="0"/>
+        <v>1.7320508075688772</v>
+      </c>
+      <c r="AF38">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="AG38">
+        <f t="shared" si="0"/>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="AH38">
+        <f t="shared" si="0"/>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="AI38">
+        <f t="shared" si="0"/>
+        <v>2.6457513110645907</v>
+      </c>
+      <c r="AJ38">
+        <f t="shared" si="0"/>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="AK38">
+        <f t="shared" si="0"/>
+        <v>2.2360679774997898</v>
+      </c>
+      <c r="AL38">
+        <f t="shared" si="0"/>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="AM38">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="AN38">
+        <f t="shared" si="0"/>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="AO38">
+        <f t="shared" si="0"/>
+        <v>1.7320508075688772</v>
+      </c>
+      <c r="AP38">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="AQ38">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="AR38">
+        <f t="shared" si="0"/>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="AS38">
+        <f t="shared" si="0"/>
+        <v>2.4494897427831779</v>
+      </c>
+      <c r="AT38">
+        <f t="shared" si="0"/>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="AU38">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="AV38">
+        <f t="shared" si="0"/>
+        <v>1.7320508075688772</v>
+      </c>
+      <c r="AW38">
+        <f t="shared" si="0"/>
+        <v>2.2360679774997898</v>
+      </c>
+      <c r="AX38">
+        <f t="shared" si="0"/>
+        <v>2.2360679774997898</v>
+      </c>
+      <c r="AY38">
+        <f t="shared" si="0"/>
+        <v>2.2360679774997898</v>
+      </c>
+      <c r="AZ38">
+        <f t="shared" si="0"/>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="BA38">
+        <f t="shared" si="0"/>
+        <v>1.7320508075688772</v>
+      </c>
+      <c r="BB38">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="BC38">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="BD38">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="BE38">
+        <f t="shared" si="0"/>
+        <v>2.2360679774997898</v>
+      </c>
+      <c r="BF38">
+        <f t="shared" si="0"/>
+        <v>1.7320508075688772</v>
+      </c>
+      <c r="BG38">
+        <f t="shared" si="0"/>
+        <v>1.7320508075688772</v>
+      </c>
+      <c r="BH38">
+        <f t="shared" si="0"/>
+        <v>2.2360679774997898</v>
+      </c>
+      <c r="BI38">
+        <f t="shared" si="0"/>
+        <v>1.7320508075688772</v>
+      </c>
+      <c r="BJ38">
+        <f t="shared" si="0"/>
+        <v>1.7320508075688772</v>
+      </c>
+      <c r="BK38">
+        <f t="shared" si="0"/>
+        <v>2.6457513110645907</v>
+      </c>
+      <c r="BL38">
+        <f t="shared" si="0"/>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="BM38">
+        <f t="shared" si="0"/>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="BN38">
+        <f t="shared" si="0"/>
+        <v>2.4494897427831779</v>
+      </c>
+      <c r="BO38">
+        <f t="shared" si="0"/>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="BP38">
+        <f t="shared" si="0"/>
+        <v>1.7320508075688772</v>
+      </c>
+      <c r="BQ38">
+        <f t="shared" si="0"/>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="BR38">
+        <f t="shared" si="0"/>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="BS38">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="BT38">
+        <f t="shared" si="0"/>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="BU38">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="BV38">
+        <f t="shared" si="0"/>
+        <v>2.2360679774997898</v>
+      </c>
+      <c r="BW38">
+        <f t="shared" si="0"/>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="BX38">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="BY38">
+        <f t="shared" ref="BY38:DG38" si="1">MIN(BY34:BY37)</f>
+        <v>2.4494897427831779</v>
+      </c>
+      <c r="BZ38">
+        <f t="shared" si="1"/>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="CA38">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="CB38">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="CC38">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="CD38">
+        <f t="shared" si="1"/>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="CE38">
+        <f t="shared" si="1"/>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="CF38">
+        <f t="shared" si="1"/>
+        <v>1.7320508075688772</v>
+      </c>
+      <c r="CG38">
+        <f t="shared" si="1"/>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="CH38">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="CI38">
+        <f t="shared" si="1"/>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="CJ38">
+        <f t="shared" si="1"/>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="CK38">
+        <f t="shared" si="1"/>
+        <v>2.4494897427831779</v>
+      </c>
+      <c r="CL38">
+        <f t="shared" si="1"/>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="CM38">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="CN38">
+        <f t="shared" si="1"/>
+        <v>2.6457513110645907</v>
+      </c>
+      <c r="CO38">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="CP38">
+        <f t="shared" si="1"/>
+        <v>1.7320508075688772</v>
+      </c>
+      <c r="CQ38">
+        <f t="shared" si="1"/>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="CR38">
+        <f t="shared" si="1"/>
+        <v>1.7320508075688772</v>
+      </c>
+      <c r="CS38">
+        <f t="shared" si="1"/>
+        <v>1.7320508075688772</v>
+      </c>
+      <c r="CT38">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="CU38">
+        <f t="shared" si="1"/>
+        <v>2.4494897427831779</v>
+      </c>
+      <c r="CV38">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="CW38">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="CX38">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="CY38">
+        <f t="shared" si="1"/>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="CZ38">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="DA38">
+        <f t="shared" si="1"/>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="DB38">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="DC38">
+        <f t="shared" si="1"/>
+        <v>1.7320508075688772</v>
+      </c>
+      <c r="DD38">
+        <f t="shared" si="1"/>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="DE38">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="DF38">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="DG38">
+        <f t="shared" si="1"/>
+        <v>2.4494897427831779</v>
+      </c>
+    </row>
+    <row r="39" spans="1:113" x14ac:dyDescent="0.2">
+      <c r="G39" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="L39">
+        <f>MATCH(L38,L34:L37,0)</f>
+        <v>1</v>
+      </c>
+      <c r="M39">
+        <f t="shared" ref="M39:BX39" si="2">MATCH(M38,M34:M37,0)</f>
+        <v>1</v>
+      </c>
+      <c r="N39">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="O39">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="P39">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="Q39">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="R39">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="S39">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="T39">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="U39">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="V39">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="W39">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="X39">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="Y39">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="Z39">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="AA39">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="AB39">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="AC39">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="AD39">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="AE39">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="AF39">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="AG39">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="AH39">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="AI39">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="AJ39">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="AK39">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="AL39">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="AM39">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="AN39">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="AO39">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="AP39">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="AQ39">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="AR39">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="AS39">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="AT39">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="AU39">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="AV39">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="AW39">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="AX39">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="AY39">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="AZ39">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="BA39">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="BB39">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="BC39">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="BD39">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="BE39">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="BF39">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="BG39">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="BH39">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="BI39">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="BJ39">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="BK39">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="BL39">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="BM39">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="BN39">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="BO39">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="BP39">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="BQ39">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="BR39">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="BS39">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="BT39">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="BU39">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="BV39">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="BW39">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="BX39">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="BY39">
+        <f t="shared" ref="BY39:DG39" si="3">MATCH(BY38,BY34:BY37,0)</f>
+        <v>1</v>
+      </c>
+      <c r="BZ39">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="CA39">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="CB39">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="CC39">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="CD39">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="CE39">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="CF39">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="CG39">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="CH39">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="CI39">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="CJ39">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="CK39">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="CL39">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="CM39">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="CN39">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="CO39">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="CP39">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="CQ39">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="CR39">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="CS39">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="CT39">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="CU39">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="CV39">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="CW39">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="CX39">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="CY39">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="CZ39">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="DA39">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="DB39">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="DC39">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="DD39">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="DE39">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="DF39">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="DG39">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Run k-means clustering with k=4
</commit_message>
<xml_diff>
--- a/chapter-02/exercise-02.xlsx
+++ b/chapter-02/exercise-02.xlsx
@@ -18,6 +18,37 @@
     <sheet name="Matrix" sheetId="4" r:id="rId4"/>
     <sheet name="4MC" sheetId="5" r:id="rId5"/>
   </sheets>
+  <definedNames>
+    <definedName name="solver_adj" localSheetId="4" hidden="1">'4MC'!$H$2:$K$33</definedName>
+    <definedName name="solver_cvg" localSheetId="4" hidden="1">0.0001</definedName>
+    <definedName name="solver_drv" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="solver_eng" localSheetId="4" hidden="1">3</definedName>
+    <definedName name="solver_itr" localSheetId="4" hidden="1">2147483647</definedName>
+    <definedName name="solver_lhs1" localSheetId="4" hidden="1">'4MC'!$H$2:$K$33</definedName>
+    <definedName name="solver_lin" localSheetId="4" hidden="1">2</definedName>
+    <definedName name="solver_mip" localSheetId="4" hidden="1">2147483647</definedName>
+    <definedName name="solver_mni" localSheetId="4" hidden="1">600</definedName>
+    <definedName name="solver_mrt" localSheetId="4" hidden="1">0.075</definedName>
+    <definedName name="solver_msl" localSheetId="4" hidden="1">2</definedName>
+    <definedName name="solver_neg" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="solver_nod" localSheetId="4" hidden="1">2147483647</definedName>
+    <definedName name="solver_num" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="solver_opt" localSheetId="4" hidden="1">'4MC'!$A$36</definedName>
+    <definedName name="solver_pre" localSheetId="4" hidden="1">0.000001</definedName>
+    <definedName name="solver_rbv" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="solver_rel1" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="solver_rhs1" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="solver_rlx" localSheetId="4" hidden="1">2</definedName>
+    <definedName name="solver_rsd" localSheetId="4" hidden="1">0</definedName>
+    <definedName name="solver_scl" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="solver_sho" localSheetId="4" hidden="1">2</definedName>
+    <definedName name="solver_ssz" localSheetId="4" hidden="1">100</definedName>
+    <definedName name="solver_tim" localSheetId="4" hidden="1">2147483647</definedName>
+    <definedName name="solver_tol" localSheetId="4" hidden="1">0.01</definedName>
+    <definedName name="solver_typ" localSheetId="4" hidden="1">2</definedName>
+    <definedName name="solver_val" localSheetId="4" hidden="1">0</definedName>
+    <definedName name="solver_ver" localSheetId="4" hidden="1">2</definedName>
+  </definedNames>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <pivotCaches>
     <pivotCache cacheId="7" r:id="rId6"/>
@@ -34,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1052" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1051" uniqueCount="155">
   <si>
     <t>Campaign</t>
   </si>
@@ -13400,15 +13431,15 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:DI39"/>
+  <dimension ref="A1:DH39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="DC5" workbookViewId="0">
-      <selection activeCell="L39" sqref="L39:DG39"/>
+    <sheetView tabSelected="1" topLeftCell="DA1" workbookViewId="0">
+      <selection activeCell="DJ3" sqref="DJ3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:113" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:112" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>39</v>
       </c>
@@ -13743,13 +13774,10 @@
         <v>70</v>
       </c>
       <c r="DH1" t="s">
-        <v>141</v>
-      </c>
-      <c r="DI1" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="2" spans="1:113" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:112" x14ac:dyDescent="0.2">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -13771,6 +13799,18 @@
       <c r="G2" t="s">
         <v>9</v>
       </c>
+      <c r="H2">
+        <v>9.8098141190622101E-2</v>
+      </c>
+      <c r="I2">
+        <v>1.6976872499022123E-2</v>
+      </c>
+      <c r="J2">
+        <v>0.18809869025384318</v>
+      </c>
+      <c r="K2">
+        <v>1.2010479399100746E-2</v>
+      </c>
       <c r="V2">
         <v>1</v>
       </c>
@@ -13801,11 +13841,11 @@
       <c r="DE2">
         <v>1</v>
       </c>
-      <c r="DI2">
+      <c r="DH2">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:113" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:112" x14ac:dyDescent="0.2">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -13827,6 +13867,18 @@
       <c r="G3" t="s">
         <v>9</v>
       </c>
+      <c r="H3">
+        <v>8.9120611357485766E-2</v>
+      </c>
+      <c r="I3">
+        <v>6.8989823599790801E-3</v>
+      </c>
+      <c r="J3">
+        <v>9.8109924692461783E-2</v>
+      </c>
+      <c r="K3">
+        <v>0.3162326713142094</v>
+      </c>
       <c r="R3">
         <v>1</v>
       </c>
@@ -13857,11 +13909,11 @@
       <c r="CQ3">
         <v>1</v>
       </c>
-      <c r="DI3">
+      <c r="DH3">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:113" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:112" x14ac:dyDescent="0.2">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -13883,6 +13935,18 @@
       <c r="G4" t="s">
         <v>14</v>
       </c>
+      <c r="H4">
+        <v>2.5397005965878943E-2</v>
+      </c>
+      <c r="I4">
+        <v>2.7537034369223858E-2</v>
+      </c>
+      <c r="J4">
+        <v>0.2194658717458644</v>
+      </c>
+      <c r="K4">
+        <v>1.3798332784306335E-2</v>
+      </c>
       <c r="T4">
         <v>1</v>
       </c>
@@ -13901,11 +13965,11 @@
       <c r="CK4">
         <v>1</v>
       </c>
-      <c r="DI4">
+      <c r="DH4">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:113" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:112" x14ac:dyDescent="0.2">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -13927,6 +13991,18 @@
       <c r="G5" t="s">
         <v>14</v>
       </c>
+      <c r="H5">
+        <v>0.20332512772751074</v>
+      </c>
+      <c r="I5">
+        <v>1.1179690948788666E-2</v>
+      </c>
+      <c r="J5">
+        <v>0.15698496314026172</v>
+      </c>
+      <c r="K5">
+        <v>4.085786032616491E-2</v>
+      </c>
       <c r="V5">
         <v>1</v>
       </c>
@@ -13963,11 +14039,11 @@
       <c r="DF5">
         <v>1</v>
       </c>
-      <c r="DI5">
+      <c r="DH5">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:113" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:112" x14ac:dyDescent="0.2">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -13989,6 +14065,18 @@
       <c r="G6" t="s">
         <v>14</v>
       </c>
+      <c r="H6">
+        <v>8.1552860053866624E-2</v>
+      </c>
+      <c r="I6">
+        <v>1.1146936670206241E-2</v>
+      </c>
+      <c r="J6">
+        <v>3.2314890707839286E-2</v>
+      </c>
+      <c r="K6">
+        <v>2.7949828435221775E-2</v>
+      </c>
       <c r="CA6">
         <v>1</v>
       </c>
@@ -14001,11 +14089,11 @@
       <c r="CO6">
         <v>1</v>
       </c>
-      <c r="DI6">
+      <c r="DH6">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:113" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:112" x14ac:dyDescent="0.2">
       <c r="A7" s="4">
         <v>6</v>
       </c>
@@ -14027,6 +14115,18 @@
       <c r="G7" t="s">
         <v>9</v>
       </c>
+      <c r="H7">
+        <v>0.11069299562886073</v>
+      </c>
+      <c r="I7">
+        <v>2.8194618332972907E-2</v>
+      </c>
+      <c r="J7">
+        <v>0.23391601838337206</v>
+      </c>
+      <c r="K7">
+        <v>7.0756605273044918E-3</v>
+      </c>
       <c r="AQ7">
         <v>1</v>
       </c>
@@ -14063,11 +14163,11 @@
       <c r="DG7">
         <v>1</v>
       </c>
-      <c r="DI7">
+      <c r="DH7">
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:113" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:112" x14ac:dyDescent="0.2">
       <c r="A8" s="4">
         <v>7</v>
       </c>
@@ -14089,6 +14189,18 @@
       <c r="G8" t="s">
         <v>14</v>
       </c>
+      <c r="H8">
+        <v>1.3750096697858833E-2</v>
+      </c>
+      <c r="I8">
+        <v>0.5462794106142127</v>
+      </c>
+      <c r="J8">
+        <v>0.12350982527976925</v>
+      </c>
+      <c r="K8">
+        <v>4.9663845273855152E-2</v>
+      </c>
       <c r="O8">
         <v>1</v>
       </c>
@@ -14146,11 +14258,11 @@
       <c r="DA8">
         <v>1</v>
       </c>
-      <c r="DI8">
+      <c r="DH8">
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:113" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:112" x14ac:dyDescent="0.2">
       <c r="A9" s="4">
         <v>8</v>
       </c>
@@ -14172,6 +14284,18 @@
       <c r="G9" t="s">
         <v>9</v>
       </c>
+      <c r="H9">
+        <v>0.15008671027316384</v>
+      </c>
+      <c r="I9">
+        <v>0.36082493248438385</v>
+      </c>
+      <c r="J9">
+        <v>0.15186473826057587</v>
+      </c>
+      <c r="K9">
+        <v>1.1303392107518354E-2</v>
+      </c>
       <c r="S9">
         <v>1</v>
       </c>
@@ -14232,11 +14356,11 @@
       <c r="DD9">
         <v>1</v>
       </c>
-      <c r="DI9">
+      <c r="DH9">
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:113" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:112" x14ac:dyDescent="0.2">
       <c r="A10" s="4">
         <v>9</v>
       </c>
@@ -14258,6 +14382,18 @@
       <c r="G10" t="s">
         <v>9</v>
       </c>
+      <c r="H10">
+        <v>0.19768539938279617</v>
+      </c>
+      <c r="I10">
+        <v>1.043816045589447E-2</v>
+      </c>
+      <c r="J10">
+        <v>0.11160446035673276</v>
+      </c>
+      <c r="K10">
+        <v>8.4038218872610412E-3</v>
+      </c>
       <c r="M10">
         <v>1</v>
       </c>
@@ -14288,11 +14424,11 @@
       <c r="DG10">
         <v>1</v>
       </c>
-      <c r="DI10">
+      <c r="DH10">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:113" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:112" x14ac:dyDescent="0.2">
       <c r="A11" s="4">
         <v>10</v>
       </c>
@@ -14314,6 +14450,18 @@
       <c r="G11" t="s">
         <v>9</v>
       </c>
+      <c r="H11">
+        <v>6.2931279383046559E-2</v>
+      </c>
+      <c r="I11">
+        <v>3.8743461206360366E-2</v>
+      </c>
+      <c r="J11">
+        <v>8.8350305236403165E-2</v>
+      </c>
+      <c r="K11">
+        <v>6.939826210696097E-2</v>
+      </c>
       <c r="P11">
         <v>1</v>
       </c>
@@ -14335,11 +14483,11 @@
       <c r="DE11">
         <v>1</v>
       </c>
-      <c r="DI11">
+      <c r="DH11">
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:113" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:112" x14ac:dyDescent="0.2">
       <c r="A12" s="4">
         <v>11</v>
       </c>
@@ -14361,6 +14509,18 @@
       <c r="G12" t="s">
         <v>9</v>
       </c>
+      <c r="H12">
+        <v>0.15390105367612669</v>
+      </c>
+      <c r="I12">
+        <v>1.570008583242204E-2</v>
+      </c>
+      <c r="J12">
+        <v>0.26246527058761787</v>
+      </c>
+      <c r="K12">
+        <v>1.6887711083141327E-2</v>
+      </c>
       <c r="T12">
         <v>1</v>
       </c>
@@ -14400,11 +14560,11 @@
       <c r="CU12">
         <v>1</v>
       </c>
-      <c r="DI12">
+      <c r="DH12">
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:113" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:112" x14ac:dyDescent="0.2">
       <c r="A13" s="4">
         <v>12</v>
       </c>
@@ -14426,6 +14586,18 @@
       <c r="G13" t="s">
         <v>9</v>
       </c>
+      <c r="H13">
+        <v>5.1330351057927374E-2</v>
+      </c>
+      <c r="I13">
+        <v>3.5878336127182803E-2</v>
+      </c>
+      <c r="J13">
+        <v>0.10271738633030665</v>
+      </c>
+      <c r="K13">
+        <v>6.2677714434680263E-3</v>
+      </c>
       <c r="AE13">
         <v>1</v>
       </c>
@@ -14441,11 +14613,11 @@
       <c r="BQ13">
         <v>1</v>
       </c>
-      <c r="DI13">
+      <c r="DH13">
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:113" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:112" x14ac:dyDescent="0.2">
       <c r="A14" s="4">
         <v>13</v>
       </c>
@@ -14467,6 +14639,18 @@
       <c r="G14" t="s">
         <v>9</v>
       </c>
+      <c r="H14">
+        <v>2.3877078255815688E-2</v>
+      </c>
+      <c r="I14">
+        <v>0.16711508691895285</v>
+      </c>
+      <c r="J14">
+        <v>1.0700930539018506E-2</v>
+      </c>
+      <c r="K14">
+        <v>4.0779255008244301E-2</v>
+      </c>
       <c r="X14">
         <v>1</v>
       </c>
@@ -14485,11 +14669,11 @@
       <c r="CS14">
         <v>1</v>
       </c>
-      <c r="DI14">
+      <c r="DH14">
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:113" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:112" x14ac:dyDescent="0.2">
       <c r="A15" s="4">
         <v>14</v>
       </c>
@@ -14511,6 +14695,18 @@
       <c r="G15" t="s">
         <v>9</v>
       </c>
+      <c r="H15">
+        <v>0.11212213205097947</v>
+      </c>
+      <c r="I15">
+        <v>3.3850964531510763E-2</v>
+      </c>
+      <c r="J15">
+        <v>0.17160568392803774</v>
+      </c>
+      <c r="K15">
+        <v>8.7307387640118816E-3</v>
+      </c>
       <c r="AK15">
         <v>1</v>
       </c>
@@ -14538,11 +14734,11 @@
       <c r="DE15">
         <v>1</v>
       </c>
-      <c r="DI15">
+      <c r="DH15">
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:113" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:112" x14ac:dyDescent="0.2">
       <c r="A16" s="4">
         <v>15</v>
       </c>
@@ -14564,6 +14760,18 @@
       <c r="G16" t="s">
         <v>9</v>
       </c>
+      <c r="H16">
+        <v>4.7258929048442103E-2</v>
+      </c>
+      <c r="I16">
+        <v>1.5578306214278885E-2</v>
+      </c>
+      <c r="J16">
+        <v>0.13116900093706096</v>
+      </c>
+      <c r="K16">
+        <v>1.9372179169787635E-2</v>
+      </c>
       <c r="AL16">
         <v>1</v>
       </c>
@@ -14582,11 +14790,11 @@
       <c r="DG16">
         <v>1</v>
       </c>
-      <c r="DI16">
+      <c r="DH16">
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:113" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:112" x14ac:dyDescent="0.2">
       <c r="A17" s="4">
         <v>16</v>
       </c>
@@ -14608,6 +14816,18 @@
       <c r="G17" t="s">
         <v>9</v>
       </c>
+      <c r="H17">
+        <v>0.1027249893573314</v>
+      </c>
+      <c r="I17">
+        <v>7.8711929720714346E-3</v>
+      </c>
+      <c r="J17">
+        <v>1.6551111427656241E-2</v>
+      </c>
+      <c r="K17">
+        <v>8.1177201661149778E-3</v>
+      </c>
       <c r="AB17">
         <v>1</v>
       </c>
@@ -14623,11 +14843,11 @@
       <c r="CV17">
         <v>1</v>
       </c>
-      <c r="DI17">
+      <c r="DH17">
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:113" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:112" x14ac:dyDescent="0.2">
       <c r="A18" s="4">
         <v>17</v>
       </c>
@@ -14649,6 +14869,18 @@
       <c r="G18" t="s">
         <v>9</v>
       </c>
+      <c r="H18">
+        <v>6.0822359691202746E-3</v>
+      </c>
+      <c r="I18">
+        <v>3.7639321090010094E-3</v>
+      </c>
+      <c r="J18">
+        <v>1.6142561159172106E-2</v>
+      </c>
+      <c r="K18">
+        <v>0.56370785270948287</v>
+      </c>
       <c r="R18">
         <v>1</v>
       </c>
@@ -14670,11 +14902,11 @@
       <c r="BZ18">
         <v>1</v>
       </c>
-      <c r="DI18">
+      <c r="DH18">
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:113" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:112" x14ac:dyDescent="0.2">
       <c r="A19" s="4">
         <v>18</v>
       </c>
@@ -14696,6 +14928,18 @@
       <c r="G19" t="s">
         <v>9</v>
       </c>
+      <c r="H19">
+        <v>1.7296725704250906E-2</v>
+      </c>
+      <c r="I19">
+        <v>0.39945661540408511</v>
+      </c>
+      <c r="J19">
+        <v>4.9512014456998175E-2</v>
+      </c>
+      <c r="K19">
+        <v>3.7712685865900396E-2</v>
+      </c>
       <c r="L19">
         <v>1</v>
       </c>
@@ -14738,11 +14982,11 @@
       <c r="DC19">
         <v>1</v>
       </c>
-      <c r="DI19">
+      <c r="DH19">
         <v>14</v>
       </c>
     </row>
-    <row r="20" spans="1:113" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:112" x14ac:dyDescent="0.2">
       <c r="A20" s="4">
         <v>19</v>
       </c>
@@ -14764,6 +15008,18 @@
       <c r="G20" t="s">
         <v>9</v>
       </c>
+      <c r="H20">
+        <v>5.6539585397052762E-2</v>
+      </c>
+      <c r="I20">
+        <v>1.7762850049536094E-2</v>
+      </c>
+      <c r="J20">
+        <v>0.10608953559286886</v>
+      </c>
+      <c r="K20">
+        <v>9.7805305989658205E-3</v>
+      </c>
       <c r="P20">
         <v>1</v>
       </c>
@@ -14779,11 +15035,11 @@
       <c r="CK20">
         <v>1</v>
       </c>
-      <c r="DI20">
+      <c r="DH20">
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:113" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:112" x14ac:dyDescent="0.2">
       <c r="A21" s="4">
         <v>20</v>
       </c>
@@ -14805,6 +15061,18 @@
       <c r="G21" t="s">
         <v>9</v>
       </c>
+      <c r="H21">
+        <v>0.10518966519749837</v>
+      </c>
+      <c r="I21">
+        <v>7.8474992310627514E-3</v>
+      </c>
+      <c r="J21">
+        <v>3.8614249840990024E-2</v>
+      </c>
+      <c r="K21">
+        <v>1.5075481773904586E-2</v>
+      </c>
       <c r="AB21">
         <v>1</v>
       </c>
@@ -14823,11 +15091,11 @@
       <c r="CO21">
         <v>1</v>
       </c>
-      <c r="DI21">
+      <c r="DH21">
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:113" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:112" x14ac:dyDescent="0.2">
       <c r="A22" s="4">
         <v>21</v>
       </c>
@@ -14849,6 +15117,18 @@
       <c r="G22" t="s">
         <v>9</v>
       </c>
+      <c r="H22">
+        <v>4.036914245052723E-2</v>
+      </c>
+      <c r="I22">
+        <v>0</v>
+      </c>
+      <c r="J22">
+        <v>8.6867597489324197E-2</v>
+      </c>
+      <c r="K22">
+        <v>7.6526359722270754E-3</v>
+      </c>
       <c r="Q22">
         <v>1</v>
       </c>
@@ -14861,11 +15141,11 @@
       <c r="DF22">
         <v>1</v>
       </c>
-      <c r="DI22">
+      <c r="DH22">
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:113" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:112" x14ac:dyDescent="0.2">
       <c r="A23" s="4">
         <v>22</v>
       </c>
@@ -14887,6 +15167,18 @@
       <c r="G23" t="s">
         <v>9</v>
       </c>
+      <c r="H23">
+        <v>2.6235588935620141E-3</v>
+      </c>
+      <c r="I23">
+        <v>8.5226700263187679E-3</v>
+      </c>
+      <c r="J23">
+        <v>0.97984758450435017</v>
+      </c>
+      <c r="K23">
+        <v>9.7637806021819862E-3</v>
+      </c>
       <c r="Q23">
         <v>1</v>
       </c>
@@ -14950,11 +15242,11 @@
       <c r="DG23">
         <v>1</v>
       </c>
-      <c r="DI23">
+      <c r="DH23">
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:113" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:112" x14ac:dyDescent="0.2">
       <c r="A24" s="4">
         <v>23</v>
       </c>
@@ -14976,6 +15268,18 @@
       <c r="G24" t="s">
         <v>9</v>
       </c>
+      <c r="H24">
+        <v>6.7932780915100785E-2</v>
+      </c>
+      <c r="I24">
+        <v>1.4170362925057451E-2</v>
+      </c>
+      <c r="J24">
+        <v>8.006990057305155E-2</v>
+      </c>
+      <c r="K24">
+        <v>2.0386576047895347E-2</v>
+      </c>
       <c r="AK24">
         <v>1</v>
       </c>
@@ -14991,11 +15295,11 @@
       <c r="CP24">
         <v>1</v>
       </c>
-      <c r="DI24">
+      <c r="DH24">
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:113" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:112" x14ac:dyDescent="0.2">
       <c r="A25" s="4">
         <v>24</v>
       </c>
@@ -15017,6 +15321,18 @@
       <c r="G25" t="s">
         <v>9</v>
       </c>
+      <c r="H25">
+        <v>6.2009104157658406E-3</v>
+      </c>
+      <c r="I25">
+        <v>4.5652689638222546E-3</v>
+      </c>
+      <c r="J25">
+        <v>1.8152399318654078E-2</v>
+      </c>
+      <c r="K25">
+        <v>0.93853692774867414</v>
+      </c>
       <c r="N25">
         <v>1</v>
       </c>
@@ -15053,11 +15369,11 @@
       <c r="CQ25">
         <v>1</v>
       </c>
-      <c r="DI25">
+      <c r="DH25">
         <v>12</v>
       </c>
     </row>
-    <row r="26" spans="1:113" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:112" x14ac:dyDescent="0.2">
       <c r="A26" s="4">
         <v>25</v>
       </c>
@@ -15079,6 +15395,18 @@
       <c r="G26" t="s">
         <v>14</v>
       </c>
+      <c r="H26">
+        <v>7.2960246512473514E-2</v>
+      </c>
+      <c r="I26">
+        <v>3.6237761161483548E-3</v>
+      </c>
+      <c r="J26">
+        <v>8.608776339877254E-2</v>
+      </c>
+      <c r="K26">
+        <v>6.6214311804350017E-3</v>
+      </c>
       <c r="AE26">
         <v>1</v>
       </c>
@@ -15097,11 +15425,11 @@
       <c r="DB26">
         <v>1</v>
       </c>
-      <c r="DI26">
+      <c r="DH26">
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:113" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:112" x14ac:dyDescent="0.2">
       <c r="A27" s="4">
         <v>26</v>
       </c>
@@ -15123,6 +15451,18 @@
       <c r="G27" t="s">
         <v>9</v>
       </c>
+      <c r="H27">
+        <v>0.12401544748834485</v>
+      </c>
+      <c r="I27">
+        <v>1.4032908005567113E-2</v>
+      </c>
+      <c r="J27">
+        <v>3.9766329669111915E-2</v>
+      </c>
+      <c r="K27">
+        <v>0.75604603186283614</v>
+      </c>
       <c r="N27">
         <v>1</v>
       </c>
@@ -15168,11 +15508,11 @@
       <c r="CU27">
         <v>1</v>
       </c>
-      <c r="DI27">
+      <c r="DH27">
         <v>15</v>
       </c>
     </row>
-    <row r="28" spans="1:113" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:112" x14ac:dyDescent="0.2">
       <c r="A28" s="4">
         <v>27</v>
       </c>
@@ -15194,6 +15534,18 @@
       <c r="G28" t="s">
         <v>9</v>
       </c>
+      <c r="H28">
+        <v>0.14573273838517922</v>
+      </c>
+      <c r="I28">
+        <v>1.918081190330832E-2</v>
+      </c>
+      <c r="J28">
+        <v>0.14450542597582575</v>
+      </c>
+      <c r="K28">
+        <v>2.5656535690098691E-2</v>
+      </c>
       <c r="M28">
         <v>1</v>
       </c>
@@ -15221,11 +15573,11 @@
       <c r="DF28">
         <v>1</v>
       </c>
-      <c r="DI28">
+      <c r="DH28">
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:113" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:112" x14ac:dyDescent="0.2">
       <c r="A29" s="4">
         <v>28</v>
       </c>
@@ -15247,6 +15599,18 @@
       <c r="G29" t="s">
         <v>14</v>
       </c>
+      <c r="H29">
+        <v>0.10922139025912911</v>
+      </c>
+      <c r="I29">
+        <v>8.8695031965744589E-3</v>
+      </c>
+      <c r="J29">
+        <v>5.4120086645323404E-2</v>
+      </c>
+      <c r="K29">
+        <v>3.0864187068609544E-3</v>
+      </c>
       <c r="V29">
         <v>1</v>
       </c>
@@ -15265,11 +15629,11 @@
       <c r="BJ29">
         <v>1</v>
       </c>
-      <c r="DI29">
+      <c r="DH29">
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="1:113" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:112" x14ac:dyDescent="0.2">
       <c r="A30" s="4">
         <v>29</v>
       </c>
@@ -15291,6 +15655,18 @@
       <c r="G30" t="s">
         <v>9</v>
       </c>
+      <c r="H30">
+        <v>0.13442072387563284</v>
+      </c>
+      <c r="I30">
+        <v>0.5674396576738745</v>
+      </c>
+      <c r="J30">
+        <v>8.361251805543788E-3</v>
+      </c>
+      <c r="K30">
+        <v>5.6245455729565554E-3</v>
+      </c>
       <c r="L30">
         <v>1</v>
       </c>
@@ -15342,11 +15718,11 @@
       <c r="DA30">
         <v>1</v>
       </c>
-      <c r="DI30">
+      <c r="DH30">
         <v>17</v>
       </c>
     </row>
-    <row r="31" spans="1:113" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:112" x14ac:dyDescent="0.2">
       <c r="A31" s="4">
         <v>30</v>
       </c>
@@ -15368,6 +15744,18 @@
       <c r="G31" t="s">
         <v>9</v>
       </c>
+      <c r="H31">
+        <v>3.510128575268575E-2</v>
+      </c>
+      <c r="I31">
+        <v>0.5853673999822756</v>
+      </c>
+      <c r="J31">
+        <v>0.18920617740392395</v>
+      </c>
+      <c r="K31">
+        <v>1.808072316356792E-2</v>
+      </c>
       <c r="L31">
         <v>1</v>
       </c>
@@ -15434,11 +15822,11 @@
       <c r="DD31">
         <v>1</v>
       </c>
-      <c r="DI31">
+      <c r="DH31">
         <v>22</v>
       </c>
     </row>
-    <row r="32" spans="1:113" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:112" x14ac:dyDescent="0.2">
       <c r="A32" s="4">
         <v>31</v>
       </c>
@@ -15460,6 +15848,18 @@
       <c r="G32" t="s">
         <v>9</v>
       </c>
+      <c r="H32">
+        <v>0.26834449545383871</v>
+      </c>
+      <c r="I32">
+        <v>1.4436219897892193E-2</v>
+      </c>
+      <c r="J32">
+        <v>0.34764149622847901</v>
+      </c>
+      <c r="K32">
+        <v>7.0019378672965968E-2</v>
+      </c>
       <c r="P32">
         <v>1</v>
       </c>
@@ -15511,11 +15911,11 @@
       <c r="DG32">
         <v>1</v>
       </c>
-      <c r="DI32">
+      <c r="DH32">
         <v>17</v>
       </c>
     </row>
-    <row r="33" spans="1:113" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:112" x14ac:dyDescent="0.2">
       <c r="A33" s="4">
         <v>32</v>
       </c>
@@ -15537,6 +15937,18 @@
       <c r="G33" t="s">
         <v>14</v>
       </c>
+      <c r="H33">
+        <v>8.6531377268210932E-2</v>
+      </c>
+      <c r="I33">
+        <v>6.2623775755442897E-3</v>
+      </c>
+      <c r="J33">
+        <v>4.8742415418733552E-2</v>
+      </c>
+      <c r="K33">
+        <v>2.2667681457093001E-2</v>
+      </c>
       <c r="AB33">
         <v>1</v>
       </c>
@@ -15549,2042 +15961,2046 @@
       <c r="DG33">
         <v>1</v>
       </c>
-      <c r="DI33">
+      <c r="DH33">
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="1:113" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:112" x14ac:dyDescent="0.2">
       <c r="G34" t="s">
         <v>149</v>
       </c>
       <c r="L34">
         <f t="array" ref="L34">SQRT(SUM((L$2:L$33-$H$2:$H$33)^2))</f>
-        <v>1.7320508075688772</v>
+        <v>1.7310044087490744</v>
       </c>
       <c r="M34">
         <f t="array" ref="M34">SQRT(SUM((M$2:M$33-$H$2:$H$33)^2))</f>
-        <v>1.4142135623730951</v>
+        <v>1.2973732917853369</v>
       </c>
       <c r="N34">
         <f t="array" ref="N34">SQRT(SUM((N$2:N$33-$H$2:$H$33)^2))</f>
-        <v>1.4142135623730951</v>
+        <v>1.4524396779094308</v>
       </c>
       <c r="O34">
         <f t="array" ref="O34">SQRT(SUM((O$2:O$33-$H$2:$H$33)^2))</f>
-        <v>1.4142135623730951</v>
+        <v>1.5074186441970203</v>
       </c>
       <c r="P34">
         <f t="array" ref="P34">SQRT(SUM((P$2:P$33-$H$2:$H$33)^2))</f>
-        <v>2</v>
+        <v>1.8886192892984752</v>
       </c>
       <c r="Q34">
         <f t="array" ref="Q34">SQRT(SUM((Q$2:Q$33-$H$2:$H$33)^2))</f>
-        <v>2</v>
+        <v>1.9030178090107099</v>
       </c>
       <c r="R34">
         <f t="array" ref="R34">SQRT(SUM((R$2:R$33-$H$2:$H$33)^2))</f>
-        <v>2</v>
+        <v>1.9796907140542026</v>
       </c>
       <c r="S34">
         <f t="array" ref="S34">SQRT(SUM((S$2:S$33-$H$2:$H$33)^2))</f>
-        <v>1.4142135623730951</v>
+        <v>1.3420129900549691</v>
       </c>
       <c r="T34">
         <f t="array" ref="T34">SQRT(SUM((T$2:T$33-$H$2:$H$33)^2))</f>
-        <v>2</v>
+        <v>1.9250966407316827</v>
       </c>
       <c r="U34">
         <f t="array" ref="U34">SQRT(SUM((U$2:U$33-$H$2:$H$33)^2))</f>
-        <v>1.7320508075688772</v>
+        <v>1.7330520826338478</v>
       </c>
       <c r="V34">
         <f t="array" ref="V34">SQRT(SUM((V$2:V$33-$H$2:$H$33)^2))</f>
-        <v>2.2360679774997898</v>
+        <v>2.1150117555528745</v>
       </c>
       <c r="W34">
         <f t="array" ref="W34">SQRT(SUM((W$2:W$33-$H$2:$H$33)^2))</f>
-        <v>1.7320508075688772</v>
+        <v>1.7121155905051153</v>
       </c>
       <c r="X34">
         <f t="array" ref="X34">SQRT(SUM((X$2:X$33-$H$2:$H$33)^2))</f>
-        <v>2</v>
+        <v>1.9888980277052632</v>
       </c>
       <c r="Y34">
         <f t="array" ref="Y34">SQRT(SUM((Y$2:Y$33-$H$2:$H$33)^2))</f>
-        <v>2</v>
+        <v>1.7030647666899406</v>
       </c>
       <c r="Z34">
         <f t="array" ref="Z34">SQRT(SUM((Z$2:Z$33-$H$2:$H$33)^2))</f>
-        <v>1.4142135623730951</v>
+        <v>1.4113855089649485</v>
       </c>
       <c r="AA34">
         <f t="array" ref="AA34">SQRT(SUM((AA$2:AA$33-$H$2:$H$33)^2))</f>
-        <v>1.4142135623730951</v>
+        <v>1.4524396779094308</v>
       </c>
       <c r="AB34">
         <f t="array" ref="AB34">SQRT(SUM((AB$2:AB$33-$H$2:$H$33)^2))</f>
-        <v>2</v>
+        <v>1.8369734387499372</v>
       </c>
       <c r="AC34">
         <f t="array" ref="AC34">SQRT(SUM((AC$2:AC$33-$H$2:$H$33)^2))</f>
-        <v>2</v>
+        <v>1.9796907140542026</v>
       </c>
       <c r="AD34">
         <f t="array" ref="AD34">SQRT(SUM((AD$2:AD$33-$H$2:$H$33)^2))</f>
-        <v>1.4142135623730951</v>
+        <v>1.4251209473294661</v>
       </c>
       <c r="AE34">
         <f t="array" ref="AE34">SQRT(SUM((AE$2:AE$33-$H$2:$H$33)^2))</f>
-        <v>1.7320508075688772</v>
+        <v>1.7652720529272385</v>
       </c>
       <c r="AF34">
         <f t="array" ref="AF34">SQRT(SUM((AF$2:AF$33-$H$2:$H$33)^2))</f>
-        <v>2</v>
+        <v>1.9243949959858007</v>
       </c>
       <c r="AG34">
         <f t="array" ref="AG34">SQRT(SUM((AG$2:AG$33-$H$2:$H$33)^2))</f>
-        <v>1.4142135623730951</v>
+        <v>1.3335572115425667</v>
       </c>
       <c r="AH34">
         <f t="array" ref="AH34">SQRT(SUM((AH$2:AH$33-$H$2:$H$33)^2))</f>
-        <v>1.4142135623730951</v>
+        <v>1.4398962251552678</v>
       </c>
       <c r="AI34">
         <f t="array" ref="AI34">SQRT(SUM((AI$2:AI$33-$H$2:$H$33)^2))</f>
-        <v>2.6457513110645907</v>
+        <v>2.4201637673114131</v>
       </c>
       <c r="AJ34">
         <f t="array" ref="AJ34">SQRT(SUM((AJ$2:AJ$33-$H$2:$H$33)^2))</f>
-        <v>1.4142135623730951</v>
+        <v>1.531485370809692</v>
       </c>
       <c r="AK34">
         <f t="array" ref="AK34">SQRT(SUM((AK$2:AK$33-$H$2:$H$33)^2))</f>
-        <v>2.2360679774997898</v>
+        <v>2.1007355161723122</v>
       </c>
       <c r="AL34">
         <f t="array" ref="AL34">SQRT(SUM((AL$2:AL$33-$H$2:$H$33)^2))</f>
-        <v>1.4142135623730951</v>
+        <v>1.4322191213550493</v>
       </c>
       <c r="AM34">
         <f t="array" ref="AM34">SQRT(SUM((AM$2:AM$33-$H$2:$H$33)^2))</f>
-        <v>2</v>
+        <v>1.87958746762827</v>
       </c>
       <c r="AN34">
         <f t="array" ref="AN34">SQRT(SUM((AN$2:AN$33-$H$2:$H$33)^2))</f>
-        <v>1.4142135623730951</v>
+        <v>1.1991471736615995</v>
       </c>
       <c r="AO34">
         <f t="array" ref="AO34">SQRT(SUM((AO$2:AO$33-$H$2:$H$33)^2))</f>
-        <v>1.7320508075688772</v>
+        <v>1.6774600317046797</v>
       </c>
       <c r="AP34">
         <f t="array" ref="AP34">SQRT(SUM((AP$2:AP$33-$H$2:$H$33)^2))</f>
-        <v>1</v>
+        <v>1.1586688657153752</v>
       </c>
       <c r="AQ34">
         <f t="array" ref="AQ34">SQRT(SUM((AQ$2:AQ$33-$H$2:$H$33)^2))</f>
-        <v>2</v>
+        <v>1.9204161819239152</v>
       </c>
       <c r="AR34">
         <f t="array" ref="AR34">SQRT(SUM((AR$2:AR$33-$H$2:$H$33)^2))</f>
-        <v>1.4142135623730951</v>
+        <v>1.4342121560754164</v>
       </c>
       <c r="AS34">
         <f t="array" ref="AS34">SQRT(SUM((AS$2:AS$33-$H$2:$H$33)^2))</f>
-        <v>2.4494897427831779</v>
+        <v>2.303190293552364</v>
       </c>
       <c r="AT34">
         <f t="array" ref="AT34">SQRT(SUM((AT$2:AT$33-$H$2:$H$33)^2))</f>
-        <v>1.4142135623730951</v>
+        <v>1.3721259073074701</v>
       </c>
       <c r="AU34">
         <f t="array" ref="AU34">SQRT(SUM((AU$2:AU$33-$H$2:$H$33)^2))</f>
-        <v>2</v>
+        <v>1.9792145244520714</v>
       </c>
       <c r="AV34">
         <f t="array" ref="AV34">SQRT(SUM((AV$2:AV$33-$H$2:$H$33)^2))</f>
-        <v>1.7320508075688772</v>
+        <v>1.7188088336166534</v>
       </c>
       <c r="AW34">
         <f t="array" ref="AW34">SQRT(SUM((AW$2:AW$33-$H$2:$H$33)^2))</f>
-        <v>2.2360679774997898</v>
+        <v>2.1576704901498651</v>
       </c>
       <c r="AX34">
         <f t="array" ref="AX34">SQRT(SUM((AX$2:AX$33-$H$2:$H$33)^2))</f>
-        <v>2.2360679774997898</v>
+        <v>2.141963852505778</v>
       </c>
       <c r="AY34">
         <f t="array" ref="AY34">SQRT(SUM((AY$2:AY$33-$H$2:$H$33)^2))</f>
-        <v>2.2360679774997898</v>
+        <v>2.2112869421235954</v>
       </c>
       <c r="AZ34">
         <f t="array" ref="AZ34">SQRT(SUM((AZ$2:AZ$33-$H$2:$H$33)^2))</f>
-        <v>1.4142135623730951</v>
+        <v>1.4524396779094308</v>
       </c>
       <c r="BA34">
         <f t="array" ref="BA34">SQRT(SUM((BA$2:BA$33-$H$2:$H$33)^2))</f>
-        <v>1.7320508075688772</v>
+        <v>1.7599478816224674</v>
       </c>
       <c r="BB34">
         <f t="array" ref="BB34">SQRT(SUM((BB$2:BB$33-$H$2:$H$33)^2))</f>
-        <v>1</v>
+        <v>1.0343308528839041</v>
       </c>
       <c r="BC34">
         <f t="array" ref="BC34">SQRT(SUM((BC$2:BC$33-$H$2:$H$33)^2))</f>
-        <v>2</v>
+        <v>1.7968017883665004</v>
       </c>
       <c r="BD34">
         <f t="array" ref="BD34">SQRT(SUM((BD$2:BD$33-$H$2:$H$33)^2))</f>
-        <v>2</v>
+        <v>1.9978299438908098</v>
       </c>
       <c r="BE34">
         <f t="array" ref="BE34">SQRT(SUM((BE$2:BE$33-$H$2:$H$33)^2))</f>
-        <v>2.2360679774997898</v>
+        <v>2.0962993299077994</v>
       </c>
       <c r="BF34">
         <f t="array" ref="BF34">SQRT(SUM((BF$2:BF$33-$H$2:$H$33)^2))</f>
-        <v>1.7320508075688772</v>
+        <v>1.7239888480864531</v>
       </c>
       <c r="BG34">
         <f t="array" ref="BG34">SQRT(SUM((BG$2:BG$33-$H$2:$H$33)^2))</f>
-        <v>1.7320508075688772</v>
+        <v>1.7792855222477093</v>
       </c>
       <c r="BH34">
         <f t="array" ref="BH34">SQRT(SUM((BH$2:BH$33-$H$2:$H$33)^2))</f>
-        <v>2.2360679774997898</v>
+        <v>2.0187638579274498</v>
       </c>
       <c r="BI34">
         <f t="array" ref="BI34">SQRT(SUM((BI$2:BI$33-$H$2:$H$33)^2))</f>
-        <v>1.7320508075688772</v>
+        <v>1.6326443651905302</v>
       </c>
       <c r="BJ34">
         <f t="array" ref="BJ34">SQRT(SUM((BJ$2:BJ$33-$H$2:$H$33)^2))</f>
-        <v>1.7320508075688772</v>
+        <v>1.7038162336692337</v>
       </c>
       <c r="BK34">
         <f t="array" ref="BK34">SQRT(SUM((BK$2:BK$33-$H$2:$H$33)^2))</f>
-        <v>2.6457513110645907</v>
+        <v>2.4548322531338496</v>
       </c>
       <c r="BL34">
         <f t="array" ref="BL34">SQRT(SUM((BL$2:BL$33-$H$2:$H$33)^2))</f>
-        <v>1.4142135623730951</v>
+        <v>1.412648657195998</v>
       </c>
       <c r="BM34">
         <f t="array" ref="BM34">SQRT(SUM((BM$2:BM$33-$H$2:$H$33)^2))</f>
-        <v>1.4142135623730951</v>
+        <v>1.531485370809692</v>
       </c>
       <c r="BN34">
         <f t="array" ref="BN34">SQRT(SUM((BN$2:BN$33-$H$2:$H$33)^2))</f>
-        <v>2.4494897427831779</v>
+        <v>2.2728701786695162</v>
       </c>
       <c r="BO34">
         <f t="array" ref="BO34">SQRT(SUM((BO$2:BO$33-$H$2:$H$33)^2))</f>
-        <v>1.4142135623730951</v>
+        <v>1.3420129900549691</v>
       </c>
       <c r="BP34">
         <f t="array" ref="BP34">SQRT(SUM((BP$2:BP$33-$H$2:$H$33)^2))</f>
-        <v>1.7320508075688772</v>
+        <v>1.7599478816224674</v>
       </c>
       <c r="BQ34">
         <f t="array" ref="BQ34">SQRT(SUM((BQ$2:BQ$33-$H$2:$H$33)^2))</f>
-        <v>1.4142135623730951</v>
+        <v>1.4966137906161026</v>
       </c>
       <c r="BR34">
         <f t="array" ref="BR34">SQRT(SUM((BR$2:BR$33-$H$2:$H$33)^2))</f>
-        <v>1.4142135623730951</v>
+        <v>1.5050640221797871</v>
       </c>
       <c r="BS34">
         <f t="array" ref="BS34">SQRT(SUM((BS$2:BS$33-$H$2:$H$33)^2))</f>
-        <v>2</v>
+        <v>1.7537693847633125</v>
       </c>
       <c r="BT34">
         <f t="array" ref="BT34">SQRT(SUM((BT$2:BT$33-$H$2:$H$33)^2))</f>
-        <v>1.4142135623730951</v>
+        <v>1.3115813249936463</v>
       </c>
       <c r="BU34">
         <f t="array" ref="BU34">SQRT(SUM((BU$2:BU$33-$H$2:$H$33)^2))</f>
-        <v>1</v>
+        <v>1.0343308528839041</v>
       </c>
       <c r="BV34">
         <f t="array" ref="BV34">SQRT(SUM((BV$2:BV$33-$H$2:$H$33)^2))</f>
-        <v>2.2360679774997898</v>
+        <v>1.9598091434252001</v>
       </c>
       <c r="BW34">
         <f t="array" ref="BW34">SQRT(SUM((BW$2:BW$33-$H$2:$H$33)^2))</f>
-        <v>1.4142135623730951</v>
+        <v>1.5050640221797871</v>
       </c>
       <c r="BX34">
         <f t="array" ref="BX34">SQRT(SUM((BX$2:BX$33-$H$2:$H$33)^2))</f>
-        <v>2</v>
+        <v>1.9225511287251651</v>
       </c>
       <c r="BY34">
         <f t="array" ref="BY34">SQRT(SUM((BY$2:BY$33-$H$2:$H$33)^2))</f>
-        <v>2.4494897427831779</v>
+        <v>2.2791120499734792</v>
       </c>
       <c r="BZ34">
         <f t="array" ref="BZ34">SQRT(SUM((BZ$2:BZ$33-$H$2:$H$33)^2))</f>
-        <v>1.4142135623730951</v>
+        <v>1.531485370809692</v>
       </c>
       <c r="CA34">
         <f t="array" ref="CA34">SQRT(SUM((CA$2:CA$33-$H$2:$H$33)^2))</f>
-        <v>1</v>
+        <v>1.0985936526605908</v>
       </c>
       <c r="CB34">
         <f t="array" ref="CB34">SQRT(SUM((CB$2:CB$33-$H$2:$H$33)^2))</f>
-        <v>2</v>
+        <v>1.8872410474532537</v>
       </c>
       <c r="CC34">
         <f t="array" ref="CC34">SQRT(SUM((CC$2:CC$33-$H$2:$H$33)^2))</f>
-        <v>1</v>
+        <v>0.98724005946288462</v>
       </c>
       <c r="CD34">
         <f t="array" ref="CD34">SQRT(SUM((CD$2:CD$33-$H$2:$H$33)^2))</f>
-        <v>1.4142135623730951</v>
+        <v>1.4080709320073972</v>
       </c>
       <c r="CE34">
         <f t="array" ref="CE34">SQRT(SUM((CE$2:CE$33-$H$2:$H$33)^2))</f>
-        <v>1.4142135623730951</v>
+        <v>1.3560152555108214</v>
       </c>
       <c r="CF34">
         <f t="array" ref="CF34">SQRT(SUM((CF$2:CF$33-$H$2:$H$33)^2))</f>
-        <v>1.7320508075688772</v>
+        <v>1.7585751655238595</v>
       </c>
       <c r="CG34">
         <f t="array" ref="CG34">SQRT(SUM((CG$2:CG$33-$H$2:$H$33)^2))</f>
-        <v>1.4142135623730951</v>
+        <v>1.5191840207722211</v>
       </c>
       <c r="CH34">
         <f t="array" ref="CH34">SQRT(SUM((CH$2:CH$33-$H$2:$H$33)^2))</f>
-        <v>1</v>
+        <v>0.91286622397051942</v>
       </c>
       <c r="CI34">
         <f t="array" ref="CI34">SQRT(SUM((CI$2:CI$33-$H$2:$H$33)^2))</f>
-        <v>1.4142135623730951</v>
+        <v>1.4400250319445453</v>
       </c>
       <c r="CJ34">
         <f t="array" ref="CJ34">SQRT(SUM((CJ$2:CJ$33-$H$2:$H$33)^2))</f>
-        <v>1.4142135623730951</v>
+        <v>1.3941813426101393</v>
       </c>
       <c r="CK34">
         <f t="array" ref="CK34">SQRT(SUM((CK$2:CK$33-$H$2:$H$33)^2))</f>
-        <v>2.4494897427831779</v>
+        <v>2.4067574731197547</v>
       </c>
       <c r="CL34">
         <f t="array" ref="CL34">SQRT(SUM((CL$2:CL$33-$H$2:$H$33)^2))</f>
-        <v>1.4142135623730951</v>
+        <v>1.5015598547724682</v>
       </c>
       <c r="CM34">
         <f t="array" ref="CM34">SQRT(SUM((CM$2:CM$33-$H$2:$H$33)^2))</f>
-        <v>1</v>
+        <v>1.0592369134415502</v>
       </c>
       <c r="CN34">
         <f t="array" ref="CN34">SQRT(SUM((CN$2:CN$33-$H$2:$H$33)^2))</f>
-        <v>2.6457513110645907</v>
+        <v>2.4531282666940726</v>
       </c>
       <c r="CO34">
         <f t="array" ref="CO34">SQRT(SUM((CO$2:CO$33-$H$2:$H$33)^2))</f>
-        <v>3</v>
+        <v>2.6599195213497859</v>
       </c>
       <c r="CP34">
         <f t="array" ref="CP34">SQRT(SUM((CP$2:CP$33-$H$2:$H$33)^2))</f>
-        <v>1.7320508075688772</v>
+        <v>1.6698855998492803</v>
       </c>
       <c r="CQ34">
         <f t="array" ref="CQ34">SQRT(SUM((CQ$2:CQ$33-$H$2:$H$33)^2))</f>
-        <v>1.4142135623730951</v>
+        <v>1.4762691794613099</v>
       </c>
       <c r="CR34">
         <f t="array" ref="CR34">SQRT(SUM((CR$2:CR$33-$H$2:$H$33)^2))</f>
-        <v>1.7320508075688772</v>
+        <v>1.6525121161343741</v>
       </c>
       <c r="CS34">
         <f t="array" ref="CS34">SQRT(SUM((CS$2:CS$33-$H$2:$H$33)^2))</f>
-        <v>1.7320508075688772</v>
+        <v>1.7284364915458743</v>
       </c>
       <c r="CT34">
         <f t="array" ref="CT34">SQRT(SUM((CT$2:CT$33-$H$2:$H$33)^2))</f>
-        <v>2</v>
+        <v>1.9922038223316947</v>
       </c>
       <c r="CU34">
         <f t="array" ref="CU34">SQRT(SUM((CU$2:CU$33-$H$2:$H$33)^2))</f>
-        <v>2.4494897427831779</v>
+        <v>2.1428297017591276</v>
       </c>
       <c r="CV34">
         <f t="array" ref="CV34">SQRT(SUM((CV$2:CV$33-$H$2:$H$33)^2))</f>
-        <v>2</v>
+        <v>1.884958856782635</v>
       </c>
       <c r="CW34">
         <f t="array" ref="CW34">SQRT(SUM((CW$2:CW$33-$H$2:$H$33)^2))</f>
-        <v>1</v>
+        <v>1.0343308528839041</v>
       </c>
       <c r="CX34">
         <f t="array" ref="CX34">SQRT(SUM((CX$2:CX$33-$H$2:$H$33)^2))</f>
-        <v>2</v>
+        <v>1.7069923899605102</v>
       </c>
       <c r="CY34">
         <f t="array" ref="CY34">SQRT(SUM((CY$2:CY$33-$H$2:$H$33)^2))</f>
-        <v>1.4142135623730951</v>
+        <v>1.4375600281776426</v>
       </c>
       <c r="CZ34">
         <f t="array" ref="CZ34">SQRT(SUM((CZ$2:CZ$33-$H$2:$H$33)^2))</f>
-        <v>1</v>
+        <v>0.98151081416296715</v>
       </c>
       <c r="DA34">
         <f t="array" ref="DA34">SQRT(SUM((DA$2:DA$33-$H$2:$H$33)^2))</f>
-        <v>1.4142135623730951</v>
+        <v>1.4400250319445453</v>
       </c>
       <c r="DB34">
         <f t="array" ref="DB34">SQRT(SUM((DB$2:DB$33-$H$2:$H$33)^2))</f>
-        <v>2</v>
+        <v>1.9810096636196579</v>
       </c>
       <c r="DC34">
         <f t="array" ref="DC34">SQRT(SUM((DC$2:DC$33-$H$2:$H$33)^2))</f>
-        <v>1.7320508075688772</v>
+        <v>1.6713719435453525</v>
       </c>
       <c r="DD34">
         <f t="array" ref="DD34">SQRT(SUM((DD$2:DD$33-$H$2:$H$33)^2))</f>
-        <v>1.4142135623730951</v>
+        <v>1.4140854789305253</v>
       </c>
       <c r="DE34">
         <f t="array" ref="DE34">SQRT(SUM((DE$2:DE$33-$H$2:$H$33)^2))</f>
-        <v>2</v>
+        <v>1.8130145166591742</v>
       </c>
       <c r="DF34">
         <f t="array" ref="DF34">SQRT(SUM((DF$2:DF$33-$H$2:$H$33)^2))</f>
-        <v>2</v>
+        <v>1.8356943442168461</v>
       </c>
       <c r="DG34">
         <f t="array" ref="DG34">SQRT(SUM((DG$2:DG$33-$H$2:$H$33)^2))</f>
-        <v>2.4494897427831779</v>
-      </c>
-    </row>
-    <row r="35" spans="1:113" x14ac:dyDescent="0.2">
+        <v>2.2234523206991534</v>
+      </c>
+    </row>
+    <row r="35" spans="1:112" x14ac:dyDescent="0.2">
       <c r="G35" t="s">
         <v>150</v>
       </c>
       <c r="L35">
         <f t="array" ref="L35">SQRT(SUM((L$2:L$33-$I$2:$I$33)^2))</f>
-        <v>1.7320508075688772</v>
+        <v>1.0883687942579159</v>
       </c>
       <c r="M35">
         <f t="array" ref="M35">SQRT(SUM((M$2:M$33-$I$2:$I$33)^2))</f>
-        <v>1.4142135623730951</v>
+        <v>1.797174458341898</v>
       </c>
       <c r="N35">
         <f t="array" ref="N35">SQRT(SUM((N$2:N$33-$I$2:$I$33)^2))</f>
-        <v>1.4142135623730951</v>
+        <v>1.8032963218772786</v>
       </c>
       <c r="O35">
         <f t="array" ref="O35">SQRT(SUM((O$2:O$33-$I$2:$I$33)^2))</f>
-        <v>1.4142135623730951</v>
+        <v>1.0128081542137797</v>
       </c>
       <c r="P35">
         <f t="array" ref="P35">SQRT(SUM((P$2:P$33-$I$2:$I$33)^2))</f>
-        <v>2</v>
+        <v>2.0136112074824415</v>
       </c>
       <c r="Q35">
         <f t="array" ref="Q35">SQRT(SUM((Q$2:Q$33-$I$2:$I$33)^2))</f>
-        <v>2</v>
+        <v>2.2728108755841867</v>
       </c>
       <c r="R35">
         <f t="array" ref="R35">SQRT(SUM((R$2:R$33-$I$2:$I$33)^2))</f>
-        <v>2</v>
+        <v>2.2870399636994017</v>
       </c>
       <c r="S35">
         <f t="array" ref="S35">SQRT(SUM((S$2:S$33-$I$2:$I$33)^2))</f>
-        <v>1.4142135623730951</v>
+        <v>1.1968896348947062</v>
       </c>
       <c r="T35">
         <f t="array" ref="T35">SQRT(SUM((T$2:T$33-$I$2:$I$33)^2))</f>
-        <v>2</v>
+        <v>2.1127954309421919</v>
       </c>
       <c r="U35">
         <f t="array" ref="U35">SQRT(SUM((U$2:U$33-$I$2:$I$33)^2))</f>
-        <v>1.7320508075688772</v>
+        <v>0.94387554364660509</v>
       </c>
       <c r="V35">
         <f t="array" ref="V35">SQRT(SUM((V$2:V$33-$I$2:$I$33)^2))</f>
-        <v>2.2360679774997898</v>
+        <v>2.2421511334272139</v>
       </c>
       <c r="W35">
         <f t="array" ref="W35">SQRT(SUM((W$2:W$33-$I$2:$I$33)^2))</f>
-        <v>1.7320508075688772</v>
+        <v>2.0586596755598441</v>
       </c>
       <c r="X35">
         <f t="array" ref="X35">SQRT(SUM((X$2:X$33-$I$2:$I$33)^2))</f>
-        <v>2</v>
+        <v>1.2476661685147472</v>
       </c>
       <c r="Y35">
         <f t="array" ref="Y35">SQRT(SUM((Y$2:Y$33-$I$2:$I$33)^2))</f>
-        <v>2</v>
+        <v>2.2778724676073385</v>
       </c>
       <c r="Z35">
         <f t="array" ref="Z35">SQRT(SUM((Z$2:Z$33-$I$2:$I$33)^2))</f>
-        <v>1.4142135623730951</v>
+        <v>1.4446241749346109</v>
       </c>
       <c r="AA35">
         <f t="array" ref="AA35">SQRT(SUM((AA$2:AA$33-$I$2:$I$33)^2))</f>
-        <v>1.4142135623730951</v>
+        <v>1.8032963218772786</v>
       </c>
       <c r="AB35">
         <f t="array" ref="AB35">SQRT(SUM((AB$2:AB$33-$I$2:$I$33)^2))</f>
-        <v>2</v>
+        <v>2.2853342112216248</v>
       </c>
       <c r="AC35">
         <f t="array" ref="AC35">SQRT(SUM((AC$2:AC$33-$I$2:$I$33)^2))</f>
-        <v>2</v>
+        <v>2.2870399636994017</v>
       </c>
       <c r="AD35">
         <f t="array" ref="AD35">SQRT(SUM((AD$2:AD$33-$I$2:$I$33)^2))</f>
-        <v>1.4142135623730951</v>
+        <v>0.99169544877578208</v>
       </c>
       <c r="AE35">
         <f t="array" ref="AE35">SQRT(SUM((AE$2:AE$33-$I$2:$I$33)^2))</f>
-        <v>1.7320508075688772</v>
+        <v>2.0476875772186536</v>
       </c>
       <c r="AF35">
         <f t="array" ref="AF35">SQRT(SUM((AF$2:AF$33-$I$2:$I$33)^2))</f>
-        <v>2</v>
+        <v>1.0813191836481062</v>
       </c>
       <c r="AG35">
         <f t="array" ref="AG35">SQRT(SUM((AG$2:AG$33-$I$2:$I$33)^2))</f>
-        <v>1.4142135623730951</v>
+        <v>1.5903026409018868</v>
       </c>
       <c r="AH35">
         <f t="array" ref="AH35">SQRT(SUM((AH$2:AH$33-$I$2:$I$33)^2))</f>
-        <v>1.4142135623730951</v>
+        <v>1.7982399769151074</v>
       </c>
       <c r="AI35">
         <f t="array" ref="AI35">SQRT(SUM((AI$2:AI$33-$I$2:$I$33)^2))</f>
-        <v>2.6457513110645907</v>
+        <v>2.641122963976863</v>
       </c>
       <c r="AJ35">
         <f t="array" ref="AJ35">SQRT(SUM((AJ$2:AJ$33-$I$2:$I$33)^2))</f>
-        <v>1.4142135623730951</v>
+        <v>1.8089819170708294</v>
       </c>
       <c r="AK35">
         <f t="array" ref="AK35">SQRT(SUM((AK$2:AK$33-$I$2:$I$33)^2))</f>
-        <v>2.2360679774997898</v>
+        <v>2.4740969903298642</v>
       </c>
       <c r="AL35">
         <f t="array" ref="AL35">SQRT(SUM((AL$2:AL$33-$I$2:$I$33)^2))</f>
-        <v>1.4142135623730951</v>
+        <v>1.7861174196965104</v>
       </c>
       <c r="AM35">
         <f t="array" ref="AM35">SQRT(SUM((AM$2:AM$33-$I$2:$I$33)^2))</f>
-        <v>2</v>
+        <v>2.2852147603506645</v>
       </c>
       <c r="AN35">
         <f t="array" ref="AN35">SQRT(SUM((AN$2:AN$33-$I$2:$I$33)^2))</f>
-        <v>1.4142135623730951</v>
+        <v>1.7998125507194707</v>
       </c>
       <c r="AO35">
         <f t="array" ref="AO35">SQRT(SUM((AO$2:AO$33-$I$2:$I$33)^2))</f>
-        <v>1.7320508075688772</v>
+        <v>2.0429168128500135</v>
       </c>
       <c r="AP35">
         <f t="array" ref="AP35">SQRT(SUM((AP$2:AP$33-$I$2:$I$33)^2))</f>
-        <v>1</v>
+        <v>1.0938533526970031</v>
       </c>
       <c r="AQ35">
         <f t="array" ref="AQ35">SQRT(SUM((AQ$2:AQ$33-$I$2:$I$33)^2))</f>
-        <v>2</v>
+        <v>1.9064717998384595</v>
       </c>
       <c r="AR35">
         <f t="array" ref="AR35">SQRT(SUM((AR$2:AR$33-$I$2:$I$33)^2))</f>
-        <v>1.4142135623730951</v>
+        <v>1.8001745656234061</v>
       </c>
       <c r="AS35">
         <f t="array" ref="AS35">SQRT(SUM((AS$2:AS$33-$I$2:$I$33)^2))</f>
-        <v>2.4494897427831779</v>
+        <v>2.4549610739652521</v>
       </c>
       <c r="AT35">
         <f t="array" ref="AT35">SQRT(SUM((AT$2:AT$33-$I$2:$I$33)^2))</f>
-        <v>1.4142135623730951</v>
+        <v>1.4616619502107873</v>
       </c>
       <c r="AU35">
         <f t="array" ref="AU35">SQRT(SUM((AU$2:AU$33-$I$2:$I$33)^2))</f>
-        <v>2</v>
+        <v>1.5045085273455601</v>
       </c>
       <c r="AV35">
         <f t="array" ref="AV35">SQRT(SUM((AV$2:AV$33-$I$2:$I$33)^2))</f>
-        <v>1.7320508075688772</v>
+        <v>2.0417815246649318</v>
       </c>
       <c r="AW35">
         <f t="array" ref="AW35">SQRT(SUM((AW$2:AW$33-$I$2:$I$33)^2))</f>
-        <v>2.2360679774997898</v>
+        <v>1.3546294707732818</v>
       </c>
       <c r="AX35">
         <f t="array" ref="AX35">SQRT(SUM((AX$2:AX$33-$I$2:$I$33)^2))</f>
-        <v>2.2360679774997898</v>
+        <v>2.4822812380088717</v>
       </c>
       <c r="AY35">
         <f t="array" ref="AY35">SQRT(SUM((AY$2:AY$33-$I$2:$I$33)^2))</f>
-        <v>2.2360679774997898</v>
+        <v>1.4734269875453891</v>
       </c>
       <c r="AZ35">
         <f t="array" ref="AZ35">SQRT(SUM((AZ$2:AZ$33-$I$2:$I$33)^2))</f>
-        <v>1.4142135623730951</v>
+        <v>1.8032963218772786</v>
       </c>
       <c r="BA35">
         <f t="array" ref="BA35">SQRT(SUM((BA$2:BA$33-$I$2:$I$33)^2))</f>
-        <v>1.7320508075688772</v>
+        <v>2.0601819726126425</v>
       </c>
       <c r="BB35">
         <f t="array" ref="BB35">SQRT(SUM((BB$2:BB$33-$I$2:$I$33)^2))</f>
-        <v>1</v>
+        <v>1.2519680960256665</v>
       </c>
       <c r="BC35">
         <f t="array" ref="BC35">SQRT(SUM((BC$2:BC$33-$I$2:$I$33)^2))</f>
-        <v>2</v>
+        <v>2.2749928677602389</v>
       </c>
       <c r="BD35">
         <f t="array" ref="BD35">SQRT(SUM((BD$2:BD$33-$I$2:$I$33)^2))</f>
-        <v>2</v>
+        <v>1.3887017092279574</v>
       </c>
       <c r="BE35">
         <f t="array" ref="BE35">SQRT(SUM((BE$2:BE$33-$I$2:$I$33)^2))</f>
-        <v>2.2360679774997898</v>
+        <v>2.4697862918223663</v>
       </c>
       <c r="BF35">
         <f t="array" ref="BF35">SQRT(SUM((BF$2:BF$33-$I$2:$I$33)^2))</f>
-        <v>1.7320508075688772</v>
+        <v>1.1419853292722966</v>
       </c>
       <c r="BG35">
         <f t="array" ref="BG35">SQRT(SUM((BG$2:BG$33-$I$2:$I$33)^2))</f>
-        <v>1.7320508075688772</v>
+        <v>1.7504154267074161</v>
       </c>
       <c r="BH35">
         <f t="array" ref="BH35">SQRT(SUM((BH$2:BH$33-$I$2:$I$33)^2))</f>
-        <v>2.2360679774997898</v>
+        <v>2.4802291957960154</v>
       </c>
       <c r="BI35">
         <f t="array" ref="BI35">SQRT(SUM((BI$2:BI$33-$I$2:$I$33)^2))</f>
-        <v>1.7320508075688772</v>
+        <v>2.0557569982021096</v>
       </c>
       <c r="BJ35">
         <f t="array" ref="BJ35">SQRT(SUM((BJ$2:BJ$33-$I$2:$I$33)^2))</f>
-        <v>1.7320508075688772</v>
+        <v>2.0475181922403252</v>
       </c>
       <c r="BK35">
         <f t="array" ref="BK35">SQRT(SUM((BK$2:BK$33-$I$2:$I$33)^2))</f>
-        <v>2.6457513110645907</v>
+        <v>2.825257647041437</v>
       </c>
       <c r="BL35">
         <f t="array" ref="BL35">SQRT(SUM((BL$2:BL$33-$I$2:$I$33)^2))</f>
-        <v>1.4142135623730951</v>
+        <v>1.8003672593992863</v>
       </c>
       <c r="BM35">
         <f t="array" ref="BM35">SQRT(SUM((BM$2:BM$33-$I$2:$I$33)^2))</f>
-        <v>1.4142135623730951</v>
+        <v>1.8089819170708294</v>
       </c>
       <c r="BN35">
         <f t="array" ref="BN35">SQRT(SUM((BN$2:BN$33-$I$2:$I$33)^2))</f>
-        <v>2.4494897427831779</v>
+        <v>2.3102018473770354</v>
       </c>
       <c r="BO35">
         <f t="array" ref="BO35">SQRT(SUM((BO$2:BO$33-$I$2:$I$33)^2))</f>
-        <v>1.4142135623730951</v>
+        <v>1.1968896348947062</v>
       </c>
       <c r="BP35">
         <f t="array" ref="BP35">SQRT(SUM((BP$2:BP$33-$I$2:$I$33)^2))</f>
-        <v>1.7320508075688772</v>
+        <v>2.0601819726126425</v>
       </c>
       <c r="BQ35">
         <f t="array" ref="BQ35">SQRT(SUM((BQ$2:BQ$33-$I$2:$I$33)^2))</f>
-        <v>1.4142135623730951</v>
+        <v>1.4576551323794356</v>
       </c>
       <c r="BR35">
         <f t="array" ref="BR35">SQRT(SUM((BR$2:BR$33-$I$2:$I$33)^2))</f>
-        <v>1.4142135623730951</v>
+        <v>1.1486626779268918</v>
       </c>
       <c r="BS35">
         <f t="array" ref="BS35">SQRT(SUM((BS$2:BS$33-$I$2:$I$33)^2))</f>
-        <v>2</v>
+        <v>2.1121359385783678</v>
       </c>
       <c r="BT35">
         <f t="array" ref="BT35">SQRT(SUM((BT$2:BT$33-$I$2:$I$33)^2))</f>
-        <v>1.4142135623730951</v>
+        <v>1.7957382433250242</v>
       </c>
       <c r="BU35">
         <f t="array" ref="BU35">SQRT(SUM((BU$2:BU$33-$I$2:$I$33)^2))</f>
-        <v>1</v>
+        <v>1.2519680960256665</v>
       </c>
       <c r="BV35">
         <f t="array" ref="BV35">SQRT(SUM((BV$2:BV$33-$I$2:$I$33)^2))</f>
-        <v>2.2360679774997898</v>
+        <v>2.2499965927130323</v>
       </c>
       <c r="BW35">
         <f t="array" ref="BW35">SQRT(SUM((BW$2:BW$33-$I$2:$I$33)^2))</f>
-        <v>1.4142135623730951</v>
+        <v>1.1486626779268918</v>
       </c>
       <c r="BX35">
         <f t="array" ref="BX35">SQRT(SUM((BX$2:BX$33-$I$2:$I$33)^2))</f>
-        <v>2</v>
+        <v>1.2095026942283604</v>
       </c>
       <c r="BY35">
         <f t="array" ref="BY35">SQRT(SUM((BY$2:BY$33-$I$2:$I$33)^2))</f>
-        <v>2.4494897427831779</v>
+        <v>2.658771742861036</v>
       </c>
       <c r="BZ35">
         <f t="array" ref="BZ35">SQRT(SUM((BZ$2:BZ$33-$I$2:$I$33)^2))</f>
-        <v>1.4142135623730951</v>
+        <v>1.8089819170708294</v>
       </c>
       <c r="CA35">
         <f t="array" ref="CA35">SQRT(SUM((CA$2:CA$33-$I$2:$I$33)^2))</f>
-        <v>1</v>
+        <v>1.5055829784819192</v>
       </c>
       <c r="CB35">
         <f t="array" ref="CB35">SQRT(SUM((CB$2:CB$33-$I$2:$I$33)^2))</f>
-        <v>2</v>
+        <v>2.0095939026638896</v>
       </c>
       <c r="CC35">
         <f t="array" ref="CC35">SQRT(SUM((CC$2:CC$33-$I$2:$I$33)^2))</f>
-        <v>1</v>
+        <v>1.5060536702000733</v>
       </c>
       <c r="CD35">
         <f t="array" ref="CD35">SQRT(SUM((CD$2:CD$33-$I$2:$I$33)^2))</f>
-        <v>1.4142135623730951</v>
+        <v>1.7885967058091843</v>
       </c>
       <c r="CE35">
         <f t="array" ref="CE35">SQRT(SUM((CE$2:CE$33-$I$2:$I$33)^2))</f>
-        <v>1.4142135623730951</v>
+        <v>1.7999602583593328</v>
       </c>
       <c r="CF35">
         <f t="array" ref="CF35">SQRT(SUM((CF$2:CF$33-$I$2:$I$33)^2))</f>
-        <v>1.7320508075688772</v>
+        <v>2.0397463893773335</v>
       </c>
       <c r="CG35">
         <f t="array" ref="CG35">SQRT(SUM((CG$2:CG$33-$I$2:$I$33)^2))</f>
-        <v>1.4142135623730951</v>
+        <v>1.1822021512407699</v>
       </c>
       <c r="CH35">
         <f t="array" ref="CH35">SQRT(SUM((CH$2:CH$33-$I$2:$I$33)^2))</f>
-        <v>1</v>
+        <v>1.5033966670972487</v>
       </c>
       <c r="CI35">
         <f t="array" ref="CI35">SQRT(SUM((CI$2:CI$33-$I$2:$I$33)^2))</f>
-        <v>1.4142135623730951</v>
+        <v>1.0303571428678142</v>
       </c>
       <c r="CJ35">
         <f t="array" ref="CJ35">SQRT(SUM((CJ$2:CJ$33-$I$2:$I$33)^2))</f>
-        <v>1.4142135623730951</v>
+        <v>1.802001719672822</v>
       </c>
       <c r="CK35">
         <f t="array" ref="CK35">SQRT(SUM((CK$2:CK$33-$I$2:$I$33)^2))</f>
-        <v>2.4494897427831779</v>
+        <v>2.3167261778957715</v>
       </c>
       <c r="CL35">
         <f t="array" ref="CL35">SQRT(SUM((CL$2:CL$33-$I$2:$I$33)^2))</f>
-        <v>1.4142135623730951</v>
+        <v>1.5780243178185596</v>
       </c>
       <c r="CM35">
         <f t="array" ref="CM35">SQRT(SUM((CM$2:CM$33-$I$2:$I$33)^2))</f>
-        <v>1</v>
+        <v>1.5036649102854551</v>
       </c>
       <c r="CN35">
         <f t="array" ref="CN35">SQRT(SUM((CN$2:CN$33-$I$2:$I$33)^2))</f>
-        <v>2.6457513110645907</v>
+        <v>2.8433705399014451</v>
       </c>
       <c r="CO35">
         <f t="array" ref="CO35">SQRT(SUM((CO$2:CO$33-$I$2:$I$33)^2))</f>
-        <v>3</v>
+        <v>3.1702985478107153</v>
       </c>
       <c r="CP35">
         <f t="array" ref="CP35">SQRT(SUM((CP$2:CP$33-$I$2:$I$33)^2))</f>
-        <v>1.7320508075688772</v>
+        <v>2.0338736654118459</v>
       </c>
       <c r="CQ35">
         <f t="array" ref="CQ35">SQRT(SUM((CQ$2:CQ$33-$I$2:$I$33)^2))</f>
-        <v>1.4142135623730951</v>
+        <v>1.8072480393646293</v>
       </c>
       <c r="CR35">
         <f t="array" ref="CR35">SQRT(SUM((CR$2:CR$33-$I$2:$I$33)^2))</f>
-        <v>1.7320508075688772</v>
+        <v>1.1233031639561211</v>
       </c>
       <c r="CS35">
         <f t="array" ref="CS35">SQRT(SUM((CS$2:CS$33-$I$2:$I$33)^2))</f>
-        <v>1.7320508075688772</v>
+        <v>1.5602181606493553</v>
       </c>
       <c r="CT35">
         <f t="array" ref="CT35">SQRT(SUM((CT$2:CT$33-$I$2:$I$33)^2))</f>
-        <v>2</v>
+        <v>1.044982206109752</v>
       </c>
       <c r="CU35">
         <f t="array" ref="CU35">SQRT(SUM((CU$2:CU$33-$I$2:$I$33)^2))</f>
-        <v>2.4494897427831779</v>
+        <v>2.66171309759119</v>
       </c>
       <c r="CV35">
         <f t="array" ref="CV35">SQRT(SUM((CV$2:CV$33-$I$2:$I$33)^2))</f>
-        <v>2</v>
+        <v>2.0185323676825497</v>
       </c>
       <c r="CW35">
         <f t="array" ref="CW35">SQRT(SUM((CW$2:CW$33-$I$2:$I$33)^2))</f>
-        <v>1</v>
+        <v>1.2519680960256665</v>
       </c>
       <c r="CX35">
         <f t="array" ref="CX35">SQRT(SUM((CX$2:CX$33-$I$2:$I$33)^2))</f>
-        <v>2</v>
+        <v>2.2678384634424416</v>
       </c>
       <c r="CY35">
         <f t="array" ref="CY35">SQRT(SUM((CY$2:CY$33-$I$2:$I$33)^2))</f>
-        <v>1.4142135623730951</v>
+        <v>1.1641655519207657</v>
       </c>
       <c r="CZ35">
         <f t="array" ref="CZ35">SQRT(SUM((CZ$2:CZ$33-$I$2:$I$33)^2))</f>
-        <v>1</v>
+        <v>1.5055612231116087</v>
       </c>
       <c r="DA35">
         <f t="array" ref="DA35">SQRT(SUM((DA$2:DA$33-$I$2:$I$33)^2))</f>
-        <v>1.4142135623730951</v>
+        <v>1.0303571428678142</v>
       </c>
       <c r="DB35">
         <f t="array" ref="DB35">SQRT(SUM((DB$2:DB$33-$I$2:$I$33)^2))</f>
-        <v>2</v>
+        <v>2.0065752807015222</v>
       </c>
       <c r="DC35">
         <f t="array" ref="DC35">SQRT(SUM((DC$2:DC$33-$I$2:$I$33)^2))</f>
-        <v>1.7320508075688772</v>
+        <v>1.855867174066697</v>
       </c>
       <c r="DD35">
         <f t="array" ref="DD35">SQRT(SUM((DD$2:DD$33-$I$2:$I$33)^2))</f>
-        <v>1.4142135623730951</v>
+        <v>1.1818161081579406</v>
       </c>
       <c r="DE35">
         <f t="array" ref="DE35">SQRT(SUM((DE$2:DE$33-$I$2:$I$33)^2))</f>
-        <v>2</v>
+        <v>2.254120436481895</v>
       </c>
       <c r="DF35">
         <f t="array" ref="DF35">SQRT(SUM((DF$2:DF$33-$I$2:$I$33)^2))</f>
-        <v>2</v>
+        <v>2.2741951842497512</v>
       </c>
       <c r="DG35">
         <f t="array" ref="DG35">SQRT(SUM((DG$2:DG$33-$I$2:$I$33)^2))</f>
-        <v>2.4494897427831779</v>
-      </c>
-    </row>
-    <row r="36" spans="1:113" x14ac:dyDescent="0.2">
+        <v>2.6687467608278417</v>
+      </c>
+    </row>
+    <row r="36" spans="1:112" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <f>SUM(L38:DG38)</f>
+        <v>140.57239116463089</v>
+      </c>
       <c r="G36" t="s">
         <v>151</v>
       </c>
       <c r="L36">
         <f t="array" ref="L36">SQRT(SUM((L$2:L$33-$J$2:$J$33)^2))</f>
-        <v>1.7320508075688772</v>
+        <v>2.011523544569104</v>
       </c>
       <c r="M36">
         <f t="array" ref="M36">SQRT(SUM((M$2:M$33-$J$2:$J$33)^2))</f>
-        <v>1.4142135623730951</v>
+        <v>1.7401626605072489</v>
       </c>
       <c r="N36">
         <f t="array" ref="N36">SQRT(SUM((N$2:N$33-$J$2:$J$33)^2))</f>
-        <v>1.4142135623730951</v>
+        <v>1.8505535387319252</v>
       </c>
       <c r="O36">
         <f t="array" ref="O36">SQRT(SUM((O$2:O$33-$J$2:$J$33)^2))</f>
-        <v>1.4142135623730951</v>
+        <v>1.7073235933241819</v>
       </c>
       <c r="P36">
         <f t="array" ref="P36">SQRT(SUM((P$2:P$33-$J$2:$J$33)^2))</f>
-        <v>2</v>
+        <v>2.0516343565591169</v>
       </c>
       <c r="Q36">
         <f t="array" ref="Q36">SQRT(SUM((Q$2:Q$33-$J$2:$J$33)^2))</f>
-        <v>2</v>
+        <v>1.5921595054427398</v>
       </c>
       <c r="R36">
         <f t="array" ref="R36">SQRT(SUM((R$2:R$33-$J$2:$J$33)^2))</f>
-        <v>2</v>
+        <v>2.2794831493147703</v>
       </c>
       <c r="S36">
         <f t="array" ref="S36">SQRT(SUM((S$2:S$33-$J$2:$J$33)^2))</f>
-        <v>1.4142135623730951</v>
+        <v>1.7944174200994996</v>
       </c>
       <c r="T36">
         <f t="array" ref="T36">SQRT(SUM((T$2:T$33-$J$2:$J$33)^2))</f>
-        <v>2</v>
+        <v>1.5208875459717481</v>
       </c>
       <c r="U36">
         <f t="array" ref="U36">SQRT(SUM((U$2:U$33-$J$2:$J$33)^2))</f>
-        <v>1.7320508075688772</v>
+        <v>1.9743939193358322</v>
       </c>
       <c r="V36">
         <f t="array" ref="V36">SQRT(SUM((V$2:V$33-$J$2:$J$33)^2))</f>
-        <v>2.2360679774997898</v>
+        <v>1.8449582254873356</v>
       </c>
       <c r="W36">
         <f t="array" ref="W36">SQRT(SUM((W$2:W$33-$J$2:$J$33)^2))</f>
-        <v>1.7320508075688772</v>
+        <v>2.0562899966513304</v>
       </c>
       <c r="X36">
         <f t="array" ref="X36">SQRT(SUM((X$2:X$33-$J$2:$J$33)^2))</f>
-        <v>2</v>
+        <v>2.2083544750859794</v>
       </c>
       <c r="Y36">
         <f t="array" ref="Y36">SQRT(SUM((Y$2:Y$33-$J$2:$J$33)^2))</f>
-        <v>2</v>
+        <v>1.9743257645296075</v>
       </c>
       <c r="Z36">
         <f t="array" ref="Z36">SQRT(SUM((Z$2:Z$33-$J$2:$J$33)^2))</f>
-        <v>1.4142135623730951</v>
+        <v>1.6238974603421548</v>
       </c>
       <c r="AA36">
         <f t="array" ref="AA36">SQRT(SUM((AA$2:AA$33-$J$2:$J$33)^2))</f>
-        <v>1.4142135623730951</v>
+        <v>1.8505535387319252</v>
       </c>
       <c r="AB36">
         <f t="array" ref="AB36">SQRT(SUM((AB$2:AB$33-$J$2:$J$33)^2))</f>
-        <v>2</v>
+        <v>2.2402232875393246</v>
       </c>
       <c r="AC36">
         <f t="array" ref="AC36">SQRT(SUM((AC$2:AC$33-$J$2:$J$33)^2))</f>
-        <v>2</v>
+        <v>2.2794831493147703</v>
       </c>
       <c r="AD36">
         <f t="array" ref="AD36">SQRT(SUM((AD$2:AD$33-$J$2:$J$33)^2))</f>
-        <v>1.4142135623730951</v>
+        <v>1.7734855509052923</v>
       </c>
       <c r="AE36">
         <f t="array" ref="AE36">SQRT(SUM((AE$2:AE$33-$J$2:$J$33)^2))</f>
-        <v>1.7320508075688772</v>
+        <v>1.4842777331826831</v>
       </c>
       <c r="AF36">
         <f t="array" ref="AF36">SQRT(SUM((AF$2:AF$33-$J$2:$J$33)^2))</f>
-        <v>2</v>
+        <v>2.1434789180650125</v>
       </c>
       <c r="AG36">
         <f t="array" ref="AG36">SQRT(SUM((AG$2:AG$33-$J$2:$J$33)^2))</f>
-        <v>1.4142135623730951</v>
+        <v>1.7168708539712532</v>
       </c>
       <c r="AH36">
         <f t="array" ref="AH36">SQRT(SUM((AH$2:AH$33-$J$2:$J$33)^2))</f>
-        <v>1.4142135623730951</v>
+        <v>1.1365209354554062</v>
       </c>
       <c r="AI36">
         <f t="array" ref="AI36">SQRT(SUM((AI$2:AI$33-$J$2:$J$33)^2))</f>
-        <v>2.6457513110645907</v>
+        <v>2.0739834611338597</v>
       </c>
       <c r="AJ36">
         <f t="array" ref="AJ36">SQRT(SUM((AJ$2:AJ$33-$J$2:$J$33)^2))</f>
-        <v>1.4142135623730951</v>
+        <v>1.8632755933390883</v>
       </c>
       <c r="AK36">
         <f t="array" ref="AK36">SQRT(SUM((AK$2:AK$33-$J$2:$J$33)^2))</f>
-        <v>2.2360679774997898</v>
+        <v>1.8649217727445708</v>
       </c>
       <c r="AL36">
         <f t="array" ref="AL36">SQRT(SUM((AL$2:AL$33-$J$2:$J$33)^2))</f>
-        <v>1.4142135623730951</v>
+        <v>1.7131364475600259</v>
       </c>
       <c r="AM36">
         <f t="array" ref="AM36">SQRT(SUM((AM$2:AM$33-$J$2:$J$33)^2))</f>
-        <v>2</v>
+        <v>2.1606865712538119</v>
       </c>
       <c r="AN36">
         <f t="array" ref="AN36">SQRT(SUM((AN$2:AN$33-$J$2:$J$33)^2))</f>
-        <v>1.4142135623730951</v>
+        <v>1.6192263413489665</v>
       </c>
       <c r="AO36">
         <f t="array" ref="AO36">SQRT(SUM((AO$2:AO$33-$J$2:$J$33)^2))</f>
-        <v>1.7320508075688772</v>
+        <v>2.0548275360318278</v>
       </c>
       <c r="AP36">
         <f t="array" ref="AP36">SQRT(SUM((AP$2:AP$33-$J$2:$J$33)^2))</f>
-        <v>1</v>
+        <v>1.5143864127524536</v>
       </c>
       <c r="AQ36">
         <f t="array" ref="AQ36">SQRT(SUM((AQ$2:AQ$33-$J$2:$J$33)^2))</f>
-        <v>2</v>
+        <v>2.1196933044697963</v>
       </c>
       <c r="AR36">
         <f t="array" ref="AR36">SQRT(SUM((AR$2:AR$33-$J$2:$J$33)^2))</f>
-        <v>1.4142135623730951</v>
+        <v>1.0275018965942826</v>
       </c>
       <c r="AS36">
         <f t="array" ref="AS36">SQRT(SUM((AS$2:AS$33-$J$2:$J$33)^2))</f>
-        <v>2.4494897427831779</v>
+        <v>2.0126299093315407</v>
       </c>
       <c r="AT36">
         <f t="array" ref="AT36">SQRT(SUM((AT$2:AT$33-$J$2:$J$33)^2))</f>
-        <v>1.4142135623730951</v>
+        <v>1.8480863564203511</v>
       </c>
       <c r="AU36">
         <f t="array" ref="AU36">SQRT(SUM((AU$2:AU$33-$J$2:$J$33)^2))</f>
-        <v>2</v>
+        <v>2.1766529664527945</v>
       </c>
       <c r="AV36">
         <f t="array" ref="AV36">SQRT(SUM((AV$2:AV$33-$J$2:$J$33)^2))</f>
-        <v>1.7320508075688772</v>
+        <v>1.3602666557863698</v>
       </c>
       <c r="AW36">
         <f t="array" ref="AW36">SQRT(SUM((AW$2:AW$33-$J$2:$J$33)^2))</f>
-        <v>2.2360679774997898</v>
+        <v>2.3607414113178766</v>
       </c>
       <c r="AX36">
         <f t="array" ref="AX36">SQRT(SUM((AX$2:AX$33-$J$2:$J$33)^2))</f>
-        <v>2.2360679774997898</v>
+        <v>1.7947158314725244</v>
       </c>
       <c r="AY36">
         <f t="array" ref="AY36">SQRT(SUM((AY$2:AY$33-$J$2:$J$33)^2))</f>
-        <v>2.2360679774997898</v>
+        <v>2.3432452892960676</v>
       </c>
       <c r="AZ36">
         <f t="array" ref="AZ36">SQRT(SUM((AZ$2:AZ$33-$J$2:$J$33)^2))</f>
-        <v>1.4142135623730951</v>
+        <v>1.8505535387319252</v>
       </c>
       <c r="BA36">
         <f t="array" ref="BA36">SQRT(SUM((BA$2:BA$33-$J$2:$J$33)^2))</f>
-        <v>1.7320508075688772</v>
+        <v>2.0957727160631965</v>
       </c>
       <c r="BB36">
         <f t="array" ref="BB36">SQRT(SUM((BB$2:BB$33-$J$2:$J$33)^2))</f>
-        <v>1</v>
+        <v>1.4955455129041146</v>
       </c>
       <c r="BC36">
         <f t="array" ref="BC36">SQRT(SUM((BC$2:BC$33-$J$2:$J$33)^2))</f>
-        <v>2</v>
+        <v>2.0500140238412112</v>
       </c>
       <c r="BD36">
         <f t="array" ref="BD36">SQRT(SUM((BD$2:BD$33-$J$2:$J$33)^2))</f>
-        <v>2</v>
+        <v>2.2707306783337655</v>
       </c>
       <c r="BE36">
         <f t="array" ref="BE36">SQRT(SUM((BE$2:BE$33-$J$2:$J$33)^2))</f>
-        <v>2.2360679774997898</v>
+        <v>1.7524115185051239</v>
       </c>
       <c r="BF36">
         <f t="array" ref="BF36">SQRT(SUM((BF$2:BF$33-$J$2:$J$33)^2))</f>
-        <v>1.7320508075688772</v>
+        <v>1.9003221768427176</v>
       </c>
       <c r="BG36">
         <f t="array" ref="BG36">SQRT(SUM((BG$2:BG$33-$J$2:$J$33)^2))</f>
-        <v>1.7320508075688772</v>
+        <v>1.9177418630161644</v>
       </c>
       <c r="BH36">
         <f t="array" ref="BH36">SQRT(SUM((BH$2:BH$33-$J$2:$J$33)^2))</f>
-        <v>2.2360679774997898</v>
+        <v>2.2820594468854214</v>
       </c>
       <c r="BI36">
         <f t="array" ref="BI36">SQRT(SUM((BI$2:BI$33-$J$2:$J$33)^2))</f>
-        <v>1.7320508075688772</v>
+        <v>1.9263943765070479</v>
       </c>
       <c r="BJ36">
         <f t="array" ref="BJ36">SQRT(SUM((BJ$2:BJ$33-$J$2:$J$33)^2))</f>
-        <v>1.7320508075688772</v>
+        <v>2.013587689905751</v>
       </c>
       <c r="BK36">
         <f t="array" ref="BK36">SQRT(SUM((BK$2:BK$33-$J$2:$J$33)^2))</f>
-        <v>2.6457513110645907</v>
+        <v>2.1154635137735829</v>
       </c>
       <c r="BL36">
         <f t="array" ref="BL36">SQRT(SUM((BL$2:BL$33-$J$2:$J$33)^2))</f>
-        <v>1.4142135623730951</v>
+        <v>1.7227793322988796</v>
       </c>
       <c r="BM36">
         <f t="array" ref="BM36">SQRT(SUM((BM$2:BM$33-$J$2:$J$33)^2))</f>
-        <v>1.4142135623730951</v>
+        <v>1.8632755933390883</v>
       </c>
       <c r="BN36">
         <f t="array" ref="BN36">SQRT(SUM((BN$2:BN$33-$J$2:$J$33)^2))</f>
-        <v>2.4494897427831779</v>
+        <v>1.9117132267131365</v>
       </c>
       <c r="BO36">
         <f t="array" ref="BO36">SQRT(SUM((BO$2:BO$33-$J$2:$J$33)^2))</f>
-        <v>1.4142135623730951</v>
+        <v>1.7944174200994996</v>
       </c>
       <c r="BP36">
         <f t="array" ref="BP36">SQRT(SUM((BP$2:BP$33-$J$2:$J$33)^2))</f>
-        <v>1.7320508075688772</v>
+        <v>2.0957727160631965</v>
       </c>
       <c r="BQ36">
         <f t="array" ref="BQ36">SQRT(SUM((BQ$2:BQ$33-$J$2:$J$33)^2))</f>
-        <v>1.4142135623730951</v>
+        <v>1.757251101712169</v>
       </c>
       <c r="BR36">
         <f t="array" ref="BR36">SQRT(SUM((BR$2:BR$33-$J$2:$J$33)^2))</f>
-        <v>1.4142135623730951</v>
+        <v>1.7501284164217605</v>
       </c>
       <c r="BS36">
         <f t="array" ref="BS36">SQRT(SUM((BS$2:BS$33-$J$2:$J$33)^2))</f>
-        <v>2</v>
+        <v>1.9463996811904845</v>
       </c>
       <c r="BT36">
         <f t="array" ref="BT36">SQRT(SUM((BT$2:BT$33-$J$2:$J$33)^2))</f>
-        <v>1.4142135623730951</v>
+        <v>1.622628667947811</v>
       </c>
       <c r="BU36">
         <f t="array" ref="BU36">SQRT(SUM((BU$2:BU$33-$J$2:$J$33)^2))</f>
-        <v>1</v>
+        <v>1.4955455129041146</v>
       </c>
       <c r="BV36">
         <f t="array" ref="BV36">SQRT(SUM((BV$2:BV$33-$J$2:$J$33)^2))</f>
-        <v>2.2360679774997898</v>
+        <v>2.2788416131684555</v>
       </c>
       <c r="BW36">
         <f t="array" ref="BW36">SQRT(SUM((BW$2:BW$33-$J$2:$J$33)^2))</f>
-        <v>1.4142135623730951</v>
+        <v>1.7501284164217605</v>
       </c>
       <c r="BX36">
         <f t="array" ref="BX36">SQRT(SUM((BX$2:BX$33-$J$2:$J$33)^2))</f>
-        <v>2</v>
+        <v>2.1777275986299802</v>
       </c>
       <c r="BY36">
         <f t="array" ref="BY36">SQRT(SUM((BY$2:BY$33-$J$2:$J$33)^2))</f>
-        <v>2.4494897427831779</v>
+        <v>2.5025156752530817</v>
       </c>
       <c r="BZ36">
         <f t="array" ref="BZ36">SQRT(SUM((BZ$2:BZ$33-$J$2:$J$33)^2))</f>
-        <v>1.4142135623730951</v>
+        <v>1.8632755933390883</v>
       </c>
       <c r="CA36">
         <f t="array" ref="CA36">SQRT(SUM((CA$2:CA$33-$J$2:$J$33)^2))</f>
-        <v>1</v>
+        <v>1.5734535507199139</v>
       </c>
       <c r="CB36">
         <f t="array" ref="CB36">SQRT(SUM((CB$2:CB$33-$J$2:$J$33)^2))</f>
-        <v>2</v>
+        <v>1.4597253032360544</v>
       </c>
       <c r="CC36">
         <f t="array" ref="CC36">SQRT(SUM((CC$2:CC$33-$J$2:$J$33)^2))</f>
-        <v>1</v>
+        <v>1.5222276232467067</v>
       </c>
       <c r="CD36">
         <f t="array" ref="CD36">SQRT(SUM((CD$2:CD$33-$J$2:$J$33)^2))</f>
-        <v>1.4142135623730951</v>
+        <v>1.7698996323003826</v>
       </c>
       <c r="CE36">
         <f t="array" ref="CE36">SQRT(SUM((CE$2:CE$33-$J$2:$J$33)^2))</f>
-        <v>1.4142135623730951</v>
+        <v>1.7768053173685672</v>
       </c>
       <c r="CF36">
         <f t="array" ref="CF36">SQRT(SUM((CF$2:CF$33-$J$2:$J$33)^2))</f>
-        <v>1.7320508075688772</v>
+        <v>1.293803272689326</v>
       </c>
       <c r="CG36">
         <f t="array" ref="CG36">SQRT(SUM((CG$2:CG$33-$J$2:$J$33)^2))</f>
-        <v>1.4142135623730951</v>
+        <v>1.7872722731064923</v>
       </c>
       <c r="CH36">
         <f t="array" ref="CH36">SQRT(SUM((CH$2:CH$33-$J$2:$J$33)^2))</f>
-        <v>1</v>
+        <v>1.3583456354079493</v>
       </c>
       <c r="CI36">
         <f t="array" ref="CI36">SQRT(SUM((CI$2:CI$33-$J$2:$J$33)^2))</f>
-        <v>1.4142135623730951</v>
+        <v>1.8101501881109636</v>
       </c>
       <c r="CJ36">
         <f t="array" ref="CJ36">SQRT(SUM((CJ$2:CJ$33-$J$2:$J$33)^2))</f>
-        <v>1.4142135623730951</v>
+        <v>1.8068296402720527</v>
       </c>
       <c r="CK36">
         <f t="array" ref="CK36">SQRT(SUM((CK$2:CK$33-$J$2:$J$33)^2))</f>
-        <v>2.4494897427831779</v>
+        <v>2.0506329637317542</v>
       </c>
       <c r="CL36">
         <f t="array" ref="CL36">SQRT(SUM((CL$2:CL$33-$J$2:$J$33)^2))</f>
-        <v>1.4142135623730951</v>
+        <v>1.8076577756301491</v>
       </c>
       <c r="CM36">
         <f t="array" ref="CM36">SQRT(SUM((CM$2:CM$33-$J$2:$J$33)^2))</f>
-        <v>1</v>
+        <v>1.5687106802564197</v>
       </c>
       <c r="CN36">
         <f t="array" ref="CN36">SQRT(SUM((CN$2:CN$33-$J$2:$J$33)^2))</f>
-        <v>2.6457513110645907</v>
+        <v>2.3323336922990845</v>
       </c>
       <c r="CO36">
         <f t="array" ref="CO36">SQRT(SUM((CO$2:CO$33-$J$2:$J$33)^2))</f>
-        <v>3</v>
+        <v>2.8706585629453918</v>
       </c>
       <c r="CP36">
         <f t="array" ref="CP36">SQRT(SUM((CP$2:CP$33-$J$2:$J$33)^2))</f>
-        <v>1.7320508075688772</v>
+        <v>1.8892333503090244</v>
       </c>
       <c r="CQ36">
         <f t="array" ref="CQ36">SQRT(SUM((CQ$2:CQ$33-$J$2:$J$33)^2))</f>
-        <v>1.4142135623730951</v>
+        <v>1.8187526521400736</v>
       </c>
       <c r="CR36">
         <f t="array" ref="CR36">SQRT(SUM((CR$2:CR$33-$J$2:$J$33)^2))</f>
-        <v>1.7320508075688772</v>
+        <v>1.9599799801907916</v>
       </c>
       <c r="CS36">
         <f t="array" ref="CS36">SQRT(SUM((CS$2:CS$33-$J$2:$J$33)^2))</f>
-        <v>1.7320508075688772</v>
+        <v>2.0288495486791516</v>
       </c>
       <c r="CT36">
         <f t="array" ref="CT36">SQRT(SUM((CT$2:CT$33-$J$2:$J$33)^2))</f>
-        <v>2</v>
+        <v>2.1907093188728424</v>
       </c>
       <c r="CU36">
         <f t="array" ref="CU36">SQRT(SUM((CU$2:CU$33-$J$2:$J$33)^2))</f>
-        <v>2.4494897427831779</v>
+        <v>2.3831355525478557</v>
       </c>
       <c r="CV36">
         <f t="array" ref="CV36">SQRT(SUM((CV$2:CV$33-$J$2:$J$33)^2))</f>
-        <v>2</v>
+        <v>2.1756577930627352</v>
       </c>
       <c r="CW36">
         <f t="array" ref="CW36">SQRT(SUM((CW$2:CW$33-$J$2:$J$33)^2))</f>
-        <v>1</v>
+        <v>1.4955455129041146</v>
       </c>
       <c r="CX36">
         <f t="array" ref="CX36">SQRT(SUM((CX$2:CX$33-$J$2:$J$33)^2))</f>
-        <v>2</v>
+        <v>1.9427532139293726</v>
       </c>
       <c r="CY36">
         <f t="array" ref="CY36">SQRT(SUM((CY$2:CY$33-$J$2:$J$33)^2))</f>
-        <v>1.4142135623730951</v>
+        <v>1.8505781056642001</v>
       </c>
       <c r="CZ36">
         <f t="array" ref="CZ36">SQRT(SUM((CZ$2:CZ$33-$J$2:$J$33)^2))</f>
-        <v>1</v>
+        <v>1.4921179348189135</v>
       </c>
       <c r="DA36">
         <f t="array" ref="DA36">SQRT(SUM((DA$2:DA$33-$J$2:$J$33)^2))</f>
-        <v>1.4142135623730951</v>
+        <v>1.8101501881109636</v>
       </c>
       <c r="DB36">
         <f t="array" ref="DB36">SQRT(SUM((DB$2:DB$33-$J$2:$J$33)^2))</f>
-        <v>2</v>
+        <v>1.6391740112686677</v>
       </c>
       <c r="DC36">
         <f t="array" ref="DC36">SQRT(SUM((DC$2:DC$33-$J$2:$J$33)^2))</f>
-        <v>1.7320508075688772</v>
+        <v>1.3365566457539797</v>
       </c>
       <c r="DD36">
         <f t="array" ref="DD36">SQRT(SUM((DD$2:DD$33-$J$2:$J$33)^2))</f>
-        <v>1.4142135623730951</v>
+        <v>1.6906342083253205</v>
       </c>
       <c r="DE36">
         <f t="array" ref="DE36">SQRT(SUM((DE$2:DE$33-$J$2:$J$33)^2))</f>
-        <v>2</v>
+        <v>1.9872074643567683</v>
       </c>
       <c r="DF36">
         <f t="array" ref="DF36">SQRT(SUM((DF$2:DF$33-$J$2:$J$33)^2))</f>
-        <v>2</v>
+        <v>2.0726403083292615</v>
       </c>
       <c r="DG36">
         <f t="array" ref="DG36">SQRT(SUM((DG$2:DG$33-$J$2:$J$33)^2))</f>
-        <v>2.4494897427831779</v>
-      </c>
-    </row>
-    <row r="37" spans="1:113" x14ac:dyDescent="0.2">
+        <v>1.9581991487158106</v>
+      </c>
+    </row>
+    <row r="37" spans="1:112" x14ac:dyDescent="0.2">
       <c r="G37" t="s">
         <v>152</v>
       </c>
       <c r="L37">
         <f t="array" ref="L37">SQRT(SUM((L$2:L$33-$K$2:$K$33)^2))</f>
-        <v>1.7320508075688772</v>
+        <v>2.1838070898110593</v>
       </c>
       <c r="M37">
         <f t="array" ref="M37">SQRT(SUM((M$2:M$33-$K$2:$K$33)^2))</f>
-        <v>1.4142135623730951</v>
+        <v>1.9554356546711469</v>
       </c>
       <c r="N37">
         <f t="array" ref="N37">SQRT(SUM((N$2:N$33-$K$2:$K$33)^2))</f>
-        <v>1.4142135623730951</v>
+        <v>0.70900168934275176</v>
       </c>
       <c r="O37">
         <f t="array" ref="O37">SQRT(SUM((O$2:O$33-$K$2:$K$33)^2))</f>
-        <v>1.4142135623730951</v>
+        <v>1.9381331682418139</v>
       </c>
       <c r="P37">
         <f t="array" ref="P37">SQRT(SUM((P$2:P$33-$K$2:$K$33)^2))</f>
-        <v>2</v>
+        <v>2.3439550510639919</v>
       </c>
       <c r="Q37">
         <f t="array" ref="Q37">SQRT(SUM((Q$2:Q$33-$K$2:$K$33)^2))</f>
-        <v>2</v>
+        <v>2.3618173511102047</v>
       </c>
       <c r="R37">
         <f t="array" ref="R37">SQRT(SUM((R$2:R$33-$K$2:$K$33)^2))</f>
-        <v>2</v>
+        <v>0.86185981890530861</v>
       </c>
       <c r="S37">
         <f t="array" ref="S37">SQRT(SUM((S$2:S$33-$K$2:$K$33)^2))</f>
-        <v>1.4142135623730951</v>
+        <v>1.9641775478181567</v>
       </c>
       <c r="T37">
         <f t="array" ref="T37">SQRT(SUM((T$2:T$33-$K$2:$K$33)^2))</f>
-        <v>2</v>
+        <v>2.405897521001175</v>
       </c>
       <c r="U37">
         <f t="array" ref="U37">SQRT(SUM((U$2:U$33-$K$2:$K$33)^2))</f>
-        <v>1.7320508075688772</v>
+        <v>2.1783275893889646</v>
       </c>
       <c r="V37">
         <f t="array" ref="V37">SQRT(SUM((V$2:V$33-$K$2:$K$33)^2))</f>
-        <v>2.2360679774997898</v>
+        <v>2.5931160387298795</v>
       </c>
       <c r="W37">
         <f t="array" ref="W37">SQRT(SUM((W$2:W$33-$K$2:$K$33)^2))</f>
-        <v>1.7320508075688772</v>
+        <v>0.93285478658924037</v>
       </c>
       <c r="X37">
         <f t="array" ref="X37">SQRT(SUM((X$2:X$33-$K$2:$K$33)^2))</f>
-        <v>2</v>
+        <v>2.3798219632309996</v>
       </c>
       <c r="Y37">
         <f t="array" ref="Y37">SQRT(SUM((Y$2:Y$33-$K$2:$K$33)^2))</f>
-        <v>2</v>
+        <v>2.3727929907886258</v>
       </c>
       <c r="Z37">
         <f t="array" ref="Z37">SQRT(SUM((Z$2:Z$33-$K$2:$K$33)^2))</f>
-        <v>1.4142135623730951</v>
+        <v>1.9549712136551982</v>
       </c>
       <c r="AA37">
         <f t="array" ref="AA37">SQRT(SUM((AA$2:AA$33-$K$2:$K$33)^2))</f>
-        <v>1.4142135623730951</v>
+        <v>0.70900168934275176</v>
       </c>
       <c r="AB37">
         <f t="array" ref="AB37">SQRT(SUM((AB$2:AB$33-$K$2:$K$33)^2))</f>
-        <v>2</v>
+        <v>2.3913201013806873</v>
       </c>
       <c r="AC37">
         <f t="array" ref="AC37">SQRT(SUM((AC$2:AC$33-$K$2:$K$33)^2))</f>
-        <v>2</v>
+        <v>0.86185981890530861</v>
       </c>
       <c r="AD37">
         <f t="array" ref="AD37">SQRT(SUM((AD$2:AD$33-$K$2:$K$33)^2))</f>
-        <v>1.4142135623730951</v>
+        <v>1.960724044132893</v>
       </c>
       <c r="AE37">
         <f t="array" ref="AE37">SQRT(SUM((AE$2:AE$33-$K$2:$K$33)^2))</f>
-        <v>1.7320508075688772</v>
+        <v>2.2014866223217724</v>
       </c>
       <c r="AF37">
         <f t="array" ref="AF37">SQRT(SUM((AF$2:AF$33-$K$2:$K$33)^2))</f>
-        <v>2</v>
+        <v>2.3921756420627021</v>
       </c>
       <c r="AG37">
         <f t="array" ref="AG37">SQRT(SUM((AG$2:AG$33-$K$2:$K$33)^2))</f>
-        <v>1.4142135623730951</v>
+        <v>1.9539522663357627</v>
       </c>
       <c r="AH37">
         <f t="array" ref="AH37">SQRT(SUM((AH$2:AH$33-$K$2:$K$33)^2))</f>
-        <v>1.4142135623730951</v>
+        <v>1.9547400548741349</v>
       </c>
       <c r="AI37">
         <f t="array" ref="AI37">SQRT(SUM((AI$2:AI$33-$K$2:$K$33)^2))</f>
-        <v>2.6457513110645907</v>
+        <v>2.8283717911246815</v>
       </c>
       <c r="AJ37">
         <f t="array" ref="AJ37">SQRT(SUM((AJ$2:AJ$33-$K$2:$K$33)^2))</f>
-        <v>1.4142135623730951</v>
+        <v>0.94199774617436449</v>
       </c>
       <c r="AK37">
         <f t="array" ref="AK37">SQRT(SUM((AK$2:AK$33-$K$2:$K$33)^2))</f>
-        <v>2.2360679774997898</v>
+        <v>2.6025484666597456</v>
       </c>
       <c r="AL37">
         <f t="array" ref="AL37">SQRT(SUM((AL$2:AL$33-$K$2:$K$33)^2))</f>
-        <v>1.4142135623730951</v>
+        <v>1.9584798898243243</v>
       </c>
       <c r="AM37">
         <f t="array" ref="AM37">SQRT(SUM((AM$2:AM$33-$K$2:$K$33)^2))</f>
-        <v>2</v>
+        <v>2.40194602431544</v>
       </c>
       <c r="AN37">
         <f t="array" ref="AN37">SQRT(SUM((AN$2:AN$33-$K$2:$K$33)^2))</f>
-        <v>1.4142135623730951</v>
+        <v>1.9326155628043158</v>
       </c>
       <c r="AO37">
         <f t="array" ref="AO37">SQRT(SUM((AO$2:AO$33-$K$2:$K$33)^2))</f>
-        <v>1.7320508075688772</v>
+        <v>1.8305699297675186</v>
       </c>
       <c r="AP37">
         <f t="array" ref="AP37">SQRT(SUM((AP$2:AP$33-$K$2:$K$33)^2))</f>
-        <v>1</v>
+        <v>1.6710839668209934</v>
       </c>
       <c r="AQ37">
         <f t="array" ref="AQ37">SQRT(SUM((AQ$2:AQ$33-$K$2:$K$33)^2))</f>
-        <v>2</v>
+        <v>2.3750514338638071</v>
       </c>
       <c r="AR37">
         <f t="array" ref="AR37">SQRT(SUM((AR$2:AR$33-$K$2:$K$33)^2))</f>
-        <v>1.4142135623730951</v>
+        <v>1.9592208480269013</v>
       </c>
       <c r="AS37">
         <f t="array" ref="AS37">SQRT(SUM((AS$2:AS$33-$K$2:$K$33)^2))</f>
-        <v>2.4494897427831779</v>
+        <v>2.757943597805574</v>
       </c>
       <c r="AT37">
         <f t="array" ref="AT37">SQRT(SUM((AT$2:AT$33-$K$2:$K$33)^2))</f>
-        <v>1.4142135623730951</v>
+        <v>1.9683565190671788</v>
       </c>
       <c r="AU37">
         <f t="array" ref="AU37">SQRT(SUM((AU$2:AU$33-$K$2:$K$33)^2))</f>
-        <v>2</v>
+        <v>2.3824561281214462</v>
       </c>
       <c r="AV37">
         <f t="array" ref="AV37">SQRT(SUM((AV$2:AV$33-$K$2:$K$33)^2))</f>
-        <v>1.7320508075688772</v>
+        <v>2.1968183330572222</v>
       </c>
       <c r="AW37">
         <f t="array" ref="AW37">SQRT(SUM((AW$2:AW$33-$K$2:$K$33)^2))</f>
-        <v>2.2360679774997898</v>
+        <v>2.5770032581395022</v>
       </c>
       <c r="AX37">
         <f t="array" ref="AX37">SQRT(SUM((AX$2:AX$33-$K$2:$K$33)^2))</f>
-        <v>2.2360679774997898</v>
+        <v>2.4785712964482287</v>
       </c>
       <c r="AY37">
         <f t="array" ref="AY37">SQRT(SUM((AY$2:AY$33-$K$2:$K$33)^2))</f>
-        <v>2.2360679774997898</v>
+        <v>2.5645213026753595</v>
       </c>
       <c r="AZ37">
         <f t="array" ref="AZ37">SQRT(SUM((AZ$2:AZ$33-$K$2:$K$33)^2))</f>
-        <v>1.4142135623730951</v>
+        <v>0.70900168934275176</v>
       </c>
       <c r="BA37">
         <f t="array" ref="BA37">SQRT(SUM((BA$2:BA$33-$K$2:$K$33)^2))</f>
-        <v>1.7320508075688772</v>
+        <v>0.61259096473251229</v>
       </c>
       <c r="BB37">
         <f t="array" ref="BB37">SQRT(SUM((BB$2:BB$33-$K$2:$K$33)^2))</f>
-        <v>1</v>
+        <v>1.693883859802336</v>
       </c>
       <c r="BC37">
         <f t="array" ref="BC37">SQRT(SUM((BC$2:BC$33-$K$2:$K$33)^2))</f>
-        <v>2</v>
+        <v>2.3795320779202287</v>
       </c>
       <c r="BD37">
         <f t="array" ref="BD37">SQRT(SUM((BD$2:BD$33-$K$2:$K$33)^2))</f>
-        <v>2</v>
+        <v>2.3715582749053379</v>
       </c>
       <c r="BE37">
         <f t="array" ref="BE37">SQRT(SUM((BE$2:BE$33-$K$2:$K$33)^2))</f>
-        <v>2.2360679774997898</v>
+        <v>2.5879615481791425</v>
       </c>
       <c r="BF37">
         <f t="array" ref="BF37">SQRT(SUM((BF$2:BF$33-$K$2:$K$33)^2))</f>
-        <v>1.7320508075688772</v>
+        <v>2.17571905208922</v>
       </c>
       <c r="BG37">
         <f t="array" ref="BG37">SQRT(SUM((BG$2:BG$33-$K$2:$K$33)^2))</f>
-        <v>1.7320508075688772</v>
+        <v>2.1508436564249971</v>
       </c>
       <c r="BH37">
         <f t="array" ref="BH37">SQRT(SUM((BH$2:BH$33-$K$2:$K$33)^2))</f>
-        <v>2.2360679774997898</v>
+        <v>2.5951827254975877</v>
       </c>
       <c r="BI37">
         <f t="array" ref="BI37">SQRT(SUM((BI$2:BI$33-$K$2:$K$33)^2))</f>
-        <v>1.7320508075688772</v>
+        <v>2.054126508398515</v>
       </c>
       <c r="BJ37">
         <f t="array" ref="BJ37">SQRT(SUM((BJ$2:BJ$33-$K$2:$K$33)^2))</f>
-        <v>1.7320508075688772</v>
+        <v>2.2045176506556641</v>
       </c>
       <c r="BK37">
         <f t="array" ref="BK37">SQRT(SUM((BK$2:BK$33-$K$2:$K$33)^2))</f>
-        <v>2.6457513110645907</v>
+        <v>2.9124484824510941</v>
       </c>
       <c r="BL37">
         <f t="array" ref="BL37">SQRT(SUM((BL$2:BL$33-$K$2:$K$33)^2))</f>
-        <v>1.4142135623730951</v>
+        <v>1.7987114869503882</v>
       </c>
       <c r="BM37">
         <f t="array" ref="BM37">SQRT(SUM((BM$2:BM$33-$K$2:$K$33)^2))</f>
-        <v>1.4142135623730951</v>
+        <v>0.94199774617436449</v>
       </c>
       <c r="BN37">
         <f t="array" ref="BN37">SQRT(SUM((BN$2:BN$33-$K$2:$K$33)^2))</f>
-        <v>2.4494897427831779</v>
+        <v>2.7525690071546456</v>
       </c>
       <c r="BO37">
         <f t="array" ref="BO37">SQRT(SUM((BO$2:BO$33-$K$2:$K$33)^2))</f>
-        <v>1.4142135623730951</v>
+        <v>1.9641775478181567</v>
       </c>
       <c r="BP37">
         <f t="array" ref="BP37">SQRT(SUM((BP$2:BP$33-$K$2:$K$33)^2))</f>
-        <v>1.7320508075688772</v>
+        <v>0.61259096473251229</v>
       </c>
       <c r="BQ37">
         <f t="array" ref="BQ37">SQRT(SUM((BQ$2:BQ$33-$K$2:$K$33)^2))</f>
-        <v>1.4142135623730951</v>
+        <v>1.9442186300103312</v>
       </c>
       <c r="BR37">
         <f t="array" ref="BR37">SQRT(SUM((BR$2:BR$33-$K$2:$K$33)^2))</f>
-        <v>1.4142135623730951</v>
+        <v>1.9442897152057768</v>
       </c>
       <c r="BS37">
         <f t="array" ref="BS37">SQRT(SUM((BS$2:BS$33-$K$2:$K$33)^2))</f>
-        <v>2</v>
+        <v>2.3706310102864987</v>
       </c>
       <c r="BT37">
         <f t="array" ref="BT37">SQRT(SUM((BT$2:BT$33-$K$2:$K$33)^2))</f>
-        <v>1.4142135623730951</v>
+        <v>1.9319030762877401</v>
       </c>
       <c r="BU37">
         <f t="array" ref="BU37">SQRT(SUM((BU$2:BU$33-$K$2:$K$33)^2))</f>
-        <v>1</v>
+        <v>1.693883859802336</v>
       </c>
       <c r="BV37">
         <f t="array" ref="BV37">SQRT(SUM((BV$2:BV$33-$K$2:$K$33)^2))</f>
-        <v>2.2360679774997898</v>
+        <v>2.580775007662568</v>
       </c>
       <c r="BW37">
         <f t="array" ref="BW37">SQRT(SUM((BW$2:BW$33-$K$2:$K$33)^2))</f>
-        <v>1.4142135623730951</v>
+        <v>1.9442897152057768</v>
       </c>
       <c r="BX37">
         <f t="array" ref="BX37">SQRT(SUM((BX$2:BX$33-$K$2:$K$33)^2))</f>
-        <v>2</v>
+        <v>2.397166373302865</v>
       </c>
       <c r="BY37">
         <f t="array" ref="BY37">SQRT(SUM((BY$2:BY$33-$K$2:$K$33)^2))</f>
-        <v>2.4494897427831779</v>
+        <v>2.3435844772210994</v>
       </c>
       <c r="BZ37">
         <f t="array" ref="BZ37">SQRT(SUM((BZ$2:BZ$33-$K$2:$K$33)^2))</f>
-        <v>1.4142135623730951</v>
+        <v>0.94199774617436449</v>
       </c>
       <c r="CA37">
         <f t="array" ref="CA37">SQRT(SUM((CA$2:CA$33-$K$2:$K$33)^2))</f>
-        <v>1</v>
+        <v>1.6840278079186974</v>
       </c>
       <c r="CB37">
         <f t="array" ref="CB37">SQRT(SUM((CB$2:CB$33-$K$2:$K$33)^2))</f>
-        <v>2</v>
+        <v>2.3816172217714295</v>
       </c>
       <c r="CC37">
         <f t="array" ref="CC37">SQRT(SUM((CC$2:CC$33-$K$2:$K$33)^2))</f>
-        <v>1</v>
+        <v>1.6955947838264229</v>
       </c>
       <c r="CD37">
         <f t="array" ref="CD37">SQRT(SUM((CD$2:CD$33-$K$2:$K$33)^2))</f>
-        <v>1.4142135623730951</v>
+        <v>1.954095233174532</v>
       </c>
       <c r="CE37">
         <f t="array" ref="CE37">SQRT(SUM((CE$2:CE$33-$K$2:$K$33)^2))</f>
-        <v>1.4142135623730951</v>
+        <v>1.9581288310128075</v>
       </c>
       <c r="CF37">
         <f t="array" ref="CF37">SQRT(SUM((CF$2:CF$33-$K$2:$K$33)^2))</f>
-        <v>1.7320508075688772</v>
+        <v>2.1978566301936784</v>
       </c>
       <c r="CG37">
         <f t="array" ref="CG37">SQRT(SUM((CG$2:CG$33-$K$2:$K$33)^2))</f>
-        <v>1.4142135623730951</v>
+        <v>1.927977243754289</v>
       </c>
       <c r="CH37">
         <f t="array" ref="CH37">SQRT(SUM((CH$2:CH$33-$K$2:$K$33)^2))</f>
-        <v>1</v>
+        <v>1.6588582089401025</v>
       </c>
       <c r="CI37">
         <f t="array" ref="CI37">SQRT(SUM((CI$2:CI$33-$K$2:$K$33)^2))</f>
-        <v>1.4142135623730951</v>
+        <v>1.9445494421639871</v>
       </c>
       <c r="CJ37">
         <f t="array" ref="CJ37">SQRT(SUM((CJ$2:CJ$33-$K$2:$K$33)^2))</f>
-        <v>1.4142135623730951</v>
+        <v>1.3218516968101244</v>
       </c>
       <c r="CK37">
         <f t="array" ref="CK37">SQRT(SUM((CK$2:CK$33-$K$2:$K$33)^2))</f>
-        <v>2.4494897427831779</v>
+        <v>2.7727106376316635</v>
       </c>
       <c r="CL37">
         <f t="array" ref="CL37">SQRT(SUM((CL$2:CL$33-$K$2:$K$33)^2))</f>
-        <v>1.4142135623730951</v>
+        <v>1.9496457809144823</v>
       </c>
       <c r="CM37">
         <f t="array" ref="CM37">SQRT(SUM((CM$2:CM$33-$K$2:$K$33)^2))</f>
-        <v>1</v>
+        <v>1.1746306870622034</v>
       </c>
       <c r="CN37">
         <f t="array" ref="CN37">SQRT(SUM((CN$2:CN$33-$K$2:$K$33)^2))</f>
-        <v>2.6457513110645907</v>
+        <v>2.6713774560787327</v>
       </c>
       <c r="CO37">
         <f t="array" ref="CO37">SQRT(SUM((CO$2:CO$33-$K$2:$K$33)^2))</f>
-        <v>3</v>
+        <v>3.0182764455502018</v>
       </c>
       <c r="CP37">
         <f t="array" ref="CP37">SQRT(SUM((CP$2:CP$33-$K$2:$K$33)^2))</f>
-        <v>1.7320508075688772</v>
+        <v>2.195327621116145</v>
       </c>
       <c r="CQ37">
         <f t="array" ref="CQ37">SQRT(SUM((CQ$2:CQ$33-$K$2:$K$33)^2))</f>
-        <v>1.4142135623730951</v>
+        <v>1.1757168522174586</v>
       </c>
       <c r="CR37">
         <f t="array" ref="CR37">SQRT(SUM((CR$2:CR$33-$K$2:$K$33)^2))</f>
-        <v>1.7320508075688772</v>
+        <v>2.195867025351447</v>
       </c>
       <c r="CS37">
         <f t="array" ref="CS37">SQRT(SUM((CS$2:CS$33-$K$2:$K$33)^2))</f>
-        <v>1.7320508075688772</v>
+        <v>2.1707737442558517</v>
       </c>
       <c r="CT37">
         <f t="array" ref="CT37">SQRT(SUM((CT$2:CT$33-$K$2:$K$33)^2))</f>
-        <v>2</v>
+        <v>2.381110185388601</v>
       </c>
       <c r="CU37">
         <f t="array" ref="CU37">SQRT(SUM((CU$2:CU$33-$K$2:$K$33)^2))</f>
-        <v>2.4494897427831779</v>
+        <v>2.4911796458844284</v>
       </c>
       <c r="CV37">
         <f t="array" ref="CV37">SQRT(SUM((CV$2:CV$33-$K$2:$K$33)^2))</f>
-        <v>2</v>
+        <v>2.4102700931470604</v>
       </c>
       <c r="CW37">
         <f t="array" ref="CW37">SQRT(SUM((CW$2:CW$33-$K$2:$K$33)^2))</f>
-        <v>1</v>
+        <v>1.693883859802336</v>
       </c>
       <c r="CX37">
         <f t="array" ref="CX37">SQRT(SUM((CX$2:CX$33-$K$2:$K$33)^2))</f>
-        <v>2</v>
+        <v>2.3674100710018173</v>
       </c>
       <c r="CY37">
         <f t="array" ref="CY37">SQRT(SUM((CY$2:CY$33-$K$2:$K$33)^2))</f>
-        <v>1.4142135623730951</v>
+        <v>1.9506857388713803</v>
       </c>
       <c r="CZ37">
         <f t="array" ref="CZ37">SQRT(SUM((CZ$2:CZ$33-$K$2:$K$33)^2))</f>
-        <v>1</v>
+        <v>1.6763453087182147</v>
       </c>
       <c r="DA37">
         <f t="array" ref="DA37">SQRT(SUM((DA$2:DA$33-$K$2:$K$33)^2))</f>
-        <v>1.4142135623730951</v>
+        <v>1.9445494421639871</v>
       </c>
       <c r="DB37">
         <f t="array" ref="DB37">SQRT(SUM((DB$2:DB$33-$K$2:$K$33)^2))</f>
-        <v>2</v>
+        <v>2.4094513830524789</v>
       </c>
       <c r="DC37">
         <f t="array" ref="DC37">SQRT(SUM((DC$2:DC$33-$K$2:$K$33)^2))</f>
-        <v>1.7320508075688772</v>
+        <v>2.1579753530640242</v>
       </c>
       <c r="DD37">
         <f t="array" ref="DD37">SQRT(SUM((DD$2:DD$33-$K$2:$K$33)^2))</f>
-        <v>1.4142135623730951</v>
+        <v>1.9578256010614747</v>
       </c>
       <c r="DE37">
         <f t="array" ref="DE37">SQRT(SUM((DE$2:DE$33-$K$2:$K$33)^2))</f>
-        <v>2</v>
+        <v>2.3604092011403059</v>
       </c>
       <c r="DF37">
         <f t="array" ref="DF37">SQRT(SUM((DF$2:DF$33-$K$2:$K$33)^2))</f>
-        <v>2</v>
+        <v>2.3936089759361923</v>
       </c>
       <c r="DG37">
         <f t="array" ref="DG37">SQRT(SUM((DG$2:DG$33-$K$2:$K$33)^2))</f>
-        <v>2.4494897427831779</v>
-      </c>
-    </row>
-    <row r="38" spans="1:113" x14ac:dyDescent="0.2">
+        <v>2.7599355626682134</v>
+      </c>
+    </row>
+    <row r="38" spans="1:112" x14ac:dyDescent="0.2">
       <c r="G38" t="s">
         <v>153</v>
       </c>
       <c r="L38">
         <f>MIN(L34:L37)</f>
-        <v>1.7320508075688772</v>
+        <v>1.0883687942579159</v>
       </c>
       <c r="M38">
         <f t="shared" ref="M38:BX38" si="0">MIN(M34:M37)</f>
-        <v>1.4142135623730951</v>
+        <v>1.2973732917853369</v>
       </c>
       <c r="N38">
         <f t="shared" si="0"/>
-        <v>1.4142135623730951</v>
+        <v>0.70900168934275176</v>
       </c>
       <c r="O38">
         <f t="shared" si="0"/>
-        <v>1.4142135623730951</v>
+        <v>1.0128081542137797</v>
       </c>
       <c r="P38">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1.8886192892984752</v>
       </c>
       <c r="Q38">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1.5921595054427398</v>
       </c>
       <c r="R38">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>0.86185981890530861</v>
       </c>
       <c r="S38">
         <f t="shared" si="0"/>
-        <v>1.4142135623730951</v>
+        <v>1.1968896348947062</v>
       </c>
       <c r="T38">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1.5208875459717481</v>
       </c>
       <c r="U38">
         <f t="shared" si="0"/>
-        <v>1.7320508075688772</v>
+        <v>0.94387554364660509</v>
       </c>
       <c r="V38">
         <f t="shared" si="0"/>
-        <v>2.2360679774997898</v>
+        <v>1.8449582254873356</v>
       </c>
       <c r="W38">
         <f t="shared" si="0"/>
-        <v>1.7320508075688772</v>
+        <v>0.93285478658924037</v>
       </c>
       <c r="X38">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1.2476661685147472</v>
       </c>
       <c r="Y38">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1.7030647666899406</v>
       </c>
       <c r="Z38">
         <f t="shared" si="0"/>
-        <v>1.4142135623730951</v>
+        <v>1.4113855089649485</v>
       </c>
       <c r="AA38">
         <f t="shared" si="0"/>
-        <v>1.4142135623730951</v>
+        <v>0.70900168934275176</v>
       </c>
       <c r="AB38">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1.8369734387499372</v>
       </c>
       <c r="AC38">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>0.86185981890530861</v>
       </c>
       <c r="AD38">
         <f t="shared" si="0"/>
-        <v>1.4142135623730951</v>
+        <v>0.99169544877578208</v>
       </c>
       <c r="AE38">
         <f t="shared" si="0"/>
-        <v>1.7320508075688772</v>
+        <v>1.4842777331826831</v>
       </c>
       <c r="AF38">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1.0813191836481062</v>
       </c>
       <c r="AG38">
         <f t="shared" si="0"/>
-        <v>1.4142135623730951</v>
+        <v>1.3335572115425667</v>
       </c>
       <c r="AH38">
         <f t="shared" si="0"/>
-        <v>1.4142135623730951</v>
+        <v>1.1365209354554062</v>
       </c>
       <c r="AI38">
         <f t="shared" si="0"/>
-        <v>2.6457513110645907</v>
+        <v>2.0739834611338597</v>
       </c>
       <c r="AJ38">
         <f t="shared" si="0"/>
-        <v>1.4142135623730951</v>
+        <v>0.94199774617436449</v>
       </c>
       <c r="AK38">
         <f t="shared" si="0"/>
-        <v>2.2360679774997898</v>
+        <v>1.8649217727445708</v>
       </c>
       <c r="AL38">
         <f t="shared" si="0"/>
-        <v>1.4142135623730951</v>
+        <v>1.4322191213550493</v>
       </c>
       <c r="AM38">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1.87958746762827</v>
       </c>
       <c r="AN38">
         <f t="shared" si="0"/>
-        <v>1.4142135623730951</v>
+        <v>1.1991471736615995</v>
       </c>
       <c r="AO38">
         <f t="shared" si="0"/>
-        <v>1.7320508075688772</v>
+        <v>1.6774600317046797</v>
       </c>
       <c r="AP38">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>1.0938533526970031</v>
       </c>
       <c r="AQ38">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1.9064717998384595</v>
       </c>
       <c r="AR38">
         <f t="shared" si="0"/>
-        <v>1.4142135623730951</v>
+        <v>1.0275018965942826</v>
       </c>
       <c r="AS38">
         <f t="shared" si="0"/>
-        <v>2.4494897427831779</v>
+        <v>2.0126299093315407</v>
       </c>
       <c r="AT38">
         <f t="shared" si="0"/>
-        <v>1.4142135623730951</v>
+        <v>1.3721259073074701</v>
       </c>
       <c r="AU38">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1.5045085273455601</v>
       </c>
       <c r="AV38">
         <f t="shared" si="0"/>
-        <v>1.7320508075688772</v>
+        <v>1.3602666557863698</v>
       </c>
       <c r="AW38">
         <f t="shared" si="0"/>
-        <v>2.2360679774997898</v>
+        <v>1.3546294707732818</v>
       </c>
       <c r="AX38">
         <f t="shared" si="0"/>
-        <v>2.2360679774997898</v>
+        <v>1.7947158314725244</v>
       </c>
       <c r="AY38">
         <f t="shared" si="0"/>
-        <v>2.2360679774997898</v>
+        <v>1.4734269875453891</v>
       </c>
       <c r="AZ38">
         <f t="shared" si="0"/>
-        <v>1.4142135623730951</v>
+        <v>0.70900168934275176</v>
       </c>
       <c r="BA38">
         <f t="shared" si="0"/>
-        <v>1.7320508075688772</v>
+        <v>0.61259096473251229</v>
       </c>
       <c r="BB38">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>1.0343308528839041</v>
       </c>
       <c r="BC38">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1.7968017883665004</v>
       </c>
       <c r="BD38">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1.3887017092279574</v>
       </c>
       <c r="BE38">
         <f t="shared" si="0"/>
-        <v>2.2360679774997898</v>
+        <v>1.7524115185051239</v>
       </c>
       <c r="BF38">
         <f t="shared" si="0"/>
-        <v>1.7320508075688772</v>
+        <v>1.1419853292722966</v>
       </c>
       <c r="BG38">
         <f t="shared" si="0"/>
-        <v>1.7320508075688772</v>
+        <v>1.7504154267074161</v>
       </c>
       <c r="BH38">
         <f t="shared" si="0"/>
-        <v>2.2360679774997898</v>
+        <v>2.0187638579274498</v>
       </c>
       <c r="BI38">
         <f t="shared" si="0"/>
-        <v>1.7320508075688772</v>
+        <v>1.6326443651905302</v>
       </c>
       <c r="BJ38">
         <f t="shared" si="0"/>
-        <v>1.7320508075688772</v>
+        <v>1.7038162336692337</v>
       </c>
       <c r="BK38">
         <f t="shared" si="0"/>
-        <v>2.6457513110645907</v>
+        <v>2.1154635137735829</v>
       </c>
       <c r="BL38">
         <f t="shared" si="0"/>
-        <v>1.4142135623730951</v>
+        <v>1.412648657195998</v>
       </c>
       <c r="BM38">
         <f t="shared" si="0"/>
-        <v>1.4142135623730951</v>
+        <v>0.94199774617436449</v>
       </c>
       <c r="BN38">
         <f t="shared" si="0"/>
-        <v>2.4494897427831779</v>
+        <v>1.9117132267131365</v>
       </c>
       <c r="BO38">
         <f t="shared" si="0"/>
-        <v>1.4142135623730951</v>
+        <v>1.1968896348947062</v>
       </c>
       <c r="BP38">
         <f t="shared" si="0"/>
-        <v>1.7320508075688772</v>
+        <v>0.61259096473251229</v>
       </c>
       <c r="BQ38">
         <f t="shared" si="0"/>
-        <v>1.4142135623730951</v>
+        <v>1.4576551323794356</v>
       </c>
       <c r="BR38">
         <f t="shared" si="0"/>
-        <v>1.4142135623730951</v>
+        <v>1.1486626779268918</v>
       </c>
       <c r="BS38">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1.7537693847633125</v>
       </c>
       <c r="BT38">
         <f t="shared" si="0"/>
-        <v>1.4142135623730951</v>
+        <v>1.3115813249936463</v>
       </c>
       <c r="BU38">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>1.0343308528839041</v>
       </c>
       <c r="BV38">
         <f t="shared" si="0"/>
-        <v>2.2360679774997898</v>
+        <v>1.9598091434252001</v>
       </c>
       <c r="BW38">
         <f t="shared" si="0"/>
-        <v>1.4142135623730951</v>
+        <v>1.1486626779268918</v>
       </c>
       <c r="BX38">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1.2095026942283604</v>
       </c>
       <c r="BY38">
         <f t="shared" ref="BY38:DG38" si="1">MIN(BY34:BY37)</f>
-        <v>2.4494897427831779</v>
+        <v>2.2791120499734792</v>
       </c>
       <c r="BZ38">
         <f t="shared" si="1"/>
-        <v>1.4142135623730951</v>
+        <v>0.94199774617436449</v>
       </c>
       <c r="CA38">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>1.0985936526605908</v>
       </c>
       <c r="CB38">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>1.4597253032360544</v>
       </c>
       <c r="CC38">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0.98724005946288462</v>
       </c>
       <c r="CD38">
         <f t="shared" si="1"/>
-        <v>1.4142135623730951</v>
+        <v>1.4080709320073972</v>
       </c>
       <c r="CE38">
         <f t="shared" si="1"/>
-        <v>1.4142135623730951</v>
+        <v>1.3560152555108214</v>
       </c>
       <c r="CF38">
         <f t="shared" si="1"/>
-        <v>1.7320508075688772</v>
+        <v>1.293803272689326</v>
       </c>
       <c r="CG38">
         <f t="shared" si="1"/>
-        <v>1.4142135623730951</v>
+        <v>1.1822021512407699</v>
       </c>
       <c r="CH38">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0.91286622397051942</v>
       </c>
       <c r="CI38">
         <f t="shared" si="1"/>
-        <v>1.4142135623730951</v>
+        <v>1.0303571428678142</v>
       </c>
       <c r="CJ38">
         <f t="shared" si="1"/>
-        <v>1.4142135623730951</v>
+        <v>1.3218516968101244</v>
       </c>
       <c r="CK38">
         <f t="shared" si="1"/>
-        <v>2.4494897427831779</v>
+        <v>2.0506329637317542</v>
       </c>
       <c r="CL38">
         <f t="shared" si="1"/>
-        <v>1.4142135623730951</v>
+        <v>1.5015598547724682</v>
       </c>
       <c r="CM38">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>1.0592369134415502</v>
       </c>
       <c r="CN38">
         <f t="shared" si="1"/>
-        <v>2.6457513110645907</v>
+        <v>2.3323336922990845</v>
       </c>
       <c r="CO38">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>2.6599195213497859</v>
       </c>
       <c r="CP38">
         <f t="shared" si="1"/>
-        <v>1.7320508075688772</v>
+        <v>1.6698855998492803</v>
       </c>
       <c r="CQ38">
         <f t="shared" si="1"/>
-        <v>1.4142135623730951</v>
+        <v>1.1757168522174586</v>
       </c>
       <c r="CR38">
         <f t="shared" si="1"/>
-        <v>1.7320508075688772</v>
+        <v>1.1233031639561211</v>
       </c>
       <c r="CS38">
         <f t="shared" si="1"/>
-        <v>1.7320508075688772</v>
+        <v>1.5602181606493553</v>
       </c>
       <c r="CT38">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>1.044982206109752</v>
       </c>
       <c r="CU38">
         <f t="shared" si="1"/>
-        <v>2.4494897427831779</v>
+        <v>2.1428297017591276</v>
       </c>
       <c r="CV38">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>1.884958856782635</v>
       </c>
       <c r="CW38">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>1.0343308528839041</v>
       </c>
       <c r="CX38">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>1.7069923899605102</v>
       </c>
       <c r="CY38">
         <f t="shared" si="1"/>
-        <v>1.4142135623730951</v>
+        <v>1.1641655519207657</v>
       </c>
       <c r="CZ38">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0.98151081416296715</v>
       </c>
       <c r="DA38">
         <f t="shared" si="1"/>
-        <v>1.4142135623730951</v>
+        <v>1.0303571428678142</v>
       </c>
       <c r="DB38">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>1.6391740112686677</v>
       </c>
       <c r="DC38">
         <f t="shared" si="1"/>
-        <v>1.7320508075688772</v>
+        <v>1.3365566457539797</v>
       </c>
       <c r="DD38">
         <f t="shared" si="1"/>
-        <v>1.4142135623730951</v>
+        <v>1.1818161081579406</v>
       </c>
       <c r="DE38">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>1.8130145166591742</v>
       </c>
       <c r="DF38">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>1.8356943442168461</v>
       </c>
       <c r="DG38">
         <f t="shared" si="1"/>
-        <v>2.4494897427831779</v>
-      </c>
-    </row>
-    <row r="39" spans="1:113" x14ac:dyDescent="0.2">
+        <v>1.9581991487158106</v>
+      </c>
+    </row>
+    <row r="39" spans="1:112" x14ac:dyDescent="0.2">
       <c r="G39" s="1" t="s">
         <v>154</v>
       </c>
       <c r="L39">
         <f>MATCH(L38,L34:L37,0)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M39">
         <f t="shared" ref="M39:BX39" si="2">MATCH(M38,M34:M37,0)</f>
@@ -17592,11 +18008,11 @@
       </c>
       <c r="N39">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="O39">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P39">
         <f t="shared" si="2"/>
@@ -17604,35 +18020,35 @@
       </c>
       <c r="Q39">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="R39">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="S39">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T39">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="U39">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="V39">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="W39">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="X39">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Y39">
         <f t="shared" si="2"/>
@@ -17644,7 +18060,7 @@
       </c>
       <c r="AA39">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="AB39">
         <f t="shared" si="2"/>
@@ -17652,19 +18068,19 @@
       </c>
       <c r="AC39">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="AD39">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AE39">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AF39">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AG39">
         <f t="shared" si="2"/>
@@ -17672,19 +18088,19 @@
       </c>
       <c r="AH39">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AI39">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AJ39">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="AK39">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AL39">
         <f t="shared" si="2"/>
@@ -17704,19 +18120,19 @@
       </c>
       <c r="AP39">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AQ39">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AR39">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AS39">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AT39">
         <f t="shared" si="2"/>
@@ -17724,31 +18140,31 @@
       </c>
       <c r="AU39">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AV39">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AW39">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AX39">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AY39">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AZ39">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="BA39">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="BB39">
         <f t="shared" si="2"/>
@@ -17760,19 +18176,19 @@
       </c>
       <c r="BD39">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="BE39">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="BF39">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="BG39">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="BH39">
         <f t="shared" si="2"/>
@@ -17788,7 +18204,7 @@
       </c>
       <c r="BK39">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="BL39">
         <f t="shared" si="2"/>
@@ -17796,27 +18212,27 @@
       </c>
       <c r="BM39">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="BN39">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="BO39">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="BP39">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="BQ39">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="BR39">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="BS39">
         <f t="shared" si="2"/>
@@ -17836,11 +18252,11 @@
       </c>
       <c r="BW39">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="BX39">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="BY39">
         <f t="shared" ref="BY39:DG39" si="3">MATCH(BY38,BY34:BY37,0)</f>
@@ -17848,7 +18264,7 @@
       </c>
       <c r="BZ39">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="CA39">
         <f t="shared" si="3"/>
@@ -17856,7 +18272,7 @@
       </c>
       <c r="CB39">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="CC39">
         <f t="shared" si="3"/>
@@ -17872,11 +18288,11 @@
       </c>
       <c r="CF39">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="CG39">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="CH39">
         <f t="shared" si="3"/>
@@ -17884,15 +18300,15 @@
       </c>
       <c r="CI39">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="CJ39">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="CK39">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="CL39">
         <f t="shared" si="3"/>
@@ -17904,7 +18320,7 @@
       </c>
       <c r="CN39">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="CO39">
         <f t="shared" si="3"/>
@@ -17916,19 +18332,19 @@
       </c>
       <c r="CQ39">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="CR39">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="CS39">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="CT39">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="CU39">
         <f t="shared" si="3"/>
@@ -17948,7 +18364,7 @@
       </c>
       <c r="CY39">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="CZ39">
         <f t="shared" si="3"/>
@@ -17956,19 +18372,19 @@
       </c>
       <c r="DA39">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="DB39">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="DC39">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="DD39">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="DE39">
         <f t="shared" si="3"/>
@@ -17980,7 +18396,7 @@
       </c>
       <c r="DG39">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>